<commit_message>
reapair few of my mistakes
While was not able to test my chane when was do it 2 mounth in past
cause some hard unbalaces that i now kind of fix.
</commit_message>
<xml_diff>
--- a/Units.xlsx
+++ b/Units.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="217">
   <si>
     <t>Stats</t>
   </si>
@@ -153,9 +153,6 @@
     <t>single shot kill t1 unit</t>
   </si>
   <si>
-    <t>Golem</t>
-  </si>
-  <si>
     <t>T2 transport</t>
   </si>
   <si>
@@ -661,6 +658,18 @@
   </si>
   <si>
     <t>T3 stealth shield</t>
+  </si>
+  <si>
+    <t>ina1003</t>
+  </si>
+  <si>
+    <t>ina1002</t>
+  </si>
+  <si>
+    <t>ina1001</t>
+  </si>
+  <si>
+    <t>ina1004</t>
   </si>
 </sst>
 </file>
@@ -1420,10 +1429,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AL113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A73" sqref="A73"/>
-      <selection pane="topRight" activeCell="AL105" sqref="AL105"/>
+      <selection pane="topRight" activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,7 +1444,7 @@
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2066,7 +2075,19 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>215</v>
+      </c>
+      <c r="C36" t="s">
+        <v>214</v>
+      </c>
+      <c r="D36" t="s">
+        <v>213</v>
+      </c>
+      <c r="E36" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2084,7 +2105,7 @@
       <c r="H37" s="30"/>
       <c r="I37" s="30"/>
       <c r="J37" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K37" s="30"/>
       <c r="L37" s="30"/>
@@ -2107,28 +2128,28 @@
         <v>37</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L38" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2151,25 +2172,25 @@
         <v>41</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M39" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="L39" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="M39" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2183,13 +2204,13 @@
         <v>50</v>
       </c>
       <c r="D40" s="5">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="E40" s="7">
         <v>120</v>
       </c>
       <c r="F40" s="7">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G40" s="5">
         <v>300</v>
@@ -2220,13 +2241,13 @@
         <v>2250</v>
       </c>
       <c r="D41" s="5">
-        <v>2450</v>
+        <v>2400</v>
       </c>
       <c r="E41" s="7">
         <v>4800</v>
       </c>
       <c r="F41" s="7">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="G41" s="5">
         <v>12000</v>
@@ -2263,7 +2284,7 @@
         <v>800</v>
       </c>
       <c r="F42" s="7">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="G42" s="5">
         <v>2400</v>
@@ -2305,7 +2326,7 @@
       </c>
       <c r="F43" s="7">
         <f t="shared" ref="F43" si="8">F42/$C$34</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G43" s="7">
         <f>G42/$D$34</f>
@@ -2350,7 +2371,7 @@
       </c>
       <c r="D44" s="7">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>3.4285714285714284</v>
       </c>
       <c r="E44" s="7">
         <f t="shared" si="10"/>
@@ -2403,7 +2424,7 @@
       </c>
       <c r="D45" s="7">
         <f t="shared" si="12"/>
-        <v>70</v>
+        <v>68.571428571428569</v>
       </c>
       <c r="E45" s="7">
         <f t="shared" si="12"/>
@@ -2586,7 +2607,7 @@
       </c>
       <c r="E51" s="7"/>
       <c r="F51" s="7">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
@@ -2596,7 +2617,7 @@
         <v>360</v>
       </c>
       <c r="L51" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M51" s="7"/>
     </row>
@@ -2634,7 +2655,7 @@
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
@@ -2865,7 +2886,7 @@
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
       <c r="L62" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M62" s="7"/>
     </row>
@@ -2907,7 +2928,7 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H65" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
@@ -2942,7 +2963,7 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B69" s="26"/>
       <c r="C69" s="26"/>
@@ -2951,149 +2972,149 @@
       <c r="F69" s="26"/>
       <c r="G69" s="26"/>
       <c r="I69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J69" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K69" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L69" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M69" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N69" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q69" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R69" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B70" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C70" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D70" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="D70" s="21" t="s">
+      <c r="E70" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="E70" s="22" t="s">
+      <c r="F70" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="F70" s="22" t="s">
+      <c r="G70" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="G70" s="22" t="s">
-        <v>91</v>
-      </c>
       <c r="H70" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I70" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J70" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K70" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L70" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M70" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N70" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O70" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P70" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q70" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="R70" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S70" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B71" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C71" s="24"/>
       <c r="D71" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E71" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F71" s="24" t="s">
         <v>97</v>
-      </c>
-      <c r="E71" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F71" s="24" t="s">
-        <v>98</v>
       </c>
       <c r="G71" s="24"/>
       <c r="H71" s="24"/>
       <c r="I71" s="25"/>
       <c r="J71" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K71" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L71" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M71" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N71" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P71" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q71" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R71" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S71" s="28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B72" s="16">
         <v>12</v>
@@ -3142,7 +3163,7 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B73" s="16">
         <v>40</v>
@@ -3191,7 +3212,7 @@
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B74" s="16">
         <v>80</v>
@@ -3240,7 +3261,7 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B75" s="16">
         <f>B74/$B$67</f>
@@ -3296,7 +3317,7 @@
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B76" s="16">
         <f>B72/$B$75</f>
@@ -3352,7 +3373,7 @@
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B77" s="16">
         <f>B73/$B$75</f>
@@ -3408,7 +3429,7 @@
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B78" s="16"/>
       <c r="C78" s="16"/>
@@ -3456,7 +3477,7 @@
         <v>640</v>
       </c>
       <c r="J79" s="18">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="K79" s="18">
         <v>600</v>
@@ -3481,7 +3502,7 @@
         <v>1600</v>
       </c>
       <c r="S79" s="23">
-        <v>5000</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
@@ -3510,7 +3531,7 @@
       </c>
       <c r="L80" s="20"/>
       <c r="M80" s="29">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="N80" s="23">
         <v>2.7</v>
@@ -3524,12 +3545,12 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="S80" s="29">
-        <v>3</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B81" s="16"/>
       <c r="C81" s="16">
@@ -3548,7 +3569,7 @@
       <c r="H81" s="17"/>
       <c r="I81" s="18"/>
       <c r="J81" s="18">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="K81" s="18"/>
       <c r="L81" s="19"/>
@@ -3565,12 +3586,12 @@
         <v>600</v>
       </c>
       <c r="S81" s="29">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B82" s="16"/>
       <c r="C82" s="16"/>
@@ -3593,7 +3614,7 @@
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B83" s="16"/>
       <c r="C83" s="16"/>
@@ -3616,7 +3637,7 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B84" s="16"/>
       <c r="C84" s="16"/>
@@ -3641,7 +3662,7 @@
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B85" s="16"/>
       <c r="C85" s="16"/>
@@ -3668,7 +3689,7 @@
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B86" s="16"/>
       <c r="C86" s="16"/>
@@ -3693,7 +3714,7 @@
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B87" s="16"/>
       <c r="C87" s="16"/>
@@ -3716,7 +3737,7 @@
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B88" s="16"/>
       <c r="C88" s="16">
@@ -3750,15 +3771,15 @@
       </c>
       <c r="R88" s="29"/>
       <c r="S88" s="29">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C89" s="16"/>
       <c r="D89" s="16"/>
@@ -3788,18 +3809,18 @@
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D90" s="14"/>
       <c r="E90" s="15"/>
       <c r="F90" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G90" s="15"/>
       <c r="H90" s="15"/>
@@ -3808,21 +3829,21 @@
       <c r="K90" s="15"/>
       <c r="L90" s="15"/>
       <c r="M90" t="s">
+        <v>116</v>
+      </c>
+      <c r="N90" t="s">
         <v>117</v>
       </c>
-      <c r="N90" t="s">
-        <v>118</v>
-      </c>
       <c r="P90" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="R90" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B91" s="14"/>
       <c r="C91" s="15"/>
@@ -3838,7 +3859,7 @@
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B92" s="14"/>
       <c r="C92" s="14"/>
@@ -3854,209 +3875,209 @@
     </row>
     <row r="98" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C98" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D98" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E98" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F98" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G98" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H98" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J98" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K98" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L98" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M98" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N98" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O98" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P98" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="R98" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S98" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T98" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="U98" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V98" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="W98" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="X98" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Z98" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AA98" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AB98" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC98" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AD98" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AE98" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AF98" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AG98" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AH98" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AI98" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AJ98" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AL98" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C99" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D99" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E99" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F99" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G99" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H99" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J99" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K99" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L99" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M99" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N99" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O99" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P99" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R99" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S99" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="T99" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="U99" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="V99" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="W99" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="X99" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Z99" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AA99" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AB99" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AC99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AD99" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AE99" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AF99" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AG99" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AH99" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI99" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AJ99" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AL99" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="101" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B101">
         <v>8000</v>
@@ -4131,19 +4152,19 @@
         <v>7000</v>
       </c>
       <c r="AF101" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AG101" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AH101" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AI101">
         <v>3800</v>
       </c>
       <c r="AJ101" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL101">
         <v>500</v>
@@ -4151,7 +4172,7 @@
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B102">
         <v>13300</v>
@@ -4234,7 +4255,7 @@
     </row>
     <row r="103" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B103">
         <v>1520</v>
@@ -4317,7 +4338,7 @@
     </row>
     <row r="104" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B104">
         <v>2600</v>
@@ -4400,7 +4421,7 @@
     </row>
     <row r="105" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B105">
         <v>40</v>
@@ -4444,7 +4465,7 @@
     </row>
     <row r="106" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J106">
         <v>150</v>
@@ -4476,7 +4497,7 @@
     </row>
     <row r="107" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J107">
         <v>1</v>
@@ -4484,7 +4505,7 @@
     </row>
     <row r="108" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R108">
         <v>35</v>
@@ -4525,7 +4546,7 @@
     </row>
     <row r="109" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R109">
         <v>44</v>
@@ -4566,7 +4587,7 @@
     </row>
     <row r="110" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S110">
         <v>1.5</v>
@@ -4601,7 +4622,7 @@
     </row>
     <row r="111" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R111">
         <v>2</v>
@@ -4630,7 +4651,7 @@
     </row>
     <row r="112" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V112">
         <v>5</v>
@@ -4641,16 +4662,16 @@
     </row>
     <row r="113" spans="26:29" x14ac:dyDescent="0.25">
       <c r="Z113" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AA113" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AB113" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AC113" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
t1 artylery bombrd move
errors in log,> bombard mod not work.. no clue whats going on there.
</commit_message>
<xml_diff>
--- a/Units.xlsx
+++ b/Units.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="268">
   <si>
     <t>Stats</t>
   </si>
@@ -273,9 +273,6 @@
     <t>lab</t>
   </si>
   <si>
-    <t>aa/arty</t>
-  </si>
-  <si>
     <t>tank</t>
   </si>
   <si>
@@ -796,6 +793,36 @@
   </si>
   <si>
     <t>Golem</t>
+  </si>
+  <si>
+    <t>inu1007</t>
+  </si>
+  <si>
+    <t>Astor</t>
+  </si>
+  <si>
+    <t>inu1004</t>
+  </si>
+  <si>
+    <t>inu1001</t>
+  </si>
+  <si>
+    <t>inu1005</t>
+  </si>
+  <si>
+    <t>inu1006</t>
+  </si>
+  <si>
+    <t>inu1008</t>
+  </si>
+  <si>
+    <t>inu1002</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>arty</t>
   </si>
 </sst>
 </file>
@@ -1086,85 +1113,7 @@
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1555,10 +1504,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A73" sqref="A73"/>
-      <selection pane="topRight" activeCell="F24" sqref="F24"/>
+      <selection pane="topRight" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,19 +1562,19 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F5" t="s">
         <v>212</v>
-      </c>
-      <c r="C5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E5" t="s">
-        <v>257</v>
-      </c>
-      <c r="F5" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1666,7 +1615,7 @@
         <v>37</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>43</v>
@@ -2447,7 +2396,7 @@
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
@@ -2464,12 +2413,12 @@
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>15</v>
       </c>
@@ -2484,7 +2433,7 @@
       </c>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>19</v>
       </c>
@@ -2499,51 +2448,69 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="I38" t="s">
-        <v>96</v>
+      <c r="B38" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="H38" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="I38" s="26" t="s">
+        <v>262</v>
       </c>
       <c r="J38" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K38" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="L38" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="M38" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="N38" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="O38" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="P38" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Q38" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="R38" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="S38" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="T38" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>82</v>
       </c>
@@ -2554,103 +2521,111 @@
         <v>83</v>
       </c>
       <c r="D39" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="F39" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="22" t="s">
+      <c r="G39" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="H39" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="G39" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="H39" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="I39" s="27" t="s">
-        <v>97</v>
+      <c r="I39" s="22" t="s">
+        <v>91</v>
       </c>
       <c r="J39" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K39" s="27" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="L39" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="M39" s="22" t="s">
-        <v>108</v>
+        <v>101</v>
+      </c>
+      <c r="M39" s="27" t="s">
+        <v>104</v>
       </c>
       <c r="N39" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="O39" s="22" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="P39" s="22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="Q39" s="22" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="R39" s="22" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="S39" s="22" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="T39" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>61</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" s="24"/>
+        <v>87</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>259</v>
+      </c>
       <c r="D40" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="F40" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="E40" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="F40" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="G40" s="24"/>
       <c r="H40" s="24"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25" t="s">
-        <v>100</v>
-      </c>
+      <c r="I40" s="24"/>
+      <c r="J40" s="25"/>
       <c r="K40" s="25" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="L40" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="M40" s="28" t="s">
-        <v>109</v>
+        <v>102</v>
+      </c>
+      <c r="M40" s="25" t="s">
+        <v>105</v>
       </c>
       <c r="N40" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="P40" s="28" t="s">
-        <v>119</v>
+        <v>108</v>
+      </c>
+      <c r="O40" s="28" t="s">
+        <v>111</v>
       </c>
       <c r="Q40" s="28" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="R40" s="28" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="S40" s="28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="T40" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>62</v>
       </c>
@@ -2660,46 +2635,49 @@
       <c r="C41" s="16">
         <v>35</v>
       </c>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16">
+      <c r="D41" s="16">
+        <v>55</v>
+      </c>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16">
         <v>54</v>
       </c>
-      <c r="F41" s="17">
+      <c r="G41" s="17">
         <v>66</v>
       </c>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17">
+      <c r="H41" s="17"/>
+      <c r="I41" s="17">
         <v>130</v>
       </c>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18">
+      <c r="J41" s="18"/>
+      <c r="K41" s="18">
         <v>100</v>
       </c>
-      <c r="K41" s="18">
+      <c r="L41" s="18">
         <v>220</v>
       </c>
-      <c r="L41" s="19"/>
-      <c r="M41" s="23">
+      <c r="M41" s="19"/>
+      <c r="N41" s="23">
         <v>197</v>
       </c>
-      <c r="N41" s="23">
+      <c r="O41" s="23">
         <v>12500</v>
       </c>
-      <c r="O41" s="29"/>
-      <c r="P41" s="23">
+      <c r="P41" s="29"/>
+      <c r="Q41" s="23">
         <v>640</v>
       </c>
-      <c r="Q41" s="23">
+      <c r="R41" s="23">
         <v>360</v>
       </c>
-      <c r="R41" s="23">
+      <c r="S41" s="23">
         <v>960</v>
       </c>
-      <c r="S41" s="23">
+      <c r="T41" s="23">
         <v>480</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>63</v>
       </c>
@@ -2709,46 +2687,49 @@
       <c r="C42" s="16">
         <v>140</v>
       </c>
-      <c r="D42" s="16"/>
-      <c r="E42" s="17">
+      <c r="D42" s="16">
+        <v>275</v>
+      </c>
+      <c r="E42" s="16"/>
+      <c r="F42" s="17">
         <v>270</v>
       </c>
-      <c r="F42" s="17">
+      <c r="G42" s="17">
         <v>330</v>
       </c>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17">
+      <c r="H42" s="17"/>
+      <c r="I42" s="17">
         <v>650</v>
       </c>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18">
+      <c r="J42" s="18"/>
+      <c r="K42" s="18">
         <v>750</v>
       </c>
-      <c r="K42" s="18">
+      <c r="L42" s="18">
         <v>1650</v>
       </c>
-      <c r="L42" s="20"/>
-      <c r="M42" s="23">
+      <c r="M42" s="20"/>
+      <c r="N42" s="23">
         <v>990</v>
       </c>
-      <c r="N42" s="23">
+      <c r="O42" s="23">
         <v>240000</v>
       </c>
-      <c r="O42" s="29"/>
-      <c r="P42" s="23">
+      <c r="P42" s="29"/>
+      <c r="Q42" s="23">
         <v>8000</v>
       </c>
-      <c r="Q42" s="23">
+      <c r="R42" s="23">
         <v>1800</v>
       </c>
-      <c r="R42" s="23">
+      <c r="S42" s="23">
         <v>9600</v>
       </c>
-      <c r="S42" s="23">
+      <c r="T42" s="23">
         <v>5400</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>64</v>
       </c>
@@ -2758,46 +2739,49 @@
       <c r="C43" s="16">
         <v>120</v>
       </c>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16">
+      <c r="D43" s="16">
+        <v>220</v>
+      </c>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16">
         <v>270</v>
       </c>
-      <c r="F43" s="17">
+      <c r="G43" s="17">
         <v>330</v>
       </c>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17">
+      <c r="H43" s="17"/>
+      <c r="I43" s="17">
         <v>650</v>
       </c>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18">
+      <c r="J43" s="18"/>
+      <c r="K43" s="18">
         <v>500</v>
       </c>
-      <c r="K43" s="18">
+      <c r="L43" s="18">
         <v>1100</v>
       </c>
-      <c r="L43" s="19"/>
-      <c r="M43" s="23">
+      <c r="M43" s="19"/>
+      <c r="N43" s="23">
         <v>880</v>
       </c>
-      <c r="N43" s="23">
+      <c r="O43" s="23">
         <v>12000</v>
       </c>
-      <c r="O43" s="29"/>
-      <c r="P43" s="23">
+      <c r="P43" s="29"/>
+      <c r="Q43" s="23">
         <v>640</v>
       </c>
-      <c r="Q43" s="23">
+      <c r="R43" s="23">
         <v>1600</v>
       </c>
-      <c r="R43" s="23">
+      <c r="S43" s="23">
         <v>5000</v>
       </c>
-      <c r="S43" s="23">
+      <c r="T43" s="23">
         <v>2400</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>65</v>
       </c>
@@ -2806,54 +2790,55 @@
         <v>4</v>
       </c>
       <c r="C44" s="16">
-        <f t="shared" ref="C44:L44" si="9">C43/$B$36</f>
+        <f t="shared" ref="C44:M44" si="9">C43/$B$36</f>
         <v>6</v>
       </c>
       <c r="D44" s="16">
+        <f t="shared" ref="D44" si="10">D43/$B$36</f>
+        <v>11</v>
+      </c>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16">
+        <f t="shared" si="9"/>
+        <v>13.5</v>
+      </c>
+      <c r="G44" s="16">
+        <f t="shared" ref="G44" si="11">G43/$B$36</f>
+        <v>16.5</v>
+      </c>
+      <c r="H44" s="16">
+        <f t="shared" ref="H44" si="12">H43/$B$36</f>
+        <v>0</v>
+      </c>
+      <c r="I44" s="16">
+        <f>I43/$B$36</f>
+        <v>32.5</v>
+      </c>
+      <c r="J44" s="16">
+        <f t="shared" ref="J44" si="13">J43/$B$36</f>
+        <v>0</v>
+      </c>
+      <c r="K44" s="16">
+        <f>K43/$C$36</f>
+        <v>12.5</v>
+      </c>
+      <c r="L44" s="16">
+        <f t="shared" si="9"/>
+        <v>55</v>
+      </c>
+      <c r="M44" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="E44" s="16">
-        <f t="shared" si="9"/>
-        <v>13.5</v>
-      </c>
-      <c r="F44" s="16">
-        <f t="shared" ref="F44" si="10">F43/$B$36</f>
-        <v>16.5</v>
-      </c>
-      <c r="G44" s="16">
-        <f t="shared" ref="G44" si="11">G43/$B$36</f>
-        <v>0</v>
-      </c>
-      <c r="H44" s="16">
-        <f>H43/$B$36</f>
-        <v>32.5</v>
-      </c>
-      <c r="I44" s="16">
-        <f t="shared" ref="I44" si="12">I43/$B$36</f>
-        <v>0</v>
-      </c>
-      <c r="J44" s="16">
-        <f>J43/$C$36</f>
-        <v>12.5</v>
-      </c>
-      <c r="K44" s="16">
-        <f t="shared" si="9"/>
-        <v>55</v>
-      </c>
-      <c r="L44" s="16">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="M44" s="29"/>
       <c r="N44" s="29"/>
       <c r="O44" s="29"/>
       <c r="P44" s="29"/>
       <c r="Q44" s="29"/>
       <c r="R44" s="29"/>
       <c r="S44" s="29"/>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T44" s="29"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>66</v>
       </c>
@@ -2862,54 +2847,55 @@
         <v>3</v>
       </c>
       <c r="C45" s="16">
-        <f t="shared" ref="C45:L45" si="13">C41/$B$44</f>
+        <f t="shared" ref="C45:M45" si="14">C41/$B$44</f>
         <v>8.75</v>
       </c>
       <c r="D45" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="D45" si="15">D41/$B$44</f>
+        <v>13.75</v>
+      </c>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16">
+        <f>F41/$F$44</f>
+        <v>4</v>
+      </c>
+      <c r="G45" s="16">
+        <f t="shared" ref="G45:J45" si="16">G41/$F$44</f>
+        <v>4.8888888888888893</v>
+      </c>
+      <c r="H45" s="16">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="E45" s="16">
-        <f>E41/$E$44</f>
-        <v>4</v>
-      </c>
-      <c r="F45" s="16">
-        <f t="shared" ref="F45:I45" si="14">F41/$E$44</f>
-        <v>4.8888888888888893</v>
-      </c>
-      <c r="G45" s="16">
+      <c r="I45" s="16">
+        <f t="shared" si="16"/>
+        <v>9.6296296296296298</v>
+      </c>
+      <c r="J45" s="16">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="K45" s="16">
+        <f>K41/$K$44</f>
+        <v>8</v>
+      </c>
+      <c r="L45" s="16">
+        <f t="shared" si="14"/>
+        <v>55</v>
+      </c>
+      <c r="M45" s="16">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="H45" s="16">
-        <f t="shared" si="14"/>
-        <v>9.6296296296296298</v>
-      </c>
-      <c r="I45" s="16">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="J45" s="16">
-        <f>J41/$J$44</f>
-        <v>8</v>
-      </c>
-      <c r="K45" s="16">
-        <f t="shared" si="13"/>
-        <v>55</v>
-      </c>
-      <c r="L45" s="16">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="M45" s="29"/>
       <c r="N45" s="29"/>
       <c r="O45" s="29"/>
       <c r="P45" s="29"/>
       <c r="Q45" s="29"/>
       <c r="R45" s="29"/>
       <c r="S45" s="29"/>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T45" s="29"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>67</v>
       </c>
@@ -2918,77 +2904,79 @@
         <v>10</v>
       </c>
       <c r="C46" s="16">
-        <f t="shared" ref="C46:L46" si="15">C42/$B$44</f>
+        <f t="shared" ref="C46:M46" si="17">C42/$B$44</f>
         <v>35</v>
       </c>
       <c r="D46" s="16">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="D46" si="18">D42/$B$44</f>
+        <v>68.75</v>
+      </c>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16">
+        <f>F42/$F$44</f>
+        <v>20</v>
+      </c>
+      <c r="G46" s="16">
+        <f t="shared" ref="G46:J46" si="19">G42/$F$44</f>
+        <v>24.444444444444443</v>
+      </c>
+      <c r="H46" s="16">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="E46" s="16">
-        <f>E42/$E$44</f>
-        <v>20</v>
-      </c>
-      <c r="F46" s="16">
-        <f t="shared" ref="F46:I46" si="16">F42/$E$44</f>
-        <v>24.444444444444443</v>
-      </c>
-      <c r="G46" s="16">
-        <f t="shared" si="16"/>
+      <c r="I46" s="16">
+        <f t="shared" si="19"/>
+        <v>48.148148148148145</v>
+      </c>
+      <c r="J46" s="16">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="H46" s="16">
-        <f t="shared" si="16"/>
-        <v>48.148148148148145</v>
-      </c>
-      <c r="I46" s="16">
-        <f t="shared" si="16"/>
+      <c r="K46" s="16">
+        <f>K42/$K$44</f>
+        <v>60</v>
+      </c>
+      <c r="L46" s="16">
+        <f t="shared" si="17"/>
+        <v>412.5</v>
+      </c>
+      <c r="M46" s="16">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="J46" s="16">
-        <f>J42/$J$44</f>
-        <v>60</v>
-      </c>
-      <c r="K46" s="16">
-        <f t="shared" si="15"/>
-        <v>412.5</v>
-      </c>
-      <c r="L46" s="16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="M46" s="29"/>
       <c r="N46" s="29"/>
       <c r="O46" s="29"/>
       <c r="P46" s="29"/>
       <c r="Q46" s="29"/>
       <c r="R46" s="29"/>
       <c r="S46" s="29"/>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T46" s="29"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
-      <c r="E47" s="17"/>
+      <c r="E47" s="16"/>
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
+      <c r="I47" s="17"/>
       <c r="J47" s="18"/>
       <c r="K47" s="18"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="29"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="20"/>
       <c r="N47" s="29"/>
       <c r="O47" s="29"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="29"/>
       <c r="R47" s="29"/>
       <c r="S47" s="29"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T47" s="29"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>7</v>
       </c>
@@ -3001,49 +2989,50 @@
       <c r="D48" s="16">
         <v>280</v>
       </c>
-      <c r="E48" s="16">
+      <c r="E48" s="16"/>
+      <c r="F48" s="16">
         <v>265</v>
       </c>
-      <c r="F48" s="17">
+      <c r="G48" s="17">
         <v>150</v>
       </c>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17">
+      <c r="H48" s="17"/>
+      <c r="I48" s="17">
         <v>375</v>
       </c>
-      <c r="I48" s="18">
+      <c r="J48" s="18">
         <v>640</v>
       </c>
-      <c r="J48" s="18">
+      <c r="K48" s="18">
         <v>400</v>
       </c>
-      <c r="K48" s="18">
+      <c r="L48" s="18">
         <v>600</v>
       </c>
-      <c r="L48" s="19">
+      <c r="M48" s="19">
         <v>900</v>
       </c>
-      <c r="M48" s="23">
+      <c r="N48" s="23">
         <v>1200</v>
       </c>
-      <c r="N48" s="23">
+      <c r="O48" s="23">
         <v>30000</v>
       </c>
-      <c r="O48" s="29"/>
-      <c r="P48" s="23">
+      <c r="P48" s="29"/>
+      <c r="Q48" s="23">
         <v>3500</v>
       </c>
-      <c r="Q48" s="23">
+      <c r="R48" s="23">
         <v>2750</v>
       </c>
-      <c r="R48" s="23">
+      <c r="S48" s="23">
         <v>1600</v>
       </c>
-      <c r="S48" s="23">
+      <c r="T48" s="23">
         <v>4200</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>9</v>
       </c>
@@ -3051,42 +3040,45 @@
         <v>5</v>
       </c>
       <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="17">
+      <c r="D49" s="16">
+        <v>3</v>
+      </c>
+      <c r="E49" s="16"/>
+      <c r="F49" s="17">
         <v>3.6</v>
       </c>
-      <c r="F49" s="17">
+      <c r="G49" s="17">
         <v>2.6</v>
       </c>
-      <c r="G49" s="17"/>
       <c r="H49" s="17"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18">
+      <c r="I49" s="17"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18">
         <v>4.5</v>
       </c>
-      <c r="K49" s="18">
+      <c r="L49" s="18">
         <v>2.6</v>
       </c>
-      <c r="L49" s="20"/>
-      <c r="M49" s="29">
+      <c r="M49" s="20"/>
+      <c r="N49" s="29">
         <v>3.2</v>
       </c>
-      <c r="N49" s="23">
+      <c r="O49" s="23">
         <v>2.7</v>
       </c>
-      <c r="O49" s="29"/>
-      <c r="P49" s="23">
+      <c r="P49" s="29"/>
+      <c r="Q49" s="23">
         <v>3.75</v>
       </c>
-      <c r="Q49" s="29"/>
-      <c r="R49" s="23">
+      <c r="R49" s="29"/>
+      <c r="S49" s="23">
         <v>2.2999999999999998</v>
       </c>
-      <c r="S49" s="29">
+      <c r="T49" s="29">
         <v>3.6</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>69</v>
       </c>
@@ -3095,39 +3087,42 @@
         <v>20</v>
       </c>
       <c r="D50" s="16">
+        <v>31.25</v>
+      </c>
+      <c r="E50" s="16">
+        <v>30</v>
+      </c>
+      <c r="F50" s="16">
+        <v>25</v>
+      </c>
+      <c r="G50" s="17">
+        <v>33</v>
+      </c>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18">
         <v>35</v>
       </c>
-      <c r="E50" s="16">
-        <v>25</v>
-      </c>
-      <c r="F50" s="17">
-        <v>33</v>
-      </c>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18">
-        <v>35</v>
-      </c>
-      <c r="K50" s="18"/>
-      <c r="L50" s="19"/>
-      <c r="M50" s="29">
+      <c r="L50" s="18"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="29">
         <v>75</v>
       </c>
-      <c r="N50" s="29">
+      <c r="O50" s="29">
         <v>1380</v>
       </c>
-      <c r="O50" s="29"/>
       <c r="P50" s="29"/>
       <c r="Q50" s="29"/>
-      <c r="R50" s="29">
+      <c r="R50" s="29"/>
+      <c r="S50" s="29">
         <v>600</v>
       </c>
-      <c r="S50" s="29">
+      <c r="T50" s="29">
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>70</v>
       </c>
@@ -3138,19 +3133,20 @@
       <c r="F51" s="16"/>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
-      <c r="I51" s="18"/>
+      <c r="I51" s="16"/>
       <c r="J51" s="18"/>
       <c r="K51" s="18"/>
-      <c r="L51" s="19"/>
-      <c r="M51" s="29"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="19"/>
       <c r="N51" s="29"/>
       <c r="O51" s="29"/>
       <c r="P51" s="29"/>
       <c r="Q51" s="29"/>
       <c r="R51" s="29"/>
       <c r="S51" s="29"/>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T51" s="29"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>71</v>
       </c>
@@ -3161,44 +3157,46 @@
       <c r="F52" s="16"/>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
-      <c r="I52" s="18"/>
+      <c r="I52" s="16"/>
       <c r="J52" s="18"/>
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
-      <c r="M52" s="29"/>
+      <c r="M52" s="18"/>
       <c r="N52" s="29"/>
       <c r="O52" s="29"/>
       <c r="P52" s="29"/>
       <c r="Q52" s="29"/>
       <c r="R52" s="29"/>
       <c r="S52" s="29"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T52" s="29"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>72</v>
       </c>
       <c r="B53" s="16"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17">
+      <c r="E53" s="16"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17">
         <v>9</v>
       </c>
-      <c r="G53" s="17"/>
       <c r="H53" s="17"/>
-      <c r="I53" s="18"/>
+      <c r="I53" s="17"/>
       <c r="J53" s="18"/>
       <c r="K53" s="18"/>
-      <c r="L53" s="20"/>
-      <c r="M53" s="29"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="20"/>
       <c r="N53" s="29"/>
       <c r="O53" s="29"/>
       <c r="P53" s="29"/>
       <c r="Q53" s="29"/>
       <c r="R53" s="29"/>
       <c r="S53" s="29"/>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T53" s="29"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>73</v>
       </c>
@@ -3206,26 +3204,27 @@
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
-      <c r="F54" s="16">
+      <c r="F54" s="16"/>
+      <c r="G54" s="16">
         <v>1.5</v>
       </c>
-      <c r="G54" s="16"/>
       <c r="H54" s="16"/>
-      <c r="I54" s="18"/>
+      <c r="I54" s="16"/>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
-      <c r="M54" s="29"/>
+      <c r="M54" s="18"/>
       <c r="N54" s="29"/>
       <c r="O54" s="29"/>
       <c r="P54" s="29"/>
       <c r="Q54" s="29"/>
-      <c r="R54" s="29">
+      <c r="R54" s="29"/>
+      <c r="S54" s="29">
         <v>5</v>
       </c>
-      <c r="S54" s="29"/>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T54" s="29"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>74</v>
       </c>
@@ -3233,24 +3232,25 @@
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
-      <c r="F55" s="16">
+      <c r="F55" s="16"/>
+      <c r="G55" s="16">
         <v>5</v>
       </c>
-      <c r="G55" s="16"/>
       <c r="H55" s="16"/>
-      <c r="I55" s="18"/>
+      <c r="I55" s="16"/>
       <c r="J55" s="18"/>
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
-      <c r="M55" s="29"/>
+      <c r="M55" s="18"/>
       <c r="N55" s="29"/>
       <c r="O55" s="29"/>
       <c r="P55" s="29"/>
       <c r="Q55" s="29"/>
       <c r="R55" s="29"/>
       <c r="S55" s="29"/>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T55" s="29"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>75</v>
       </c>
@@ -3261,19 +3261,20 @@
       <c r="F56" s="16"/>
       <c r="G56" s="16"/>
       <c r="H56" s="16"/>
-      <c r="I56" s="18"/>
+      <c r="I56" s="16"/>
       <c r="J56" s="18"/>
       <c r="K56" s="18"/>
-      <c r="L56" s="19"/>
-      <c r="M56" s="29"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="19"/>
       <c r="N56" s="29"/>
       <c r="O56" s="29"/>
       <c r="P56" s="29"/>
       <c r="Q56" s="29"/>
       <c r="R56" s="29"/>
       <c r="S56" s="29"/>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T56" s="29"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>76</v>
       </c>
@@ -3281,71 +3282,79 @@
       <c r="C57" s="16">
         <v>14</v>
       </c>
-      <c r="D57" s="16"/>
-      <c r="E57" s="17">
+      <c r="D57" s="16">
+        <v>32</v>
+      </c>
+      <c r="E57" s="16">
+        <v>30</v>
+      </c>
+      <c r="F57" s="17">
         <v>18</v>
       </c>
-      <c r="F57" s="17">
+      <c r="G57" s="17">
         <v>28</v>
       </c>
-      <c r="G57" s="17"/>
       <c r="H57" s="17"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18">
+      <c r="I57" s="17"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18">
         <v>23</v>
       </c>
-      <c r="K57" s="18"/>
-      <c r="L57" s="20"/>
-      <c r="M57" s="29">
+      <c r="L57" s="18"/>
+      <c r="M57" s="20"/>
+      <c r="N57" s="29">
         <v>20</v>
       </c>
-      <c r="N57" s="23">
+      <c r="O57" s="23">
         <v>35</v>
       </c>
-      <c r="O57" s="29"/>
       <c r="P57" s="29"/>
-      <c r="Q57" s="29">
+      <c r="Q57" s="29"/>
+      <c r="R57" s="29">
         <v>35</v>
       </c>
-      <c r="R57" s="29"/>
-      <c r="S57" s="29">
+      <c r="S57" s="29"/>
+      <c r="T57" s="29">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="17">
+      <c r="D58" s="16">
         <v>20</v>
       </c>
+      <c r="E58" s="16"/>
       <c r="F58" s="17">
         <v>20</v>
       </c>
-      <c r="G58" s="17"/>
+      <c r="G58" s="17">
+        <v>20</v>
+      </c>
       <c r="H58" s="17"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="18">
+      <c r="I58" s="17"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18">
         <v>15</v>
       </c>
-      <c r="K58" s="18">
+      <c r="L58" s="18">
         <v>18</v>
       </c>
-      <c r="L58" s="23"/>
-      <c r="M58" s="29"/>
+      <c r="M58" s="23"/>
       <c r="N58" s="29"/>
       <c r="O58" s="29"/>
       <c r="P58" s="29"/>
       <c r="Q58" s="29"/>
       <c r="R58" s="29"/>
       <c r="S58" s="29"/>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T58" s="29"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>77</v>
       </c>
@@ -3355,38 +3364,39 @@
       <c r="C59" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D59" s="14"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="G59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H59" s="15"/>
       <c r="I59" s="15"/>
       <c r="J59" s="15"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
-      <c r="M59" t="s">
+      <c r="M59" s="15"/>
+      <c r="N59" t="s">
+        <v>112</v>
+      </c>
+      <c r="O59" t="s">
         <v>113</v>
       </c>
-      <c r="N59" t="s">
-        <v>114</v>
-      </c>
-      <c r="P59" t="s">
-        <v>120</v>
-      </c>
-      <c r="R59" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q59" t="s">
+        <v>119</v>
+      </c>
+      <c r="S59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>78</v>
       </c>
       <c r="B60" s="14"/>
       <c r="C60" s="15"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="14"/>
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
@@ -3394,14 +3404,15 @@
       <c r="J60" s="15"/>
       <c r="K60" s="15"/>
       <c r="L60" s="15"/>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M60" s="15"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>79</v>
       </c>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
-      <c r="D61" s="15"/>
+      <c r="D61" s="14"/>
       <c r="E61" s="15"/>
       <c r="F61" s="15"/>
       <c r="G61" s="15"/>
@@ -3410,212 +3421,213 @@
       <c r="J61" s="15"/>
       <c r="K61" s="15"/>
       <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
     </row>
     <row r="67" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C67" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D67" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E67" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G67" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H67" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J67" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K67" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M67" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N67" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O67" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R67" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S67" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T67" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="V67" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="W67" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X67" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z67" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AA67" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AB67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AC67" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AD67" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AE67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AF67" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AG67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AH67" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AI67" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AJ67" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AL67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F68" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G68" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H68" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J68" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K68" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L68" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M68" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N68" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P68" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R68" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="S68" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T68" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="U68" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="V68" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W68" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="X68" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z68" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AA68" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AB68" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AC68" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AD68" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AE68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AF68" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AG68" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AH68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AI68" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AJ68" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL68" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B70">
         <v>8000</v>
@@ -3690,19 +3702,19 @@
         <v>7000</v>
       </c>
       <c r="AF70" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AG70" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AH70" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AI70">
         <v>3800</v>
       </c>
       <c r="AJ70" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AL70">
         <v>500</v>
@@ -3710,7 +3722,7 @@
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B71">
         <v>13300</v>
@@ -3793,7 +3805,7 @@
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B72">
         <v>1520</v>
@@ -3876,7 +3888,7 @@
     </row>
     <row r="73" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B73">
         <v>2600</v>
@@ -3959,7 +3971,7 @@
     </row>
     <row r="74" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B74">
         <v>40</v>
@@ -4003,7 +4015,7 @@
     </row>
     <row r="75" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J75">
         <v>150</v>
@@ -4035,7 +4047,7 @@
     </row>
     <row r="76" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J76">
         <v>1</v>
@@ -4043,7 +4055,7 @@
     </row>
     <row r="77" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="R77">
         <v>35</v>
@@ -4084,7 +4096,7 @@
     </row>
     <row r="78" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R78">
         <v>44</v>
@@ -4125,7 +4137,7 @@
     </row>
     <row r="79" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S79">
         <v>1.5</v>
@@ -4160,7 +4172,7 @@
     </row>
     <row r="80" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R80">
         <v>2</v>
@@ -4189,7 +4201,7 @@
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="V81">
         <v>5</v>
@@ -4200,135 +4212,135 @@
     </row>
     <row r="82" spans="1:30" x14ac:dyDescent="0.25">
       <c r="Z82" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AA82" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB82" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AC82" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B87" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C87" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D87" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E87" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F87" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G87" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H87" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I87" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J87" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K87" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L87" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B88" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C88" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D88" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E88" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F88" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G88" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H88" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I88" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J88" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K88" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L88" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B89" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C89" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D89" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E89" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F89" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G89" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H89" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I89" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J89" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K89" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L89" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B90">
         <v>500</v>
@@ -4357,7 +4369,7 @@
     </row>
     <row r="92" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B92">
         <v>2880</v>
@@ -4386,7 +4398,7 @@
     </row>
     <row r="93" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B93">
         <v>360</v>
@@ -4415,7 +4427,7 @@
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B94">
         <v>1440</v>
@@ -4444,7 +4456,7 @@
     </row>
     <row r="96" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B96">
         <v>6</v>
@@ -4473,45 +4485,45 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E97" t="s">
+        <v>235</v>
+      </c>
+      <c r="F97" t="s">
+        <v>234</v>
+      </c>
+      <c r="G97" t="s">
+        <v>240</v>
+      </c>
+      <c r="H97" t="s">
+        <v>241</v>
+      </c>
+      <c r="I97" t="s">
+        <v>245</v>
+      </c>
+      <c r="J97" t="s">
+        <v>246</v>
+      </c>
+      <c r="K97" t="s">
+        <v>234</v>
+      </c>
+      <c r="L97" t="s">
         <v>236</v>
       </c>
-      <c r="F97" t="s">
-        <v>235</v>
-      </c>
-      <c r="G97" t="s">
+      <c r="M97" t="s">
+        <v>255</v>
+      </c>
+      <c r="N97" t="s">
         <v>241</v>
       </c>
-      <c r="H97" t="s">
-        <v>242</v>
-      </c>
-      <c r="I97" t="s">
-        <v>246</v>
-      </c>
-      <c r="J97" t="s">
-        <v>247</v>
-      </c>
-      <c r="K97" t="s">
-        <v>235</v>
-      </c>
-      <c r="L97" t="s">
-        <v>237</v>
-      </c>
-      <c r="M97" t="s">
-        <v>256</v>
-      </c>
-      <c r="N97" t="s">
-        <v>242</v>
-      </c>
       <c r="O97" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B98">
         <v>25</v>
@@ -4558,7 +4570,7 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -4602,7 +4614,7 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B100">
         <v>2</v>
@@ -4649,7 +4661,7 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B101">
         <v>32</v>
@@ -4696,7 +4708,7 @@
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B102">
         <v>0.83299999999999996</v>
@@ -4743,7 +4755,7 @@
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B103">
         <v>41.6</v>
@@ -4752,7 +4764,7 @@
         <v>60</v>
       </c>
       <c r="D103" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E103">
         <v>50</v>
@@ -4790,16 +4802,16 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>227</v>
+      </c>
+      <c r="D105" t="s">
         <v>228</v>
       </c>
-      <c r="D105" t="s">
-        <v>229</v>
-      </c>
       <c r="J105" t="s">
+        <v>253</v>
+      </c>
+      <c r="L105" t="s">
         <v>254</v>
-      </c>
-      <c r="L105" t="s">
-        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -4809,82 +4821,82 @@
     <mergeCell ref="J6:M6"/>
   </mergeCells>
   <conditionalFormatting sqref="G9:M33">
-    <cfRule type="expression" dxfId="51" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="71" stopIfTrue="1">
       <formula>G9&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="72" stopIfTrue="1">
       <formula>MOD(G9,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F3">
-    <cfRule type="expression" dxfId="39" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="61" stopIfTrue="1">
       <formula>B2&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="62" stopIfTrue="1">
       <formula>MOD(B2,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:F12">
-    <cfRule type="expression" dxfId="31" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="31" stopIfTrue="1">
       <formula>B12&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="32" stopIfTrue="1">
       <formula>MOD(B12,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:F33">
-    <cfRule type="expression" dxfId="21" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
       <formula>B25&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
       <formula>MOD(B25,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:F21">
-    <cfRule type="expression" dxfId="19" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="35" stopIfTrue="1">
       <formula>B20&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="36" stopIfTrue="1">
       <formula>MOD(B20,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:F22">
-    <cfRule type="expression" dxfId="17" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="33" stopIfTrue="1">
       <formula>B22&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="34" stopIfTrue="1">
       <formula>MOD(B22,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:F23">
-    <cfRule type="expression" dxfId="15" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="29" stopIfTrue="1">
       <formula>B23&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="30" stopIfTrue="1">
       <formula>MOD(B23,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:F33">
-    <cfRule type="expression" dxfId="13" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="39" stopIfTrue="1">
       <formula>B9&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="40" stopIfTrue="1">
       <formula>MOD(B9,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:F15">
-    <cfRule type="expression" dxfId="11" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="27" stopIfTrue="1">
       <formula>E15&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="28" stopIfTrue="1">
       <formula>MOD(E15,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:F16">
-    <cfRule type="expression" dxfId="9" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="25" stopIfTrue="1">
       <formula>E16&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="26" stopIfTrue="1">
       <formula>MOD(E16,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Revert "t1 artylery bombrd move"
This reverts commit ab6a54d48499b7422870041528c2e6e0ddf5e74f.
</commit_message>
<xml_diff>
--- a/Units.xlsx
+++ b/Units.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="259">
   <si>
     <t>Stats</t>
   </si>
@@ -273,6 +273,9 @@
     <t>lab</t>
   </si>
   <si>
+    <t>aa/arty</t>
+  </si>
+  <si>
     <t>tank</t>
   </si>
   <si>
@@ -793,36 +796,6 @@
   </si>
   <si>
     <t>Golem</t>
-  </si>
-  <si>
-    <t>inu1007</t>
-  </si>
-  <si>
-    <t>Astor</t>
-  </si>
-  <si>
-    <t>inu1004</t>
-  </si>
-  <si>
-    <t>inu1001</t>
-  </si>
-  <si>
-    <t>inu1005</t>
-  </si>
-  <si>
-    <t>inu1006</t>
-  </si>
-  <si>
-    <t>inu1008</t>
-  </si>
-  <si>
-    <t>inu1002</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>arty</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1086,85 @@
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="52">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1504,10 +1555,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A73" sqref="A73"/>
-      <selection pane="topRight" activeCell="E50" sqref="E50"/>
+      <selection pane="topRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,19 +1613,19 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C5" t="s">
         <v>211</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>210</v>
       </c>
-      <c r="D5" t="s">
-        <v>209</v>
-      </c>
       <c r="E5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1615,7 +1666,7 @@
         <v>37</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>43</v>
@@ -2396,7 +2447,7 @@
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
@@ -2413,12 +2464,12 @@
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>15</v>
       </c>
@@ -2433,7 +2484,7 @@
       </c>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>19</v>
       </c>
@@ -2448,69 +2499,51 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="26" t="s">
-        <v>265</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>258</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>263</v>
-      </c>
-      <c r="E38" s="26" t="s">
-        <v>263</v>
-      </c>
-      <c r="F38" s="26" t="s">
-        <v>260</v>
-      </c>
-      <c r="G38" s="26" t="s">
-        <v>264</v>
-      </c>
-      <c r="H38" s="26" t="s">
-        <v>261</v>
-      </c>
-      <c r="I38" s="26" t="s">
-        <v>262</v>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="I38" t="s">
+        <v>96</v>
       </c>
       <c r="J38" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K38" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="L38" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="M38" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="N38" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="O38" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="P38" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="Q38" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="R38" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="S38" t="s">
-        <v>123</v>
-      </c>
-      <c r="T38" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>82</v>
       </c>
@@ -2521,111 +2554,103 @@
         <v>83</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>266</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>267</v>
+        <v>84</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>85</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H39" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="I39" s="22" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="I39" s="27" t="s">
+        <v>97</v>
       </c>
       <c r="J39" s="27" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="K39" s="27" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="L39" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="M39" s="27" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="M39" s="22" t="s">
+        <v>108</v>
       </c>
       <c r="N39" s="22" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="O39" s="22" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="P39" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="Q39" s="22" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="R39" s="22" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="S39" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="T39" s="22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>61</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>259</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C40" s="24"/>
       <c r="D40" s="24" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="G40" s="24" t="s">
-        <v>93</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="G40" s="24"/>
       <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25" t="s">
+        <v>100</v>
+      </c>
       <c r="K40" s="25" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="L40" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="M40" s="25" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="M40" s="28" t="s">
+        <v>109</v>
       </c>
       <c r="N40" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="O40" s="28" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="P40" s="28" t="s">
+        <v>119</v>
       </c>
       <c r="Q40" s="28" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="R40" s="28" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="S40" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="T40" s="28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>62</v>
       </c>
@@ -2635,49 +2660,46 @@
       <c r="C41" s="16">
         <v>35</v>
       </c>
-      <c r="D41" s="16">
-        <v>55</v>
-      </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16">
+      <c r="D41" s="16"/>
+      <c r="E41" s="16">
         <v>54</v>
       </c>
-      <c r="G41" s="17">
+      <c r="F41" s="17">
         <v>66</v>
       </c>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17">
+      <c r="G41" s="17"/>
+      <c r="H41" s="17">
         <v>130</v>
       </c>
-      <c r="J41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18">
+        <v>100</v>
+      </c>
       <c r="K41" s="18">
-        <v>100</v>
-      </c>
-      <c r="L41" s="18">
         <v>220</v>
       </c>
-      <c r="M41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="23">
+        <v>197</v>
+      </c>
       <c r="N41" s="23">
-        <v>197</v>
-      </c>
-      <c r="O41" s="23">
         <v>12500</v>
       </c>
-      <c r="P41" s="29"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="23">
+        <v>640</v>
+      </c>
       <c r="Q41" s="23">
-        <v>640</v>
+        <v>360</v>
       </c>
       <c r="R41" s="23">
-        <v>360</v>
+        <v>960</v>
       </c>
       <c r="S41" s="23">
-        <v>960</v>
-      </c>
-      <c r="T41" s="23">
         <v>480</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>63</v>
       </c>
@@ -2687,49 +2709,46 @@
       <c r="C42" s="16">
         <v>140</v>
       </c>
-      <c r="D42" s="16">
-        <v>275</v>
-      </c>
-      <c r="E42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="17">
+        <v>270</v>
+      </c>
       <c r="F42" s="17">
-        <v>270</v>
-      </c>
-      <c r="G42" s="17">
         <v>330</v>
       </c>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17">
+      <c r="G42" s="17"/>
+      <c r="H42" s="17">
         <v>650</v>
       </c>
-      <c r="J42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18">
+        <v>750</v>
+      </c>
       <c r="K42" s="18">
-        <v>750</v>
-      </c>
-      <c r="L42" s="18">
         <v>1650</v>
       </c>
-      <c r="M42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="23">
+        <v>990</v>
+      </c>
       <c r="N42" s="23">
-        <v>990</v>
-      </c>
-      <c r="O42" s="23">
         <v>240000</v>
       </c>
-      <c r="P42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="23">
+        <v>8000</v>
+      </c>
       <c r="Q42" s="23">
-        <v>8000</v>
+        <v>1800</v>
       </c>
       <c r="R42" s="23">
-        <v>1800</v>
+        <v>9600</v>
       </c>
       <c r="S42" s="23">
-        <v>9600</v>
-      </c>
-      <c r="T42" s="23">
         <v>5400</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>64</v>
       </c>
@@ -2739,49 +2758,46 @@
       <c r="C43" s="16">
         <v>120</v>
       </c>
-      <c r="D43" s="16">
-        <v>220</v>
-      </c>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16">
+      <c r="D43" s="16"/>
+      <c r="E43" s="16">
         <v>270</v>
       </c>
-      <c r="G43" s="17">
+      <c r="F43" s="17">
         <v>330</v>
       </c>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17">
+      <c r="G43" s="17"/>
+      <c r="H43" s="17">
         <v>650</v>
       </c>
-      <c r="J43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18">
+        <v>500</v>
+      </c>
       <c r="K43" s="18">
-        <v>500</v>
-      </c>
-      <c r="L43" s="18">
         <v>1100</v>
       </c>
-      <c r="M43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="23">
+        <v>880</v>
+      </c>
       <c r="N43" s="23">
-        <v>880</v>
-      </c>
-      <c r="O43" s="23">
         <v>12000</v>
       </c>
-      <c r="P43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="23">
+        <v>640</v>
+      </c>
       <c r="Q43" s="23">
-        <v>640</v>
+        <v>1600</v>
       </c>
       <c r="R43" s="23">
-        <v>1600</v>
+        <v>5000</v>
       </c>
       <c r="S43" s="23">
-        <v>5000</v>
-      </c>
-      <c r="T43" s="23">
         <v>2400</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>65</v>
       </c>
@@ -2790,55 +2806,54 @@
         <v>4</v>
       </c>
       <c r="C44" s="16">
-        <f t="shared" ref="C44:M44" si="9">C43/$B$36</f>
+        <f t="shared" ref="C44:L44" si="9">C43/$B$36</f>
         <v>6</v>
       </c>
       <c r="D44" s="16">
-        <f t="shared" ref="D44" si="10">D43/$B$36</f>
-        <v>11</v>
-      </c>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="16">
         <f t="shared" si="9"/>
         <v>13.5</v>
       </c>
+      <c r="F44" s="16">
+        <f t="shared" ref="F44" si="10">F43/$B$36</f>
+        <v>16.5</v>
+      </c>
       <c r="G44" s="16">
         <f t="shared" ref="G44" si="11">G43/$B$36</f>
-        <v>16.5</v>
+        <v>0</v>
       </c>
       <c r="H44" s="16">
-        <f t="shared" ref="H44" si="12">H43/$B$36</f>
+        <f>H43/$B$36</f>
+        <v>32.5</v>
+      </c>
+      <c r="I44" s="16">
+        <f t="shared" ref="I44" si="12">I43/$B$36</f>
         <v>0</v>
       </c>
-      <c r="I44" s="16">
-        <f>I43/$B$36</f>
-        <v>32.5</v>
-      </c>
       <c r="J44" s="16">
-        <f t="shared" ref="J44" si="13">J43/$B$36</f>
-        <v>0</v>
+        <f>J43/$C$36</f>
+        <v>12.5</v>
       </c>
       <c r="K44" s="16">
-        <f>K43/$C$36</f>
-        <v>12.5</v>
+        <f t="shared" si="9"/>
+        <v>55</v>
       </c>
       <c r="L44" s="16">
         <f t="shared" si="9"/>
-        <v>55</v>
-      </c>
-      <c r="M44" s="16">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="M44" s="29"/>
       <c r="N44" s="29"/>
       <c r="O44" s="29"/>
       <c r="P44" s="29"/>
       <c r="Q44" s="29"/>
       <c r="R44" s="29"/>
       <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>66</v>
       </c>
@@ -2847,55 +2862,54 @@
         <v>3</v>
       </c>
       <c r="C45" s="16">
-        <f t="shared" ref="C45:M45" si="14">C41/$B$44</f>
+        <f t="shared" ref="C45:L45" si="13">C41/$B$44</f>
         <v>8.75</v>
       </c>
       <c r="D45" s="16">
-        <f t="shared" ref="D45" si="15">D41/$B$44</f>
-        <v>13.75</v>
-      </c>
-      <c r="E45" s="16"/>
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="16">
+        <f>E41/$E$44</f>
+        <v>4</v>
+      </c>
       <c r="F45" s="16">
-        <f>F41/$F$44</f>
-        <v>4</v>
+        <f t="shared" ref="F45:I45" si="14">F41/$E$44</f>
+        <v>4.8888888888888893</v>
       </c>
       <c r="G45" s="16">
-        <f t="shared" ref="G45:J45" si="16">G41/$F$44</f>
-        <v>4.8888888888888893</v>
-      </c>
-      <c r="H45" s="16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I45" s="16">
-        <f t="shared" si="16"/>
-        <v>9.6296296296296298</v>
-      </c>
-      <c r="J45" s="16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="K45" s="16">
-        <f>K41/$K$44</f>
-        <v>8</v>
-      </c>
-      <c r="L45" s="16">
-        <f t="shared" si="14"/>
-        <v>55</v>
-      </c>
-      <c r="M45" s="16">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="H45" s="16">
+        <f t="shared" si="14"/>
+        <v>9.6296296296296298</v>
+      </c>
+      <c r="I45" s="16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="16">
+        <f>J41/$J$44</f>
+        <v>8</v>
+      </c>
+      <c r="K45" s="16">
+        <f t="shared" si="13"/>
+        <v>55</v>
+      </c>
+      <c r="L45" s="16">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="29"/>
       <c r="N45" s="29"/>
       <c r="O45" s="29"/>
       <c r="P45" s="29"/>
       <c r="Q45" s="29"/>
       <c r="R45" s="29"/>
       <c r="S45" s="29"/>
-      <c r="T45" s="29"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>67</v>
       </c>
@@ -2904,79 +2918,77 @@
         <v>10</v>
       </c>
       <c r="C46" s="16">
-        <f t="shared" ref="C46:M46" si="17">C42/$B$44</f>
+        <f t="shared" ref="C46:L46" si="15">C42/$B$44</f>
         <v>35</v>
       </c>
       <c r="D46" s="16">
-        <f t="shared" ref="D46" si="18">D42/$B$44</f>
-        <v>68.75</v>
-      </c>
-      <c r="E46" s="16"/>
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="16">
+        <f>E42/$E$44</f>
+        <v>20</v>
+      </c>
       <c r="F46" s="16">
-        <f>F42/$F$44</f>
-        <v>20</v>
+        <f t="shared" ref="F46:I46" si="16">F42/$E$44</f>
+        <v>24.444444444444443</v>
       </c>
       <c r="G46" s="16">
-        <f t="shared" ref="G46:J46" si="19">G42/$F$44</f>
-        <v>24.444444444444443</v>
+        <f t="shared" si="16"/>
+        <v>0</v>
       </c>
       <c r="H46" s="16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
+        <v>48.148148148148145</v>
+      </c>
+      <c r="I46" s="16">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I46" s="16">
-        <f t="shared" si="19"/>
-        <v>48.148148148148145</v>
-      </c>
       <c r="J46" s="16">
-        <f t="shared" si="19"/>
+        <f>J42/$J$44</f>
+        <v>60</v>
+      </c>
+      <c r="K46" s="16">
+        <f t="shared" si="15"/>
+        <v>412.5</v>
+      </c>
+      <c r="L46" s="16">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="K46" s="16">
-        <f>K42/$K$44</f>
-        <v>60</v>
-      </c>
-      <c r="L46" s="16">
-        <f t="shared" si="17"/>
-        <v>412.5</v>
-      </c>
-      <c r="M46" s="16">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
+      <c r="M46" s="29"/>
       <c r="N46" s="29"/>
       <c r="O46" s="29"/>
       <c r="P46" s="29"/>
       <c r="Q46" s="29"/>
       <c r="R46" s="29"/>
       <c r="S46" s="29"/>
-      <c r="T46" s="29"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
+      <c r="E47" s="17"/>
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
+      <c r="I47" s="18"/>
       <c r="J47" s="18"/>
       <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="20"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="29"/>
       <c r="N47" s="29"/>
       <c r="O47" s="29"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="29"/>
       <c r="R47" s="29"/>
       <c r="S47" s="29"/>
-      <c r="T47" s="29"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>7</v>
       </c>
@@ -2989,50 +3001,49 @@
       <c r="D48" s="16">
         <v>280</v>
       </c>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16">
+      <c r="E48" s="16">
         <v>265</v>
       </c>
-      <c r="G48" s="17">
+      <c r="F48" s="17">
         <v>150</v>
       </c>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17">
+      <c r="G48" s="17"/>
+      <c r="H48" s="17">
         <v>375</v>
       </c>
+      <c r="I48" s="18">
+        <v>640</v>
+      </c>
       <c r="J48" s="18">
-        <v>640</v>
+        <v>400</v>
       </c>
       <c r="K48" s="18">
-        <v>400</v>
-      </c>
-      <c r="L48" s="18">
         <v>600</v>
       </c>
-      <c r="M48" s="19">
+      <c r="L48" s="19">
         <v>900</v>
       </c>
+      <c r="M48" s="23">
+        <v>1200</v>
+      </c>
       <c r="N48" s="23">
-        <v>1200</v>
-      </c>
-      <c r="O48" s="23">
         <v>30000</v>
       </c>
-      <c r="P48" s="29"/>
+      <c r="O48" s="29"/>
+      <c r="P48" s="23">
+        <v>3500</v>
+      </c>
       <c r="Q48" s="23">
-        <v>3500</v>
+        <v>2750</v>
       </c>
       <c r="R48" s="23">
-        <v>2750</v>
+        <v>1600</v>
       </c>
       <c r="S48" s="23">
-        <v>1600</v>
-      </c>
-      <c r="T48" s="23">
         <v>4200</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>9</v>
       </c>
@@ -3040,45 +3051,42 @@
         <v>5</v>
       </c>
       <c r="C49" s="16"/>
-      <c r="D49" s="16">
-        <v>3</v>
-      </c>
-      <c r="E49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="17">
+        <v>3.6</v>
+      </c>
       <c r="F49" s="17">
+        <v>2.6</v>
+      </c>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18">
+        <v>4.5</v>
+      </c>
+      <c r="K49" s="18">
+        <v>2.6</v>
+      </c>
+      <c r="L49" s="20"/>
+      <c r="M49" s="29">
+        <v>3.2</v>
+      </c>
+      <c r="N49" s="23">
+        <v>2.7</v>
+      </c>
+      <c r="O49" s="29"/>
+      <c r="P49" s="23">
+        <v>3.75</v>
+      </c>
+      <c r="Q49" s="29"/>
+      <c r="R49" s="23">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="S49" s="29">
         <v>3.6</v>
       </c>
-      <c r="G49" s="17">
-        <v>2.6</v>
-      </c>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18">
-        <v>4.5</v>
-      </c>
-      <c r="L49" s="18">
-        <v>2.6</v>
-      </c>
-      <c r="M49" s="20"/>
-      <c r="N49" s="29">
-        <v>3.2</v>
-      </c>
-      <c r="O49" s="23">
-        <v>2.7</v>
-      </c>
-      <c r="P49" s="29"/>
-      <c r="Q49" s="23">
-        <v>3.75</v>
-      </c>
-      <c r="R49" s="29"/>
-      <c r="S49" s="23">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="T49" s="29">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>69</v>
       </c>
@@ -3087,42 +3095,39 @@
         <v>20</v>
       </c>
       <c r="D50" s="16">
-        <v>31.25</v>
+        <v>35</v>
       </c>
       <c r="E50" s="16">
-        <v>30</v>
-      </c>
-      <c r="F50" s="16">
         <v>25</v>
       </c>
-      <c r="G50" s="17">
+      <c r="F50" s="17">
         <v>33</v>
       </c>
+      <c r="G50" s="17"/>
       <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18">
+      <c r="I50" s="18"/>
+      <c r="J50" s="18">
         <v>35</v>
       </c>
-      <c r="L50" s="18"/>
-      <c r="M50" s="19"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="29">
+        <v>75</v>
+      </c>
       <c r="N50" s="29">
-        <v>75</v>
-      </c>
-      <c r="O50" s="29">
         <v>1380</v>
       </c>
+      <c r="O50" s="29"/>
       <c r="P50" s="29"/>
       <c r="Q50" s="29"/>
-      <c r="R50" s="29"/>
+      <c r="R50" s="29">
+        <v>600</v>
+      </c>
       <c r="S50" s="29">
-        <v>600</v>
-      </c>
-      <c r="T50" s="29">
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>70</v>
       </c>
@@ -3133,20 +3138,19 @@
       <c r="F51" s="16"/>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
-      <c r="I51" s="16"/>
+      <c r="I51" s="18"/>
       <c r="J51" s="18"/>
       <c r="K51" s="18"/>
-      <c r="L51" s="18"/>
-      <c r="M51" s="19"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="29"/>
       <c r="N51" s="29"/>
       <c r="O51" s="29"/>
       <c r="P51" s="29"/>
       <c r="Q51" s="29"/>
       <c r="R51" s="29"/>
       <c r="S51" s="29"/>
-      <c r="T51" s="29"/>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>71</v>
       </c>
@@ -3157,46 +3161,44 @@
       <c r="F52" s="16"/>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
-      <c r="I52" s="16"/>
+      <c r="I52" s="18"/>
       <c r="J52" s="18"/>
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
-      <c r="M52" s="18"/>
+      <c r="M52" s="29"/>
       <c r="N52" s="29"/>
       <c r="O52" s="29"/>
       <c r="P52" s="29"/>
       <c r="Q52" s="29"/>
       <c r="R52" s="29"/>
       <c r="S52" s="29"/>
-      <c r="T52" s="29"/>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>72</v>
       </c>
       <c r="B53" s="16"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17">
+      <c r="E53" s="17"/>
+      <c r="F53" s="17">
         <v>9</v>
       </c>
+      <c r="G53" s="17"/>
       <c r="H53" s="17"/>
-      <c r="I53" s="17"/>
+      <c r="I53" s="18"/>
       <c r="J53" s="18"/>
       <c r="K53" s="18"/>
-      <c r="L53" s="18"/>
-      <c r="M53" s="20"/>
+      <c r="L53" s="20"/>
+      <c r="M53" s="29"/>
       <c r="N53" s="29"/>
       <c r="O53" s="29"/>
       <c r="P53" s="29"/>
       <c r="Q53" s="29"/>
       <c r="R53" s="29"/>
       <c r="S53" s="29"/>
-      <c r="T53" s="29"/>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>73</v>
       </c>
@@ -3204,27 +3206,26 @@
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16">
+      <c r="F54" s="16">
         <v>1.5</v>
       </c>
+      <c r="G54" s="16"/>
       <c r="H54" s="16"/>
-      <c r="I54" s="16"/>
+      <c r="I54" s="18"/>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
-      <c r="M54" s="18"/>
+      <c r="M54" s="29"/>
       <c r="N54" s="29"/>
       <c r="O54" s="29"/>
       <c r="P54" s="29"/>
       <c r="Q54" s="29"/>
-      <c r="R54" s="29"/>
-      <c r="S54" s="29">
+      <c r="R54" s="29">
         <v>5</v>
       </c>
-      <c r="T54" s="29"/>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S54" s="29"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>74</v>
       </c>
@@ -3232,25 +3233,24 @@
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16">
+      <c r="F55" s="16">
         <v>5</v>
       </c>
+      <c r="G55" s="16"/>
       <c r="H55" s="16"/>
-      <c r="I55" s="16"/>
+      <c r="I55" s="18"/>
       <c r="J55" s="18"/>
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
-      <c r="M55" s="18"/>
+      <c r="M55" s="29"/>
       <c r="N55" s="29"/>
       <c r="O55" s="29"/>
       <c r="P55" s="29"/>
       <c r="Q55" s="29"/>
       <c r="R55" s="29"/>
       <c r="S55" s="29"/>
-      <c r="T55" s="29"/>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>75</v>
       </c>
@@ -3261,20 +3261,19 @@
       <c r="F56" s="16"/>
       <c r="G56" s="16"/>
       <c r="H56" s="16"/>
-      <c r="I56" s="16"/>
+      <c r="I56" s="18"/>
       <c r="J56" s="18"/>
       <c r="K56" s="18"/>
-      <c r="L56" s="18"/>
-      <c r="M56" s="19"/>
+      <c r="L56" s="19"/>
+      <c r="M56" s="29"/>
       <c r="N56" s="29"/>
       <c r="O56" s="29"/>
       <c r="P56" s="29"/>
       <c r="Q56" s="29"/>
       <c r="R56" s="29"/>
       <c r="S56" s="29"/>
-      <c r="T56" s="29"/>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>76</v>
       </c>
@@ -3282,79 +3281,71 @@
       <c r="C57" s="16">
         <v>14</v>
       </c>
-      <c r="D57" s="16">
-        <v>32</v>
-      </c>
-      <c r="E57" s="16">
-        <v>30</v>
+      <c r="D57" s="16"/>
+      <c r="E57" s="17">
+        <v>18</v>
       </c>
       <c r="F57" s="17">
-        <v>18</v>
-      </c>
-      <c r="G57" s="17">
         <v>28</v>
       </c>
+      <c r="G57" s="17"/>
       <c r="H57" s="17"/>
-      <c r="I57" s="17"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18">
+      <c r="I57" s="18"/>
+      <c r="J57" s="18">
         <v>23</v>
       </c>
-      <c r="L57" s="18"/>
-      <c r="M57" s="20"/>
-      <c r="N57" s="29">
+      <c r="K57" s="18"/>
+      <c r="L57" s="20"/>
+      <c r="M57" s="29">
         <v>20</v>
       </c>
-      <c r="O57" s="23">
+      <c r="N57" s="23">
         <v>35</v>
       </c>
+      <c r="O57" s="29"/>
       <c r="P57" s="29"/>
-      <c r="Q57" s="29"/>
-      <c r="R57" s="29">
+      <c r="Q57" s="29">
         <v>35</v>
       </c>
-      <c r="S57" s="29"/>
-      <c r="T57" s="29">
+      <c r="R57" s="29"/>
+      <c r="S57" s="29">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C58" s="16"/>
-      <c r="D58" s="16">
+      <c r="D58" s="16"/>
+      <c r="E58" s="17">
         <v>20</v>
       </c>
-      <c r="E58" s="16"/>
       <c r="F58" s="17">
         <v>20</v>
       </c>
-      <c r="G58" s="17">
-        <v>20</v>
-      </c>
+      <c r="G58" s="17"/>
       <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18">
+        <v>15</v>
+      </c>
       <c r="K58" s="18">
-        <v>15</v>
-      </c>
-      <c r="L58" s="18">
         <v>18</v>
       </c>
-      <c r="M58" s="23"/>
+      <c r="L58" s="23"/>
+      <c r="M58" s="29"/>
       <c r="N58" s="29"/>
       <c r="O58" s="29"/>
       <c r="P58" s="29"/>
       <c r="Q58" s="29"/>
       <c r="R58" s="29"/>
       <c r="S58" s="29"/>
-      <c r="T58" s="29"/>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>77</v>
       </c>
@@ -3364,39 +3355,38 @@
       <c r="C59" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D59" s="15"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15" t="s">
-        <v>94</v>
-      </c>
+      <c r="D59" s="14"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G59" s="15"/>
       <c r="H59" s="15"/>
       <c r="I59" s="15"/>
       <c r="J59" s="15"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
-      <c r="M59" s="15"/>
+      <c r="M59" t="s">
+        <v>113</v>
+      </c>
       <c r="N59" t="s">
-        <v>112</v>
-      </c>
-      <c r="O59" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>119</v>
-      </c>
-      <c r="S59" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="P59" t="s">
+        <v>120</v>
+      </c>
+      <c r="R59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>78</v>
       </c>
       <c r="B60" s="14"/>
       <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="15"/>
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
@@ -3404,15 +3394,14 @@
       <c r="J60" s="15"/>
       <c r="K60" s="15"/>
       <c r="L60" s="15"/>
-      <c r="M60" s="15"/>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>79</v>
       </c>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
+      <c r="D61" s="15"/>
       <c r="E61" s="15"/>
       <c r="F61" s="15"/>
       <c r="G61" s="15"/>
@@ -3421,213 +3410,212 @@
       <c r="J61" s="15"/>
       <c r="K61" s="15"/>
       <c r="L61" s="15"/>
-      <c r="M61" s="15"/>
     </row>
     <row r="67" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C67" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D67" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E67" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F67" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G67" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H67" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J67" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K67" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L67" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M67" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="N67" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="O67" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="P67" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="R67" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="S67" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="T67" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U67" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="V67" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="W67" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="X67" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Z67" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AA67" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AB67" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AC67" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AD67" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AE67" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AF67" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AG67" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AH67" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AI67" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AJ67" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AL67" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
+        <v>139</v>
+      </c>
+      <c r="C68" t="s">
         <v>138</v>
       </c>
-      <c r="C68" t="s">
-        <v>137</v>
-      </c>
       <c r="D68" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E68" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F68" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G68" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H68" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J68" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K68" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="L68" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M68" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N68" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="O68" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="P68" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="R68" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="S68" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="T68" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="U68" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="V68" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="W68" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="X68" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Z68" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AA68" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AB68" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AC68" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AD68" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AE68" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AF68" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AG68" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AH68" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AI68" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AJ68" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AL68" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B70">
         <v>8000</v>
@@ -3702,19 +3690,19 @@
         <v>7000</v>
       </c>
       <c r="AF70" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AG70" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AH70" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AI70">
         <v>3800</v>
       </c>
       <c r="AJ70" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AL70">
         <v>500</v>
@@ -3722,7 +3710,7 @@
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B71">
         <v>13300</v>
@@ -3805,7 +3793,7 @@
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B72">
         <v>1520</v>
@@ -3888,7 +3876,7 @@
     </row>
     <row r="73" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B73">
         <v>2600</v>
@@ -3971,7 +3959,7 @@
     </row>
     <row r="74" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B74">
         <v>40</v>
@@ -4015,7 +4003,7 @@
     </row>
     <row r="75" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J75">
         <v>150</v>
@@ -4047,7 +4035,7 @@
     </row>
     <row r="76" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J76">
         <v>1</v>
@@ -4055,7 +4043,7 @@
     </row>
     <row r="77" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="R77">
         <v>35</v>
@@ -4096,7 +4084,7 @@
     </row>
     <row r="78" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="R78">
         <v>44</v>
@@ -4137,7 +4125,7 @@
     </row>
     <row r="79" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S79">
         <v>1.5</v>
@@ -4172,7 +4160,7 @@
     </row>
     <row r="80" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="R80">
         <v>2</v>
@@ -4201,7 +4189,7 @@
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="V81">
         <v>5</v>
@@ -4212,135 +4200,135 @@
     </row>
     <row r="82" spans="1:30" x14ac:dyDescent="0.25">
       <c r="Z82" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AA82" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AB82" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AC82" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B87" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C87" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D87" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E87" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F87" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G87" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H87" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I87" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="J87" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K87" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="L87" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B88" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C88" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D88" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E88" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F88" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G88" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H88" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I88" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="J88" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K88" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L88" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>217</v>
+      </c>
+      <c r="B89" t="s">
         <v>216</v>
       </c>
-      <c r="B89" t="s">
-        <v>215</v>
-      </c>
       <c r="C89" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D89" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E89" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F89" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G89" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H89" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I89" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="J89" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="K89" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L89" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B90">
         <v>500</v>
@@ -4369,7 +4357,7 @@
     </row>
     <row r="92" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B92">
         <v>2880</v>
@@ -4398,7 +4386,7 @@
     </row>
     <row r="93" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B93">
         <v>360</v>
@@ -4427,7 +4415,7 @@
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B94">
         <v>1440</v>
@@ -4456,7 +4444,7 @@
     </row>
     <row r="96" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B96">
         <v>6</v>
@@ -4485,45 +4473,45 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
+        <v>237</v>
+      </c>
+      <c r="E97" t="s">
         <v>236</v>
       </c>
-      <c r="E97" t="s">
+      <c r="F97" t="s">
         <v>235</v>
       </c>
-      <c r="F97" t="s">
-        <v>234</v>
-      </c>
       <c r="G97" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H97" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I97" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J97" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="K97" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L97" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="M97" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="N97" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="O97" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B98">
         <v>25</v>
@@ -4570,7 +4558,7 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -4614,7 +4602,7 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B100">
         <v>2</v>
@@ -4661,7 +4649,7 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B101">
         <v>32</v>
@@ -4708,7 +4696,7 @@
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B102">
         <v>0.83299999999999996</v>
@@ -4755,7 +4743,7 @@
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B103">
         <v>41.6</v>
@@ -4764,7 +4752,7 @@
         <v>60</v>
       </c>
       <c r="D103" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E103">
         <v>50</v>
@@ -4802,16 +4790,16 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D105" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="J105" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="L105" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -4821,82 +4809,82 @@
     <mergeCell ref="J6:M6"/>
   </mergeCells>
   <conditionalFormatting sqref="G9:M33">
-    <cfRule type="expression" dxfId="25" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="71" stopIfTrue="1">
       <formula>G9&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="72" stopIfTrue="1">
       <formula>MOD(G9,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F3">
-    <cfRule type="expression" dxfId="23" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="61" stopIfTrue="1">
       <formula>B2&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="62" stopIfTrue="1">
       <formula>MOD(B2,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:F12">
-    <cfRule type="expression" dxfId="21" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="31" stopIfTrue="1">
       <formula>B12&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
       <formula>MOD(B12,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:F33">
-    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="37" stopIfTrue="1">
       <formula>B25&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="38" stopIfTrue="1">
       <formula>MOD(B25,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:F21">
-    <cfRule type="expression" dxfId="17" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="35" stopIfTrue="1">
       <formula>B20&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="36" stopIfTrue="1">
       <formula>MOD(B20,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:F22">
-    <cfRule type="expression" dxfId="15" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="33" stopIfTrue="1">
       <formula>B22&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="34" stopIfTrue="1">
       <formula>MOD(B22,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:F23">
-    <cfRule type="expression" dxfId="13" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="29" stopIfTrue="1">
       <formula>B23&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="30" stopIfTrue="1">
       <formula>MOD(B23,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:F33">
-    <cfRule type="expression" dxfId="11" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="39" stopIfTrue="1">
       <formula>B9&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="40" stopIfTrue="1">
       <formula>MOD(B9,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:F15">
-    <cfRule type="expression" dxfId="9" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="27" stopIfTrue="1">
       <formula>E15&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="28" stopIfTrue="1">
       <formula>MOD(E15,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:F16">
-    <cfRule type="expression" dxfId="7" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="25" stopIfTrue="1">
       <formula>E16&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="26" stopIfTrue="1">
       <formula>MOD(E16,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
firing randomnes and remove ussles script
rotation speed 1 mean thats lot of randomnes, 5 was first try and it was
maddnes :D

Also i remove code that turn bombard off when shooting into air, this is
not necesary while bombardment its only for artilery weapon.

But we probably need back that uggly toggle, while be able tunr artilery
off only by air fly abou is very cancerous.
</commit_message>
<xml_diff>
--- a/Units.xlsx
+++ b/Units.xlsx
@@ -1086,85 +1086,7 @@
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1555,10 +1477,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A73" sqref="A73"/>
-      <selection pane="topRight" activeCell="F24" sqref="F24"/>
+      <selection pane="topRight" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,7 +2369,7 @@
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
@@ -2464,12 +2386,12 @@
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>15</v>
       </c>
@@ -2484,7 +2406,7 @@
       </c>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>19</v>
       </c>
@@ -2499,7 +2421,7 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>60</v>
       </c>
@@ -2543,7 +2465,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>82</v>
       </c>
@@ -2556,53 +2478,54 @@
       <c r="D39" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="22" t="s">
+      <c r="E39" s="21"/>
+      <c r="F39" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="G39" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="G39" s="22" t="s">
+      <c r="H39" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="H39" s="22" t="s">
+      <c r="I39" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="I39" s="27" t="s">
+      <c r="J39" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="J39" s="27" t="s">
+      <c r="K39" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="K39" s="27" t="s">
+      <c r="L39" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="L39" s="27" t="s">
+      <c r="M39" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="M39" s="22" t="s">
+      <c r="N39" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="N39" s="22" t="s">
+      <c r="O39" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="O39" s="22" t="s">
+      <c r="P39" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="P39" s="22" t="s">
+      <c r="Q39" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="Q39" s="22" t="s">
+      <c r="R39" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="R39" s="22" t="s">
+      <c r="S39" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="S39" s="22" t="s">
+      <c r="T39" s="22" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>61</v>
       </c>
@@ -2613,44 +2536,45 @@
       <c r="D40" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="24"/>
+      <c r="F40" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F40" s="24" t="s">
+      <c r="G40" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="G40" s="24"/>
       <c r="H40" s="24"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25" t="s">
+      <c r="I40" s="24"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="K40" s="25" t="s">
+      <c r="L40" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="L40" s="25" t="s">
+      <c r="M40" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="M40" s="28" t="s">
+      <c r="N40" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="N40" s="28" t="s">
+      <c r="O40" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="P40" s="28" t="s">
+      <c r="Q40" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="Q40" s="28" t="s">
+      <c r="R40" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="R40" s="28" t="s">
+      <c r="S40" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="S40" s="28" t="s">
+      <c r="T40" s="28" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>62</v>
       </c>
@@ -2661,45 +2585,46 @@
         <v>35</v>
       </c>
       <c r="D41" s="16"/>
-      <c r="E41" s="16">
+      <c r="E41" s="16"/>
+      <c r="F41" s="16">
         <v>54</v>
       </c>
-      <c r="F41" s="17">
+      <c r="G41" s="17">
         <v>66</v>
       </c>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17">
+      <c r="H41" s="17"/>
+      <c r="I41" s="17">
         <v>130</v>
       </c>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18">
+      <c r="J41" s="18"/>
+      <c r="K41" s="18">
         <v>100</v>
       </c>
-      <c r="K41" s="18">
+      <c r="L41" s="18">
         <v>220</v>
       </c>
-      <c r="L41" s="19"/>
-      <c r="M41" s="23">
+      <c r="M41" s="19"/>
+      <c r="N41" s="23">
         <v>197</v>
       </c>
-      <c r="N41" s="23">
+      <c r="O41" s="23">
         <v>12500</v>
       </c>
-      <c r="O41" s="29"/>
-      <c r="P41" s="23">
+      <c r="P41" s="29"/>
+      <c r="Q41" s="23">
         <v>640</v>
       </c>
-      <c r="Q41" s="23">
+      <c r="R41" s="23">
         <v>360</v>
       </c>
-      <c r="R41" s="23">
+      <c r="S41" s="23">
         <v>960</v>
       </c>
-      <c r="S41" s="23">
+      <c r="T41" s="23">
         <v>480</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>63</v>
       </c>
@@ -2710,45 +2635,46 @@
         <v>140</v>
       </c>
       <c r="D42" s="16"/>
-      <c r="E42" s="17">
+      <c r="E42" s="16"/>
+      <c r="F42" s="17">
         <v>270</v>
       </c>
-      <c r="F42" s="17">
+      <c r="G42" s="17">
         <v>330</v>
       </c>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17">
+      <c r="H42" s="17"/>
+      <c r="I42" s="17">
         <v>650</v>
       </c>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18">
+      <c r="J42" s="18"/>
+      <c r="K42" s="18">
         <v>750</v>
       </c>
-      <c r="K42" s="18">
+      <c r="L42" s="18">
         <v>1650</v>
       </c>
-      <c r="L42" s="20"/>
-      <c r="M42" s="23">
+      <c r="M42" s="20"/>
+      <c r="N42" s="23">
         <v>990</v>
       </c>
-      <c r="N42" s="23">
+      <c r="O42" s="23">
         <v>240000</v>
       </c>
-      <c r="O42" s="29"/>
-      <c r="P42" s="23">
+      <c r="P42" s="29"/>
+      <c r="Q42" s="23">
         <v>8000</v>
       </c>
-      <c r="Q42" s="23">
+      <c r="R42" s="23">
         <v>1800</v>
       </c>
-      <c r="R42" s="23">
+      <c r="S42" s="23">
         <v>9600</v>
       </c>
-      <c r="S42" s="23">
+      <c r="T42" s="23">
         <v>5400</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>64</v>
       </c>
@@ -2759,45 +2685,46 @@
         <v>120</v>
       </c>
       <c r="D43" s="16"/>
-      <c r="E43" s="16">
+      <c r="E43" s="16"/>
+      <c r="F43" s="16">
         <v>270</v>
       </c>
-      <c r="F43" s="17">
+      <c r="G43" s="17">
         <v>330</v>
       </c>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17">
+      <c r="H43" s="17"/>
+      <c r="I43" s="17">
         <v>650</v>
       </c>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18">
+      <c r="J43" s="18"/>
+      <c r="K43" s="18">
         <v>500</v>
       </c>
-      <c r="K43" s="18">
+      <c r="L43" s="18">
         <v>1100</v>
       </c>
-      <c r="L43" s="19"/>
-      <c r="M43" s="23">
+      <c r="M43" s="19"/>
+      <c r="N43" s="23">
         <v>880</v>
       </c>
-      <c r="N43" s="23">
+      <c r="O43" s="23">
         <v>12000</v>
       </c>
-      <c r="O43" s="29"/>
-      <c r="P43" s="23">
+      <c r="P43" s="29"/>
+      <c r="Q43" s="23">
         <v>640</v>
       </c>
-      <c r="Q43" s="23">
+      <c r="R43" s="23">
         <v>1600</v>
       </c>
-      <c r="R43" s="23">
+      <c r="S43" s="23">
         <v>5000</v>
       </c>
-      <c r="S43" s="23">
+      <c r="T43" s="23">
         <v>2400</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>65</v>
       </c>
@@ -2806,54 +2733,55 @@
         <v>4</v>
       </c>
       <c r="C44" s="16">
-        <f t="shared" ref="C44:L44" si="9">C43/$B$36</f>
+        <f t="shared" ref="C44:M44" si="9">C43/$B$36</f>
         <v>6</v>
       </c>
       <c r="D44" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="E44" s="16">
+      <c r="E44" s="16"/>
+      <c r="F44" s="16">
         <f t="shared" si="9"/>
         <v>13.5</v>
       </c>
-      <c r="F44" s="16">
-        <f t="shared" ref="F44" si="10">F43/$B$36</f>
+      <c r="G44" s="16">
+        <f t="shared" ref="G44" si="10">G43/$B$36</f>
         <v>16.5</v>
       </c>
-      <c r="G44" s="16">
-        <f t="shared" ref="G44" si="11">G43/$B$36</f>
+      <c r="H44" s="16">
+        <f t="shared" ref="H44" si="11">H43/$B$36</f>
         <v>0</v>
       </c>
-      <c r="H44" s="16">
-        <f>H43/$B$36</f>
+      <c r="I44" s="16">
+        <f>I43/$B$36</f>
         <v>32.5</v>
       </c>
-      <c r="I44" s="16">
-        <f t="shared" ref="I44" si="12">I43/$B$36</f>
+      <c r="J44" s="16">
+        <f t="shared" ref="J44" si="12">J43/$B$36</f>
         <v>0</v>
       </c>
-      <c r="J44" s="16">
-        <f>J43/$C$36</f>
+      <c r="K44" s="16">
+        <f>K43/$C$36</f>
         <v>12.5</v>
       </c>
-      <c r="K44" s="16">
+      <c r="L44" s="16">
         <f t="shared" si="9"/>
         <v>55</v>
       </c>
-      <c r="L44" s="16">
+      <c r="M44" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="M44" s="29"/>
       <c r="N44" s="29"/>
       <c r="O44" s="29"/>
       <c r="P44" s="29"/>
       <c r="Q44" s="29"/>
       <c r="R44" s="29"/>
       <c r="S44" s="29"/>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T44" s="29"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>66</v>
       </c>
@@ -2862,54 +2790,55 @@
         <v>3</v>
       </c>
       <c r="C45" s="16">
-        <f t="shared" ref="C45:L45" si="13">C41/$B$44</f>
+        <f t="shared" ref="C45:M45" si="13">C41/$B$44</f>
         <v>8.75</v>
       </c>
       <c r="D45" s="16">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="E45" s="16">
-        <f>E41/$E$44</f>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16">
+        <f>F41/$F$44</f>
         <v>4</v>
       </c>
-      <c r="F45" s="16">
-        <f t="shared" ref="F45:I45" si="14">F41/$E$44</f>
+      <c r="G45" s="16">
+        <f t="shared" ref="G45:J45" si="14">G41/$F$44</f>
         <v>4.8888888888888893</v>
       </c>
-      <c r="G45" s="16">
+      <c r="H45" s="16">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="H45" s="16">
+      <c r="I45" s="16">
         <f t="shared" si="14"/>
         <v>9.6296296296296298</v>
       </c>
-      <c r="I45" s="16">
+      <c r="J45" s="16">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="J45" s="16">
-        <f>J41/$J$44</f>
+      <c r="K45" s="16">
+        <f>K41/$K$44</f>
         <v>8</v>
       </c>
-      <c r="K45" s="16">
+      <c r="L45" s="16">
         <f t="shared" si="13"/>
         <v>55</v>
       </c>
-      <c r="L45" s="16">
+      <c r="M45" s="16">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="M45" s="29"/>
       <c r="N45" s="29"/>
       <c r="O45" s="29"/>
       <c r="P45" s="29"/>
       <c r="Q45" s="29"/>
       <c r="R45" s="29"/>
       <c r="S45" s="29"/>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T45" s="29"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>67</v>
       </c>
@@ -2918,77 +2847,79 @@
         <v>10</v>
       </c>
       <c r="C46" s="16">
-        <f t="shared" ref="C46:L46" si="15">C42/$B$44</f>
+        <f t="shared" ref="C46:M46" si="15">C42/$B$44</f>
         <v>35</v>
       </c>
       <c r="D46" s="16">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="E46" s="16">
-        <f>E42/$E$44</f>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16">
+        <f>F42/$F$44</f>
         <v>20</v>
       </c>
-      <c r="F46" s="16">
-        <f t="shared" ref="F46:I46" si="16">F42/$E$44</f>
+      <c r="G46" s="16">
+        <f t="shared" ref="G46:J46" si="16">G42/$F$44</f>
         <v>24.444444444444443</v>
       </c>
-      <c r="G46" s="16">
+      <c r="H46" s="16">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="H46" s="16">
+      <c r="I46" s="16">
         <f t="shared" si="16"/>
         <v>48.148148148148145</v>
       </c>
-      <c r="I46" s="16">
+      <c r="J46" s="16">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J46" s="16">
-        <f>J42/$J$44</f>
+      <c r="K46" s="16">
+        <f>K42/$K$44</f>
         <v>60</v>
       </c>
-      <c r="K46" s="16">
+      <c r="L46" s="16">
         <f t="shared" si="15"/>
         <v>412.5</v>
       </c>
-      <c r="L46" s="16">
+      <c r="M46" s="16">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="M46" s="29"/>
       <c r="N46" s="29"/>
       <c r="O46" s="29"/>
       <c r="P46" s="29"/>
       <c r="Q46" s="29"/>
       <c r="R46" s="29"/>
       <c r="S46" s="29"/>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T46" s="29"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
-      <c r="E47" s="17"/>
+      <c r="E47" s="16"/>
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
+      <c r="I47" s="17"/>
       <c r="J47" s="18"/>
       <c r="K47" s="18"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="29"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="20"/>
       <c r="N47" s="29"/>
       <c r="O47" s="29"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="29"/>
       <c r="R47" s="29"/>
       <c r="S47" s="29"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T47" s="29"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>7</v>
       </c>
@@ -3001,49 +2932,50 @@
       <c r="D48" s="16">
         <v>280</v>
       </c>
-      <c r="E48" s="16">
+      <c r="E48" s="16"/>
+      <c r="F48" s="16">
         <v>265</v>
       </c>
-      <c r="F48" s="17">
+      <c r="G48" s="17">
         <v>150</v>
       </c>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17">
+      <c r="H48" s="17"/>
+      <c r="I48" s="17">
         <v>375</v>
       </c>
-      <c r="I48" s="18">
+      <c r="J48" s="18">
         <v>640</v>
       </c>
-      <c r="J48" s="18">
+      <c r="K48" s="18">
         <v>400</v>
       </c>
-      <c r="K48" s="18">
+      <c r="L48" s="18">
         <v>600</v>
       </c>
-      <c r="L48" s="19">
+      <c r="M48" s="19">
         <v>900</v>
       </c>
-      <c r="M48" s="23">
+      <c r="N48" s="23">
         <v>1200</v>
       </c>
-      <c r="N48" s="23">
+      <c r="O48" s="23">
         <v>30000</v>
       </c>
-      <c r="O48" s="29"/>
-      <c r="P48" s="23">
+      <c r="P48" s="29"/>
+      <c r="Q48" s="23">
         <v>3500</v>
       </c>
-      <c r="Q48" s="23">
+      <c r="R48" s="23">
         <v>2750</v>
       </c>
-      <c r="R48" s="23">
+      <c r="S48" s="23">
         <v>1600</v>
       </c>
-      <c r="S48" s="23">
+      <c r="T48" s="23">
         <v>4200</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>9</v>
       </c>
@@ -3051,42 +2983,45 @@
         <v>5</v>
       </c>
       <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="17">
+      <c r="D49" s="16">
+        <v>3</v>
+      </c>
+      <c r="E49" s="16"/>
+      <c r="F49" s="17">
         <v>3.6</v>
       </c>
-      <c r="F49" s="17">
+      <c r="G49" s="17">
         <v>2.6</v>
       </c>
-      <c r="G49" s="17"/>
       <c r="H49" s="17"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18">
+      <c r="I49" s="17"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18">
         <v>4.5</v>
       </c>
-      <c r="K49" s="18">
+      <c r="L49" s="18">
         <v>2.6</v>
       </c>
-      <c r="L49" s="20"/>
-      <c r="M49" s="29">
+      <c r="M49" s="20"/>
+      <c r="N49" s="29">
         <v>3.2</v>
       </c>
-      <c r="N49" s="23">
+      <c r="O49" s="23">
         <v>2.7</v>
       </c>
-      <c r="O49" s="29"/>
-      <c r="P49" s="23">
+      <c r="P49" s="29"/>
+      <c r="Q49" s="23">
         <v>3.75</v>
       </c>
-      <c r="Q49" s="29"/>
-      <c r="R49" s="23">
+      <c r="R49" s="29"/>
+      <c r="S49" s="23">
         <v>2.2999999999999998</v>
       </c>
-      <c r="S49" s="29">
+      <c r="T49" s="29">
         <v>3.6</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>69</v>
       </c>
@@ -3095,39 +3030,42 @@
         <v>20</v>
       </c>
       <c r="D50" s="16">
+        <v>30</v>
+      </c>
+      <c r="E50" s="16">
+        <v>30</v>
+      </c>
+      <c r="F50" s="16">
+        <v>25</v>
+      </c>
+      <c r="G50" s="17">
+        <v>33</v>
+      </c>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18">
         <v>35</v>
       </c>
-      <c r="E50" s="16">
-        <v>25</v>
-      </c>
-      <c r="F50" s="17">
-        <v>33</v>
-      </c>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18">
-        <v>35</v>
-      </c>
-      <c r="K50" s="18"/>
-      <c r="L50" s="19"/>
-      <c r="M50" s="29">
+      <c r="L50" s="18"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="29">
         <v>75</v>
       </c>
-      <c r="N50" s="29">
+      <c r="O50" s="29">
         <v>1380</v>
       </c>
-      <c r="O50" s="29"/>
       <c r="P50" s="29"/>
       <c r="Q50" s="29"/>
-      <c r="R50" s="29">
+      <c r="R50" s="29"/>
+      <c r="S50" s="29">
         <v>600</v>
       </c>
-      <c r="S50" s="29">
+      <c r="T50" s="29">
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>70</v>
       </c>
@@ -3138,19 +3076,20 @@
       <c r="F51" s="16"/>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
-      <c r="I51" s="18"/>
+      <c r="I51" s="16"/>
       <c r="J51" s="18"/>
       <c r="K51" s="18"/>
-      <c r="L51" s="19"/>
-      <c r="M51" s="29"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="19"/>
       <c r="N51" s="29"/>
       <c r="O51" s="29"/>
       <c r="P51" s="29"/>
       <c r="Q51" s="29"/>
       <c r="R51" s="29"/>
       <c r="S51" s="29"/>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T51" s="29"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>71</v>
       </c>
@@ -3161,44 +3100,46 @@
       <c r="F52" s="16"/>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
-      <c r="I52" s="18"/>
+      <c r="I52" s="16"/>
       <c r="J52" s="18"/>
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
-      <c r="M52" s="29"/>
+      <c r="M52" s="18"/>
       <c r="N52" s="29"/>
       <c r="O52" s="29"/>
       <c r="P52" s="29"/>
       <c r="Q52" s="29"/>
       <c r="R52" s="29"/>
       <c r="S52" s="29"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T52" s="29"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>72</v>
       </c>
       <c r="B53" s="16"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17">
+      <c r="E53" s="16"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17">
         <v>9</v>
       </c>
-      <c r="G53" s="17"/>
       <c r="H53" s="17"/>
-      <c r="I53" s="18"/>
+      <c r="I53" s="17"/>
       <c r="J53" s="18"/>
       <c r="K53" s="18"/>
-      <c r="L53" s="20"/>
-      <c r="M53" s="29"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="20"/>
       <c r="N53" s="29"/>
       <c r="O53" s="29"/>
       <c r="P53" s="29"/>
       <c r="Q53" s="29"/>
       <c r="R53" s="29"/>
       <c r="S53" s="29"/>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T53" s="29"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>73</v>
       </c>
@@ -3206,26 +3147,27 @@
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
-      <c r="F54" s="16">
+      <c r="F54" s="16"/>
+      <c r="G54" s="16">
         <v>1.5</v>
       </c>
-      <c r="G54" s="16"/>
       <c r="H54" s="16"/>
-      <c r="I54" s="18"/>
+      <c r="I54" s="16"/>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
-      <c r="M54" s="29"/>
+      <c r="M54" s="18"/>
       <c r="N54" s="29"/>
       <c r="O54" s="29"/>
       <c r="P54" s="29"/>
       <c r="Q54" s="29"/>
-      <c r="R54" s="29">
+      <c r="R54" s="29"/>
+      <c r="S54" s="29">
         <v>5</v>
       </c>
-      <c r="S54" s="29"/>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T54" s="29"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>74</v>
       </c>
@@ -3233,24 +3175,25 @@
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
-      <c r="F55" s="16">
+      <c r="F55" s="16"/>
+      <c r="G55" s="16">
         <v>5</v>
       </c>
-      <c r="G55" s="16"/>
       <c r="H55" s="16"/>
-      <c r="I55" s="18"/>
+      <c r="I55" s="16"/>
       <c r="J55" s="18"/>
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
-      <c r="M55" s="29"/>
+      <c r="M55" s="18"/>
       <c r="N55" s="29"/>
       <c r="O55" s="29"/>
       <c r="P55" s="29"/>
       <c r="Q55" s="29"/>
       <c r="R55" s="29"/>
       <c r="S55" s="29"/>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T55" s="29"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>75</v>
       </c>
@@ -3261,19 +3204,20 @@
       <c r="F56" s="16"/>
       <c r="G56" s="16"/>
       <c r="H56" s="16"/>
-      <c r="I56" s="18"/>
+      <c r="I56" s="16"/>
       <c r="J56" s="18"/>
       <c r="K56" s="18"/>
-      <c r="L56" s="19"/>
-      <c r="M56" s="29"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="19"/>
       <c r="N56" s="29"/>
       <c r="O56" s="29"/>
       <c r="P56" s="29"/>
       <c r="Q56" s="29"/>
       <c r="R56" s="29"/>
       <c r="S56" s="29"/>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T56" s="29"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>76</v>
       </c>
@@ -3282,37 +3226,38 @@
         <v>14</v>
       </c>
       <c r="D57" s="16"/>
-      <c r="E57" s="17">
+      <c r="E57" s="16"/>
+      <c r="F57" s="17">
         <v>18</v>
       </c>
-      <c r="F57" s="17">
+      <c r="G57" s="17">
         <v>28</v>
       </c>
-      <c r="G57" s="17"/>
       <c r="H57" s="17"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18">
+      <c r="I57" s="17"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18">
         <v>23</v>
       </c>
-      <c r="K57" s="18"/>
-      <c r="L57" s="20"/>
-      <c r="M57" s="29">
+      <c r="L57" s="18"/>
+      <c r="M57" s="20"/>
+      <c r="N57" s="29">
         <v>20</v>
       </c>
-      <c r="N57" s="23">
+      <c r="O57" s="23">
         <v>35</v>
       </c>
-      <c r="O57" s="29"/>
       <c r="P57" s="29"/>
-      <c r="Q57" s="29">
+      <c r="Q57" s="29"/>
+      <c r="R57" s="29">
         <v>35</v>
       </c>
-      <c r="R57" s="29"/>
-      <c r="S57" s="29">
+      <c r="S57" s="29"/>
+      <c r="T57" s="29">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>91</v>
       </c>
@@ -3321,31 +3266,32 @@
       </c>
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
-      <c r="E58" s="17">
-        <v>20</v>
-      </c>
+      <c r="E58" s="16"/>
       <c r="F58" s="17">
         <v>20</v>
       </c>
-      <c r="G58" s="17"/>
+      <c r="G58" s="17">
+        <v>20</v>
+      </c>
       <c r="H58" s="17"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="18">
+      <c r="I58" s="17"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18">
         <v>15</v>
       </c>
-      <c r="K58" s="18">
+      <c r="L58" s="18">
         <v>18</v>
       </c>
-      <c r="L58" s="23"/>
-      <c r="M58" s="29"/>
+      <c r="M58" s="23"/>
       <c r="N58" s="29"/>
       <c r="O58" s="29"/>
       <c r="P58" s="29"/>
       <c r="Q58" s="29"/>
       <c r="R58" s="29"/>
       <c r="S58" s="29"/>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T58" s="29"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>77</v>
       </c>
@@ -3356,30 +3302,31 @@
         <v>81</v>
       </c>
       <c r="D59" s="14"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15" t="s">
+      <c r="E59" s="14"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="G59" s="15"/>
       <c r="H59" s="15"/>
       <c r="I59" s="15"/>
       <c r="J59" s="15"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
-      <c r="M59" t="s">
+      <c r="M59" s="15"/>
+      <c r="N59" t="s">
         <v>113</v>
       </c>
-      <c r="N59" t="s">
+      <c r="O59" t="s">
         <v>114</v>
       </c>
-      <c r="P59" t="s">
+      <c r="Q59" t="s">
         <v>120</v>
       </c>
-      <c r="R59" t="s">
+      <c r="S59" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>78</v>
       </c>
@@ -3395,7 +3342,7 @@
       <c r="K60" s="15"/>
       <c r="L60" s="15"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>79</v>
       </c>
@@ -4809,82 +4756,82 @@
     <mergeCell ref="J6:M6"/>
   </mergeCells>
   <conditionalFormatting sqref="G9:M33">
-    <cfRule type="expression" dxfId="51" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="71" stopIfTrue="1">
       <formula>G9&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="72" stopIfTrue="1">
       <formula>MOD(G9,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F3">
-    <cfRule type="expression" dxfId="39" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="61" stopIfTrue="1">
       <formula>B2&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="62" stopIfTrue="1">
       <formula>MOD(B2,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:F12">
-    <cfRule type="expression" dxfId="31" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="31" stopIfTrue="1">
       <formula>B12&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="32" stopIfTrue="1">
       <formula>MOD(B12,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:F33">
-    <cfRule type="expression" dxfId="21" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
       <formula>B25&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
       <formula>MOD(B25,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:F21">
-    <cfRule type="expression" dxfId="19" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="35" stopIfTrue="1">
       <formula>B20&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="36" stopIfTrue="1">
       <formula>MOD(B20,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:F22">
-    <cfRule type="expression" dxfId="17" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="33" stopIfTrue="1">
       <formula>B22&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="34" stopIfTrue="1">
       <formula>MOD(B22,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:F23">
-    <cfRule type="expression" dxfId="15" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="29" stopIfTrue="1">
       <formula>B23&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="30" stopIfTrue="1">
       <formula>MOD(B23,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:F33">
-    <cfRule type="expression" dxfId="13" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="39" stopIfTrue="1">
       <formula>B9&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="40" stopIfTrue="1">
       <formula>MOD(B9,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:F15">
-    <cfRule type="expression" dxfId="11" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="27" stopIfTrue="1">
       <formula>E15&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="28" stopIfTrue="1">
       <formula>MOD(E15,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:F16">
-    <cfRule type="expression" dxfId="9" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="25" stopIfTrue="1">
       <formula>E16&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="26" stopIfTrue="1">
       <formula>MOD(E16,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix t1 arty bombardment mode and target painter (#129)
merged before ithilis can break it again.
</commit_message>
<xml_diff>
--- a/Units.xlsx
+++ b/Units.xlsx
@@ -1086,85 +1086,7 @@
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1555,10 +1477,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A73" sqref="A73"/>
-      <selection pane="topRight" activeCell="F24" sqref="F24"/>
+      <selection pane="topRight" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,7 +2369,7 @@
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
@@ -2464,12 +2386,12 @@
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>15</v>
       </c>
@@ -2484,7 +2406,7 @@
       </c>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>19</v>
       </c>
@@ -2499,7 +2421,7 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>60</v>
       </c>
@@ -2543,7 +2465,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>82</v>
       </c>
@@ -2556,53 +2478,54 @@
       <c r="D39" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="22" t="s">
+      <c r="E39" s="21"/>
+      <c r="F39" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="G39" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="G39" s="22" t="s">
+      <c r="H39" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="H39" s="22" t="s">
+      <c r="I39" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="I39" s="27" t="s">
+      <c r="J39" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="J39" s="27" t="s">
+      <c r="K39" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="K39" s="27" t="s">
+      <c r="L39" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="L39" s="27" t="s">
+      <c r="M39" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="M39" s="22" t="s">
+      <c r="N39" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="N39" s="22" t="s">
+      <c r="O39" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="O39" s="22" t="s">
+      <c r="P39" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="P39" s="22" t="s">
+      <c r="Q39" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="Q39" s="22" t="s">
+      <c r="R39" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="R39" s="22" t="s">
+      <c r="S39" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="S39" s="22" t="s">
+      <c r="T39" s="22" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>61</v>
       </c>
@@ -2613,44 +2536,45 @@
       <c r="D40" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="24"/>
+      <c r="F40" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F40" s="24" t="s">
+      <c r="G40" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="G40" s="24"/>
       <c r="H40" s="24"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25" t="s">
+      <c r="I40" s="24"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="K40" s="25" t="s">
+      <c r="L40" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="L40" s="25" t="s">
+      <c r="M40" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="M40" s="28" t="s">
+      <c r="N40" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="N40" s="28" t="s">
+      <c r="O40" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="P40" s="28" t="s">
+      <c r="Q40" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="Q40" s="28" t="s">
+      <c r="R40" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="R40" s="28" t="s">
+      <c r="S40" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="S40" s="28" t="s">
+      <c r="T40" s="28" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>62</v>
       </c>
@@ -2661,45 +2585,46 @@
         <v>35</v>
       </c>
       <c r="D41" s="16"/>
-      <c r="E41" s="16">
+      <c r="E41" s="16"/>
+      <c r="F41" s="16">
         <v>54</v>
       </c>
-      <c r="F41" s="17">
+      <c r="G41" s="17">
         <v>66</v>
       </c>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17">
+      <c r="H41" s="17"/>
+      <c r="I41" s="17">
         <v>130</v>
       </c>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18">
+      <c r="J41" s="18"/>
+      <c r="K41" s="18">
         <v>100</v>
       </c>
-      <c r="K41" s="18">
+      <c r="L41" s="18">
         <v>220</v>
       </c>
-      <c r="L41" s="19"/>
-      <c r="M41" s="23">
+      <c r="M41" s="19"/>
+      <c r="N41" s="23">
         <v>197</v>
       </c>
-      <c r="N41" s="23">
+      <c r="O41" s="23">
         <v>12500</v>
       </c>
-      <c r="O41" s="29"/>
-      <c r="P41" s="23">
+      <c r="P41" s="29"/>
+      <c r="Q41" s="23">
         <v>640</v>
       </c>
-      <c r="Q41" s="23">
+      <c r="R41" s="23">
         <v>360</v>
       </c>
-      <c r="R41" s="23">
+      <c r="S41" s="23">
         <v>960</v>
       </c>
-      <c r="S41" s="23">
+      <c r="T41" s="23">
         <v>480</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>63</v>
       </c>
@@ -2710,45 +2635,46 @@
         <v>140</v>
       </c>
       <c r="D42" s="16"/>
-      <c r="E42" s="17">
+      <c r="E42" s="16"/>
+      <c r="F42" s="17">
         <v>270</v>
       </c>
-      <c r="F42" s="17">
+      <c r="G42" s="17">
         <v>330</v>
       </c>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17">
+      <c r="H42" s="17"/>
+      <c r="I42" s="17">
         <v>650</v>
       </c>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18">
+      <c r="J42" s="18"/>
+      <c r="K42" s="18">
         <v>750</v>
       </c>
-      <c r="K42" s="18">
+      <c r="L42" s="18">
         <v>1650</v>
       </c>
-      <c r="L42" s="20"/>
-      <c r="M42" s="23">
+      <c r="M42" s="20"/>
+      <c r="N42" s="23">
         <v>990</v>
       </c>
-      <c r="N42" s="23">
+      <c r="O42" s="23">
         <v>240000</v>
       </c>
-      <c r="O42" s="29"/>
-      <c r="P42" s="23">
+      <c r="P42" s="29"/>
+      <c r="Q42" s="23">
         <v>8000</v>
       </c>
-      <c r="Q42" s="23">
+      <c r="R42" s="23">
         <v>1800</v>
       </c>
-      <c r="R42" s="23">
+      <c r="S42" s="23">
         <v>9600</v>
       </c>
-      <c r="S42" s="23">
+      <c r="T42" s="23">
         <v>5400</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>64</v>
       </c>
@@ -2759,45 +2685,46 @@
         <v>120</v>
       </c>
       <c r="D43" s="16"/>
-      <c r="E43" s="16">
+      <c r="E43" s="16"/>
+      <c r="F43" s="16">
         <v>270</v>
       </c>
-      <c r="F43" s="17">
+      <c r="G43" s="17">
         <v>330</v>
       </c>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17">
+      <c r="H43" s="17"/>
+      <c r="I43" s="17">
         <v>650</v>
       </c>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18">
+      <c r="J43" s="18"/>
+      <c r="K43" s="18">
         <v>500</v>
       </c>
-      <c r="K43" s="18">
+      <c r="L43" s="18">
         <v>1100</v>
       </c>
-      <c r="L43" s="19"/>
-      <c r="M43" s="23">
+      <c r="M43" s="19"/>
+      <c r="N43" s="23">
         <v>880</v>
       </c>
-      <c r="N43" s="23">
+      <c r="O43" s="23">
         <v>12000</v>
       </c>
-      <c r="O43" s="29"/>
-      <c r="P43" s="23">
+      <c r="P43" s="29"/>
+      <c r="Q43" s="23">
         <v>640</v>
       </c>
-      <c r="Q43" s="23">
+      <c r="R43" s="23">
         <v>1600</v>
       </c>
-      <c r="R43" s="23">
+      <c r="S43" s="23">
         <v>5000</v>
       </c>
-      <c r="S43" s="23">
+      <c r="T43" s="23">
         <v>2400</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>65</v>
       </c>
@@ -2806,54 +2733,55 @@
         <v>4</v>
       </c>
       <c r="C44" s="16">
-        <f t="shared" ref="C44:L44" si="9">C43/$B$36</f>
+        <f t="shared" ref="C44:M44" si="9">C43/$B$36</f>
         <v>6</v>
       </c>
       <c r="D44" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="E44" s="16">
+      <c r="E44" s="16"/>
+      <c r="F44" s="16">
         <f t="shared" si="9"/>
         <v>13.5</v>
       </c>
-      <c r="F44" s="16">
-        <f t="shared" ref="F44" si="10">F43/$B$36</f>
+      <c r="G44" s="16">
+        <f t="shared" ref="G44" si="10">G43/$B$36</f>
         <v>16.5</v>
       </c>
-      <c r="G44" s="16">
-        <f t="shared" ref="G44" si="11">G43/$B$36</f>
+      <c r="H44" s="16">
+        <f t="shared" ref="H44" si="11">H43/$B$36</f>
         <v>0</v>
       </c>
-      <c r="H44" s="16">
-        <f>H43/$B$36</f>
+      <c r="I44" s="16">
+        <f>I43/$B$36</f>
         <v>32.5</v>
       </c>
-      <c r="I44" s="16">
-        <f t="shared" ref="I44" si="12">I43/$B$36</f>
+      <c r="J44" s="16">
+        <f t="shared" ref="J44" si="12">J43/$B$36</f>
         <v>0</v>
       </c>
-      <c r="J44" s="16">
-        <f>J43/$C$36</f>
+      <c r="K44" s="16">
+        <f>K43/$C$36</f>
         <v>12.5</v>
       </c>
-      <c r="K44" s="16">
+      <c r="L44" s="16">
         <f t="shared" si="9"/>
         <v>55</v>
       </c>
-      <c r="L44" s="16">
+      <c r="M44" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="M44" s="29"/>
       <c r="N44" s="29"/>
       <c r="O44" s="29"/>
       <c r="P44" s="29"/>
       <c r="Q44" s="29"/>
       <c r="R44" s="29"/>
       <c r="S44" s="29"/>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T44" s="29"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>66</v>
       </c>
@@ -2862,54 +2790,55 @@
         <v>3</v>
       </c>
       <c r="C45" s="16">
-        <f t="shared" ref="C45:L45" si="13">C41/$B$44</f>
+        <f t="shared" ref="C45:M45" si="13">C41/$B$44</f>
         <v>8.75</v>
       </c>
       <c r="D45" s="16">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="E45" s="16">
-        <f>E41/$E$44</f>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16">
+        <f>F41/$F$44</f>
         <v>4</v>
       </c>
-      <c r="F45" s="16">
-        <f t="shared" ref="F45:I45" si="14">F41/$E$44</f>
+      <c r="G45" s="16">
+        <f t="shared" ref="G45:J45" si="14">G41/$F$44</f>
         <v>4.8888888888888893</v>
       </c>
-      <c r="G45" s="16">
+      <c r="H45" s="16">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="H45" s="16">
+      <c r="I45" s="16">
         <f t="shared" si="14"/>
         <v>9.6296296296296298</v>
       </c>
-      <c r="I45" s="16">
+      <c r="J45" s="16">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="J45" s="16">
-        <f>J41/$J$44</f>
+      <c r="K45" s="16">
+        <f>K41/$K$44</f>
         <v>8</v>
       </c>
-      <c r="K45" s="16">
+      <c r="L45" s="16">
         <f t="shared" si="13"/>
         <v>55</v>
       </c>
-      <c r="L45" s="16">
+      <c r="M45" s="16">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="M45" s="29"/>
       <c r="N45" s="29"/>
       <c r="O45" s="29"/>
       <c r="P45" s="29"/>
       <c r="Q45" s="29"/>
       <c r="R45" s="29"/>
       <c r="S45" s="29"/>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T45" s="29"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>67</v>
       </c>
@@ -2918,77 +2847,79 @@
         <v>10</v>
       </c>
       <c r="C46" s="16">
-        <f t="shared" ref="C46:L46" si="15">C42/$B$44</f>
+        <f t="shared" ref="C46:M46" si="15">C42/$B$44</f>
         <v>35</v>
       </c>
       <c r="D46" s="16">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="E46" s="16">
-        <f>E42/$E$44</f>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16">
+        <f>F42/$F$44</f>
         <v>20</v>
       </c>
-      <c r="F46" s="16">
-        <f t="shared" ref="F46:I46" si="16">F42/$E$44</f>
+      <c r="G46" s="16">
+        <f t="shared" ref="G46:J46" si="16">G42/$F$44</f>
         <v>24.444444444444443</v>
       </c>
-      <c r="G46" s="16">
+      <c r="H46" s="16">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="H46" s="16">
+      <c r="I46" s="16">
         <f t="shared" si="16"/>
         <v>48.148148148148145</v>
       </c>
-      <c r="I46" s="16">
+      <c r="J46" s="16">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J46" s="16">
-        <f>J42/$J$44</f>
+      <c r="K46" s="16">
+        <f>K42/$K$44</f>
         <v>60</v>
       </c>
-      <c r="K46" s="16">
+      <c r="L46" s="16">
         <f t="shared" si="15"/>
         <v>412.5</v>
       </c>
-      <c r="L46" s="16">
+      <c r="M46" s="16">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="M46" s="29"/>
       <c r="N46" s="29"/>
       <c r="O46" s="29"/>
       <c r="P46" s="29"/>
       <c r="Q46" s="29"/>
       <c r="R46" s="29"/>
       <c r="S46" s="29"/>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T46" s="29"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
-      <c r="E47" s="17"/>
+      <c r="E47" s="16"/>
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
+      <c r="I47" s="17"/>
       <c r="J47" s="18"/>
       <c r="K47" s="18"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="29"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="20"/>
       <c r="N47" s="29"/>
       <c r="O47" s="29"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="29"/>
       <c r="R47" s="29"/>
       <c r="S47" s="29"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T47" s="29"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>7</v>
       </c>
@@ -3001,49 +2932,50 @@
       <c r="D48" s="16">
         <v>280</v>
       </c>
-      <c r="E48" s="16">
+      <c r="E48" s="16"/>
+      <c r="F48" s="16">
         <v>265</v>
       </c>
-      <c r="F48" s="17">
+      <c r="G48" s="17">
         <v>150</v>
       </c>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17">
+      <c r="H48" s="17"/>
+      <c r="I48" s="17">
         <v>375</v>
       </c>
-      <c r="I48" s="18">
+      <c r="J48" s="18">
         <v>640</v>
       </c>
-      <c r="J48" s="18">
+      <c r="K48" s="18">
         <v>400</v>
       </c>
-      <c r="K48" s="18">
+      <c r="L48" s="18">
         <v>600</v>
       </c>
-      <c r="L48" s="19">
+      <c r="M48" s="19">
         <v>900</v>
       </c>
-      <c r="M48" s="23">
+      <c r="N48" s="23">
         <v>1200</v>
       </c>
-      <c r="N48" s="23">
+      <c r="O48" s="23">
         <v>30000</v>
       </c>
-      <c r="O48" s="29"/>
-      <c r="P48" s="23">
+      <c r="P48" s="29"/>
+      <c r="Q48" s="23">
         <v>3500</v>
       </c>
-      <c r="Q48" s="23">
+      <c r="R48" s="23">
         <v>2750</v>
       </c>
-      <c r="R48" s="23">
+      <c r="S48" s="23">
         <v>1600</v>
       </c>
-      <c r="S48" s="23">
+      <c r="T48" s="23">
         <v>4200</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>9</v>
       </c>
@@ -3051,42 +2983,45 @@
         <v>5</v>
       </c>
       <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="17">
+      <c r="D49" s="16">
+        <v>3</v>
+      </c>
+      <c r="E49" s="16"/>
+      <c r="F49" s="17">
         <v>3.6</v>
       </c>
-      <c r="F49" s="17">
+      <c r="G49" s="17">
         <v>2.6</v>
       </c>
-      <c r="G49" s="17"/>
       <c r="H49" s="17"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18">
+      <c r="I49" s="17"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18">
         <v>4.5</v>
       </c>
-      <c r="K49" s="18">
+      <c r="L49" s="18">
         <v>2.6</v>
       </c>
-      <c r="L49" s="20"/>
-      <c r="M49" s="29">
+      <c r="M49" s="20"/>
+      <c r="N49" s="29">
         <v>3.2</v>
       </c>
-      <c r="N49" s="23">
+      <c r="O49" s="23">
         <v>2.7</v>
       </c>
-      <c r="O49" s="29"/>
-      <c r="P49" s="23">
+      <c r="P49" s="29"/>
+      <c r="Q49" s="23">
         <v>3.75</v>
       </c>
-      <c r="Q49" s="29"/>
-      <c r="R49" s="23">
+      <c r="R49" s="29"/>
+      <c r="S49" s="23">
         <v>2.2999999999999998</v>
       </c>
-      <c r="S49" s="29">
+      <c r="T49" s="29">
         <v>3.6</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>69</v>
       </c>
@@ -3095,39 +3030,42 @@
         <v>20</v>
       </c>
       <c r="D50" s="16">
+        <v>30</v>
+      </c>
+      <c r="E50" s="16">
+        <v>30</v>
+      </c>
+      <c r="F50" s="16">
+        <v>25</v>
+      </c>
+      <c r="G50" s="17">
+        <v>33</v>
+      </c>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18">
         <v>35</v>
       </c>
-      <c r="E50" s="16">
-        <v>25</v>
-      </c>
-      <c r="F50" s="17">
-        <v>33</v>
-      </c>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18">
-        <v>35</v>
-      </c>
-      <c r="K50" s="18"/>
-      <c r="L50" s="19"/>
-      <c r="M50" s="29">
+      <c r="L50" s="18"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="29">
         <v>75</v>
       </c>
-      <c r="N50" s="29">
+      <c r="O50" s="29">
         <v>1380</v>
       </c>
-      <c r="O50" s="29"/>
       <c r="P50" s="29"/>
       <c r="Q50" s="29"/>
-      <c r="R50" s="29">
+      <c r="R50" s="29"/>
+      <c r="S50" s="29">
         <v>600</v>
       </c>
-      <c r="S50" s="29">
+      <c r="T50" s="29">
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>70</v>
       </c>
@@ -3138,19 +3076,20 @@
       <c r="F51" s="16"/>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
-      <c r="I51" s="18"/>
+      <c r="I51" s="16"/>
       <c r="J51" s="18"/>
       <c r="K51" s="18"/>
-      <c r="L51" s="19"/>
-      <c r="M51" s="29"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="19"/>
       <c r="N51" s="29"/>
       <c r="O51" s="29"/>
       <c r="P51" s="29"/>
       <c r="Q51" s="29"/>
       <c r="R51" s="29"/>
       <c r="S51" s="29"/>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T51" s="29"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>71</v>
       </c>
@@ -3161,44 +3100,46 @@
       <c r="F52" s="16"/>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
-      <c r="I52" s="18"/>
+      <c r="I52" s="16"/>
       <c r="J52" s="18"/>
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
-      <c r="M52" s="29"/>
+      <c r="M52" s="18"/>
       <c r="N52" s="29"/>
       <c r="O52" s="29"/>
       <c r="P52" s="29"/>
       <c r="Q52" s="29"/>
       <c r="R52" s="29"/>
       <c r="S52" s="29"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T52" s="29"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>72</v>
       </c>
       <c r="B53" s="16"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17">
+      <c r="E53" s="16"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17">
         <v>9</v>
       </c>
-      <c r="G53" s="17"/>
       <c r="H53" s="17"/>
-      <c r="I53" s="18"/>
+      <c r="I53" s="17"/>
       <c r="J53" s="18"/>
       <c r="K53" s="18"/>
-      <c r="L53" s="20"/>
-      <c r="M53" s="29"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="20"/>
       <c r="N53" s="29"/>
       <c r="O53" s="29"/>
       <c r="P53" s="29"/>
       <c r="Q53" s="29"/>
       <c r="R53" s="29"/>
       <c r="S53" s="29"/>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T53" s="29"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>73</v>
       </c>
@@ -3206,26 +3147,27 @@
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
-      <c r="F54" s="16">
+      <c r="F54" s="16"/>
+      <c r="G54" s="16">
         <v>1.5</v>
       </c>
-      <c r="G54" s="16"/>
       <c r="H54" s="16"/>
-      <c r="I54" s="18"/>
+      <c r="I54" s="16"/>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
-      <c r="M54" s="29"/>
+      <c r="M54" s="18"/>
       <c r="N54" s="29"/>
       <c r="O54" s="29"/>
       <c r="P54" s="29"/>
       <c r="Q54" s="29"/>
-      <c r="R54" s="29">
+      <c r="R54" s="29"/>
+      <c r="S54" s="29">
         <v>5</v>
       </c>
-      <c r="S54" s="29"/>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T54" s="29"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>74</v>
       </c>
@@ -3233,24 +3175,25 @@
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
-      <c r="F55" s="16">
+      <c r="F55" s="16"/>
+      <c r="G55" s="16">
         <v>5</v>
       </c>
-      <c r="G55" s="16"/>
       <c r="H55" s="16"/>
-      <c r="I55" s="18"/>
+      <c r="I55" s="16"/>
       <c r="J55" s="18"/>
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
-      <c r="M55" s="29"/>
+      <c r="M55" s="18"/>
       <c r="N55" s="29"/>
       <c r="O55" s="29"/>
       <c r="P55" s="29"/>
       <c r="Q55" s="29"/>
       <c r="R55" s="29"/>
       <c r="S55" s="29"/>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T55" s="29"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>75</v>
       </c>
@@ -3261,19 +3204,20 @@
       <c r="F56" s="16"/>
       <c r="G56" s="16"/>
       <c r="H56" s="16"/>
-      <c r="I56" s="18"/>
+      <c r="I56" s="16"/>
       <c r="J56" s="18"/>
       <c r="K56" s="18"/>
-      <c r="L56" s="19"/>
-      <c r="M56" s="29"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="19"/>
       <c r="N56" s="29"/>
       <c r="O56" s="29"/>
       <c r="P56" s="29"/>
       <c r="Q56" s="29"/>
       <c r="R56" s="29"/>
       <c r="S56" s="29"/>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T56" s="29"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>76</v>
       </c>
@@ -3282,37 +3226,38 @@
         <v>14</v>
       </c>
       <c r="D57" s="16"/>
-      <c r="E57" s="17">
+      <c r="E57" s="16"/>
+      <c r="F57" s="17">
         <v>18</v>
       </c>
-      <c r="F57" s="17">
+      <c r="G57" s="17">
         <v>28</v>
       </c>
-      <c r="G57" s="17"/>
       <c r="H57" s="17"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18">
+      <c r="I57" s="17"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18">
         <v>23</v>
       </c>
-      <c r="K57" s="18"/>
-      <c r="L57" s="20"/>
-      <c r="M57" s="29">
+      <c r="L57" s="18"/>
+      <c r="M57" s="20"/>
+      <c r="N57" s="29">
         <v>20</v>
       </c>
-      <c r="N57" s="23">
+      <c r="O57" s="23">
         <v>35</v>
       </c>
-      <c r="O57" s="29"/>
       <c r="P57" s="29"/>
-      <c r="Q57" s="29">
+      <c r="Q57" s="29"/>
+      <c r="R57" s="29">
         <v>35</v>
       </c>
-      <c r="R57" s="29"/>
-      <c r="S57" s="29">
+      <c r="S57" s="29"/>
+      <c r="T57" s="29">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>91</v>
       </c>
@@ -3321,31 +3266,32 @@
       </c>
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
-      <c r="E58" s="17">
-        <v>20</v>
-      </c>
+      <c r="E58" s="16"/>
       <c r="F58" s="17">
         <v>20</v>
       </c>
-      <c r="G58" s="17"/>
+      <c r="G58" s="17">
+        <v>20</v>
+      </c>
       <c r="H58" s="17"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="18">
+      <c r="I58" s="17"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18">
         <v>15</v>
       </c>
-      <c r="K58" s="18">
+      <c r="L58" s="18">
         <v>18</v>
       </c>
-      <c r="L58" s="23"/>
-      <c r="M58" s="29"/>
+      <c r="M58" s="23"/>
       <c r="N58" s="29"/>
       <c r="O58" s="29"/>
       <c r="P58" s="29"/>
       <c r="Q58" s="29"/>
       <c r="R58" s="29"/>
       <c r="S58" s="29"/>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T58" s="29"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>77</v>
       </c>
@@ -3356,30 +3302,31 @@
         <v>81</v>
       </c>
       <c r="D59" s="14"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15" t="s">
+      <c r="E59" s="14"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="G59" s="15"/>
       <c r="H59" s="15"/>
       <c r="I59" s="15"/>
       <c r="J59" s="15"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
-      <c r="M59" t="s">
+      <c r="M59" s="15"/>
+      <c r="N59" t="s">
         <v>113</v>
       </c>
-      <c r="N59" t="s">
+      <c r="O59" t="s">
         <v>114</v>
       </c>
-      <c r="P59" t="s">
+      <c r="Q59" t="s">
         <v>120</v>
       </c>
-      <c r="R59" t="s">
+      <c r="S59" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>78</v>
       </c>
@@ -3395,7 +3342,7 @@
       <c r="K60" s="15"/>
       <c r="L60" s="15"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>79</v>
       </c>
@@ -4809,82 +4756,82 @@
     <mergeCell ref="J6:M6"/>
   </mergeCells>
   <conditionalFormatting sqref="G9:M33">
-    <cfRule type="expression" dxfId="51" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="71" stopIfTrue="1">
       <formula>G9&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="72" stopIfTrue="1">
       <formula>MOD(G9,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F3">
-    <cfRule type="expression" dxfId="39" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="61" stopIfTrue="1">
       <formula>B2&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="62" stopIfTrue="1">
       <formula>MOD(B2,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:F12">
-    <cfRule type="expression" dxfId="31" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="31" stopIfTrue="1">
       <formula>B12&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="32" stopIfTrue="1">
       <formula>MOD(B12,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:F33">
-    <cfRule type="expression" dxfId="21" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
       <formula>B25&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
       <formula>MOD(B25,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:F21">
-    <cfRule type="expression" dxfId="19" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="35" stopIfTrue="1">
       <formula>B20&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="36" stopIfTrue="1">
       <formula>MOD(B20,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:F22">
-    <cfRule type="expression" dxfId="17" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="33" stopIfTrue="1">
       <formula>B22&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="34" stopIfTrue="1">
       <formula>MOD(B22,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:F23">
-    <cfRule type="expression" dxfId="15" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="29" stopIfTrue="1">
       <formula>B23&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="30" stopIfTrue="1">
       <formula>MOD(B23,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:F33">
-    <cfRule type="expression" dxfId="13" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="39" stopIfTrue="1">
       <formula>B9&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="40" stopIfTrue="1">
       <formula>MOD(B9,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:F15">
-    <cfRule type="expression" dxfId="11" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="27" stopIfTrue="1">
       <formula>E15&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="28" stopIfTrue="1">
       <formula>MOD(E15,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:F16">
-    <cfRule type="expression" dxfId="9" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="25" stopIfTrue="1">
       <formula>E16&gt;9999</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="26" stopIfTrue="1">
       <formula>MOD(E16,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
T3 arty, swap anchor with bombardment
Becasue while is anchor only 1,5s penality, then its too big buff and
isnt reason to unanchor, while it have also deploy with similar time.

because bombardment its more cool.
</commit_message>
<xml_diff>
--- a/Units.xlsx
+++ b/Units.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="271">
   <si>
     <t>Stats</t>
   </si>
@@ -228,21 +228,6 @@
     <t>Energy maintaince</t>
   </si>
   <si>
-    <t>DPS 1st weapon</t>
-  </si>
-  <si>
-    <t>DPS 2th weapon</t>
-  </si>
-  <si>
-    <t>DPS 3rd weapon</t>
-  </si>
-  <si>
-    <t>shot/second</t>
-  </si>
-  <si>
-    <t>Area efect</t>
-  </si>
-  <si>
     <t>Minimal range/lower</t>
   </si>
   <si>
@@ -273,18 +258,12 @@
     <t>lab</t>
   </si>
   <si>
-    <t>aa/arty</t>
-  </si>
-  <si>
     <t>tank</t>
   </si>
   <si>
     <t>tank destroyer</t>
   </si>
   <si>
-    <t>Enginer</t>
-  </si>
-  <si>
     <t>Silhouette</t>
   </si>
   <si>
@@ -297,9 +276,6 @@
     <t>Intel</t>
   </si>
   <si>
-    <t>T2 enginer</t>
-  </si>
-  <si>
     <t>Barrager</t>
   </si>
   <si>
@@ -312,9 +288,6 @@
     <t>inu201</t>
   </si>
   <si>
-    <t>t3 engie</t>
-  </si>
-  <si>
     <t>inu2002</t>
   </si>
   <si>
@@ -366,9 +339,6 @@
     <t>transportable</t>
   </si>
   <si>
-    <t>inu3001</t>
-  </si>
-  <si>
     <t>Sacu</t>
   </si>
   <si>
@@ -796,6 +766,72 @@
   </si>
   <si>
     <t>Golem</t>
+  </si>
+  <si>
+    <t>inu3008</t>
+  </si>
+  <si>
+    <t>inu3007</t>
+  </si>
+  <si>
+    <t>T3 mAA</t>
+  </si>
+  <si>
+    <t>Watchman</t>
+  </si>
+  <si>
+    <t>arty</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>T2 field enginer</t>
+  </si>
+  <si>
+    <t>Scarab</t>
+  </si>
+  <si>
+    <t>inu1002</t>
+  </si>
+  <si>
+    <t>inu1001</t>
+  </si>
+  <si>
+    <t>44 radar 24 vision</t>
+  </si>
+  <si>
+    <t>T1 enginer</t>
+  </si>
+  <si>
+    <t>inu1004</t>
+  </si>
+  <si>
+    <t>T2 Enginer</t>
+  </si>
+  <si>
+    <t>inu1005</t>
+  </si>
+  <si>
+    <t>T3 enginer</t>
+  </si>
+  <si>
+    <t>12,5bp</t>
+  </si>
+  <si>
+    <t>30bp</t>
+  </si>
+  <si>
+    <t>5bp</t>
+  </si>
+  <si>
+    <t>inu1006</t>
+  </si>
+  <si>
+    <t>inu1007</t>
+  </si>
+  <si>
+    <t>Astor</t>
   </si>
 </sst>
 </file>
@@ -1477,10 +1513,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
       <selection activeCell="A73" sqref="A73"/>
-      <selection pane="topRight" activeCell="D49" sqref="D49"/>
+      <selection pane="topRight" activeCell="S64" sqref="S64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,19 +1571,19 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D5" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="E5" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="F5" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1588,7 +1624,7 @@
         <v>37</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>43</v>
@@ -1597,7 +1633,7 @@
         <v>51</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>47</v>
@@ -2369,7 +2405,7 @@
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
@@ -2386,12 +2422,12 @@
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>15</v>
       </c>
@@ -2406,7 +2442,7 @@
       </c>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>19</v>
       </c>
@@ -2421,481 +2457,521 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
+      <c r="B38" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="H38" s="26"/>
       <c r="I38" t="s">
+        <v>263</v>
+      </c>
+      <c r="J38" t="s">
+        <v>88</v>
+      </c>
+      <c r="L38" t="s">
+        <v>89</v>
+      </c>
+      <c r="M38" t="s">
+        <v>92</v>
+      </c>
+      <c r="N38" t="s">
+        <v>95</v>
+      </c>
+      <c r="O38" t="s">
+        <v>98</v>
+      </c>
+      <c r="P38" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>107</v>
+      </c>
+      <c r="R38" t="s">
+        <v>107</v>
+      </c>
+      <c r="S38" t="s">
+        <v>111</v>
+      </c>
+      <c r="T38" t="s">
+        <v>250</v>
+      </c>
+      <c r="U38" t="s">
+        <v>249</v>
+      </c>
+      <c r="V38" t="s">
+        <v>114</v>
+      </c>
+      <c r="W38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="I39" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="J39" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="M39" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="N39" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="J38" t="s">
-        <v>98</v>
-      </c>
-      <c r="K38" t="s">
-        <v>101</v>
-      </c>
-      <c r="L38" t="s">
-        <v>104</v>
-      </c>
-      <c r="M38" t="s">
-        <v>107</v>
-      </c>
-      <c r="N38" t="s">
-        <v>110</v>
-      </c>
-      <c r="O38" t="s">
+      <c r="O39" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="P39" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q39" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="R39" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="S39" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="T39" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="U39" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="V39" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="P38" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>121</v>
-      </c>
-      <c r="R38" t="s">
-        <v>124</v>
-      </c>
-      <c r="S38" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="21"/>
-      <c r="F39" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G39" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="H39" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="I39" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="J39" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="K39" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="L39" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="M39" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="N39" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="O39" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="P39" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q39" s="22" t="s">
+      <c r="W39" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="R39" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="S39" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="T39" s="22" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" s="24"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24" t="s">
+        <v>81</v>
+      </c>
       <c r="D40" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="E40" s="24"/>
+        <v>270</v>
+      </c>
+      <c r="E40" s="24" t="s">
+        <v>85</v>
+      </c>
       <c r="F40" s="24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G40" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="H40" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="M40" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25" t="s">
+      <c r="N40" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="O40" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="L40" s="25" t="s">
+      <c r="P40" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="M40" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="N40" s="28" t="s">
+      <c r="Q40" s="15"/>
+      <c r="R40" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="O40" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q40" s="28" t="s">
+      <c r="S40" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="T40" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="U40" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="V40" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="W40" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="R40" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="S40" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="T40" s="28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="16">
+        <v>52</v>
+      </c>
+      <c r="C41" s="16">
         <v>12</v>
       </c>
-      <c r="C41" s="16">
+      <c r="D41" s="16">
         <v>35</v>
       </c>
-      <c r="D41" s="16"/>
       <c r="E41" s="16"/>
-      <c r="F41" s="16">
+      <c r="F41" s="16"/>
+      <c r="G41" s="16">
         <v>54</v>
       </c>
-      <c r="G41" s="17">
+      <c r="H41" s="17">
         <v>66</v>
       </c>
-      <c r="H41" s="17"/>
       <c r="I41" s="17">
         <v>130</v>
       </c>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18">
+      <c r="J41" s="17">
+        <v>312</v>
+      </c>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18">
         <v>100</v>
       </c>
-      <c r="L41" s="18">
+      <c r="M41" s="18">
         <v>220</v>
       </c>
-      <c r="M41" s="19"/>
-      <c r="N41" s="23">
+      <c r="N41" s="19"/>
+      <c r="O41" s="23">
         <v>197</v>
       </c>
-      <c r="O41" s="23">
+      <c r="P41" s="23">
         <v>12500</v>
       </c>
-      <c r="P41" s="29"/>
-      <c r="Q41" s="23">
+      <c r="Q41" s="29"/>
+      <c r="R41" s="23">
         <v>640</v>
       </c>
-      <c r="R41" s="23">
+      <c r="S41" s="23">
         <v>360</v>
       </c>
-      <c r="S41" s="23">
+      <c r="T41" s="23">
+        <v>640</v>
+      </c>
+      <c r="V41" s="23">
         <v>960</v>
       </c>
-      <c r="T41" s="23">
+      <c r="W41" s="23">
         <v>480</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B42" s="16">
+        <v>260</v>
+      </c>
+      <c r="C42" s="16">
         <v>40</v>
       </c>
-      <c r="C42" s="16">
+      <c r="D42" s="16">
         <v>140</v>
       </c>
-      <c r="D42" s="16"/>
       <c r="E42" s="16"/>
-      <c r="F42" s="17">
+      <c r="F42" s="16"/>
+      <c r="G42" s="17">
         <v>270</v>
       </c>
-      <c r="G42" s="17">
+      <c r="H42" s="17">
         <v>330</v>
       </c>
-      <c r="H42" s="17"/>
       <c r="I42" s="17">
         <v>650</v>
       </c>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18">
+      <c r="J42" s="17">
+        <v>1560</v>
+      </c>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18">
         <v>750</v>
       </c>
-      <c r="L42" s="18">
+      <c r="M42" s="18">
         <v>1650</v>
       </c>
-      <c r="M42" s="20"/>
-      <c r="N42" s="23">
+      <c r="N42" s="20"/>
+      <c r="O42" s="23">
         <v>990</v>
       </c>
-      <c r="O42" s="23">
+      <c r="P42" s="23">
         <v>240000</v>
       </c>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="23">
+      <c r="Q42" s="29"/>
+      <c r="R42" s="23">
         <v>8000</v>
       </c>
-      <c r="R42" s="23">
+      <c r="S42" s="23">
         <v>1800</v>
       </c>
-      <c r="S42" s="23">
+      <c r="T42" s="23">
+        <v>6400</v>
+      </c>
+      <c r="V42" s="23">
         <v>9600</v>
       </c>
-      <c r="T42" s="23">
+      <c r="W42" s="23">
         <v>5400</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>64</v>
       </c>
       <c r="B43" s="16">
+        <v>260</v>
+      </c>
+      <c r="C43" s="16">
         <v>80</v>
       </c>
-      <c r="C43" s="16">
+      <c r="D43" s="16">
         <v>120</v>
       </c>
-      <c r="D43" s="16"/>
       <c r="E43" s="16"/>
-      <c r="F43" s="16">
+      <c r="F43" s="16"/>
+      <c r="G43" s="16">
         <v>270</v>
       </c>
-      <c r="G43" s="17">
+      <c r="H43" s="17">
         <v>330</v>
       </c>
-      <c r="H43" s="17"/>
       <c r="I43" s="17">
         <v>650</v>
       </c>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18">
+      <c r="J43" s="17">
+        <v>1560</v>
+      </c>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18">
         <v>500</v>
       </c>
-      <c r="L43" s="18">
+      <c r="M43" s="18">
         <v>1100</v>
       </c>
-      <c r="M43" s="19"/>
-      <c r="N43" s="23">
+      <c r="N43" s="19"/>
+      <c r="O43" s="23">
         <v>880</v>
       </c>
-      <c r="O43" s="23">
+      <c r="P43" s="23">
         <v>12000</v>
       </c>
-      <c r="P43" s="29"/>
-      <c r="Q43" s="23">
+      <c r="Q43" s="29"/>
+      <c r="R43" s="23">
         <v>640</v>
       </c>
-      <c r="R43" s="23">
+      <c r="S43" s="23">
         <v>1600</v>
       </c>
-      <c r="S43" s="23">
+      <c r="T43" s="23">
+        <v>3200</v>
+      </c>
+      <c r="V43" s="23">
         <v>5000</v>
       </c>
-      <c r="T43" s="23">
+      <c r="W43" s="23">
         <v>2400</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="16">
-        <f>B43/$B$36</f>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16">
+        <f>C43/$B$36</f>
         <v>4</v>
       </c>
-      <c r="C44" s="16">
-        <f t="shared" ref="C44:M44" si="9">C43/$B$36</f>
+      <c r="D44" s="16">
+        <f t="shared" ref="D44:N44" si="9">D43/$B$36</f>
         <v>6</v>
       </c>
-      <c r="D44" s="16">
+      <c r="E44" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16">
+      <c r="F44" s="16"/>
+      <c r="G44" s="16">
         <f t="shared" si="9"/>
         <v>13.5</v>
       </c>
-      <c r="G44" s="16">
-        <f t="shared" ref="G44" si="10">G43/$B$36</f>
+      <c r="H44" s="16">
+        <f t="shared" ref="H44" si="10">H43/$B$36</f>
         <v>16.5</v>
       </c>
-      <c r="H44" s="16">
-        <f t="shared" ref="H44" si="11">H43/$B$36</f>
-        <v>0</v>
-      </c>
-      <c r="I44" s="16">
-        <f>I43/$B$36</f>
-        <v>32.5</v>
-      </c>
-      <c r="J44" s="16">
-        <f t="shared" ref="J44" si="12">J43/$B$36</f>
-        <v>0</v>
-      </c>
-      <c r="K44" s="16">
-        <f>K43/$C$36</f>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16">
+        <f>L43/$C$36</f>
         <v>12.5</v>
       </c>
-      <c r="L44" s="16">
+      <c r="M44" s="16">
         <f t="shared" si="9"/>
         <v>55</v>
       </c>
-      <c r="M44" s="16">
+      <c r="N44" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="N44" s="29"/>
       <c r="O44" s="29"/>
       <c r="P44" s="29"/>
       <c r="Q44" s="29"/>
       <c r="R44" s="29"/>
       <c r="S44" s="29"/>
       <c r="T44" s="29"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="16">
-        <f>B41/$B$44</f>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16">
+        <f t="shared" ref="C45:E46" si="11">C41/$C$44</f>
         <v>3</v>
       </c>
-      <c r="C45" s="16">
-        <f t="shared" ref="C45:M45" si="13">C41/$B$44</f>
+      <c r="D45" s="16">
+        <f t="shared" si="11"/>
         <v>8.75</v>
       </c>
-      <c r="D45" s="16">
-        <f t="shared" si="13"/>
+      <c r="E45" s="16">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16">
-        <f>F41/$F$44</f>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16">
+        <f>G41/$G$44</f>
         <v>4</v>
       </c>
-      <c r="G45" s="16">
-        <f t="shared" ref="G45:J45" si="14">G41/$F$44</f>
-        <v>4.8888888888888893</v>
-      </c>
-      <c r="H45" s="16">
-        <f t="shared" si="14"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16">
+        <f>L41/$L$44</f>
+        <v>8</v>
+      </c>
+      <c r="M45" s="16">
+        <f>M41/$C$44</f>
+        <v>55</v>
+      </c>
+      <c r="N45" s="16">
+        <f>N41/$C$44</f>
         <v>0</v>
       </c>
-      <c r="I45" s="16">
-        <f t="shared" si="14"/>
-        <v>9.6296296296296298</v>
-      </c>
-      <c r="J45" s="16">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="K45" s="16">
-        <f>K41/$K$44</f>
-        <v>8</v>
-      </c>
-      <c r="L45" s="16">
-        <f t="shared" si="13"/>
-        <v>55</v>
-      </c>
-      <c r="M45" s="16">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="N45" s="29"/>
       <c r="O45" s="29"/>
       <c r="P45" s="29"/>
       <c r="Q45" s="29"/>
       <c r="R45" s="29"/>
       <c r="S45" s="29"/>
       <c r="T45" s="29"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V45" s="29"/>
+      <c r="W45" s="29"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="16">
-        <f>B42/$B$44</f>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16">
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
-      <c r="C46" s="16">
-        <f t="shared" ref="C46:M46" si="15">C42/$B$44</f>
+      <c r="D46" s="16">
+        <f t="shared" si="11"/>
         <v>35</v>
       </c>
-      <c r="D46" s="16">
-        <f t="shared" si="15"/>
+      <c r="E46" s="16">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16">
-        <f>F42/$F$44</f>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16">
+        <f>G42/$G$44</f>
         <v>20</v>
       </c>
-      <c r="G46" s="16">
-        <f t="shared" ref="G46:J46" si="16">G42/$F$44</f>
-        <v>24.444444444444443</v>
-      </c>
-      <c r="H46" s="16">
-        <f t="shared" si="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16">
+        <f>L42/$L$44</f>
+        <v>60</v>
+      </c>
+      <c r="M46" s="16">
+        <f>M42/$C$44</f>
+        <v>412.5</v>
+      </c>
+      <c r="N46" s="16">
+        <f>N42/$C$44</f>
         <v>0</v>
       </c>
-      <c r="I46" s="16">
-        <f t="shared" si="16"/>
-        <v>48.148148148148145</v>
-      </c>
-      <c r="J46" s="16">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="K46" s="16">
-        <f>K42/$K$44</f>
-        <v>60</v>
-      </c>
-      <c r="L46" s="16">
-        <f t="shared" si="15"/>
-        <v>412.5</v>
-      </c>
-      <c r="M46" s="16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="N46" s="29"/>
       <c r="O46" s="29"/>
       <c r="P46" s="29"/>
       <c r="Q46" s="29"/>
       <c r="R46" s="29"/>
       <c r="S46" s="29"/>
       <c r="T46" s="29"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V46" s="29"/>
+      <c r="W46" s="29"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>68</v>
       </c>
@@ -2903,299 +2979,357 @@
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
-      <c r="F47" s="17"/>
+      <c r="F47" s="16"/>
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
       <c r="I47" s="17"/>
-      <c r="J47" s="18"/>
+      <c r="J47" s="17"/>
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
-      <c r="M47" s="20"/>
-      <c r="N47" s="29"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="20"/>
       <c r="O47" s="29"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="29"/>
       <c r="R47" s="29"/>
       <c r="S47" s="29"/>
       <c r="T47" s="29"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V47" s="29"/>
+      <c r="W47" s="29"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B48" s="16">
+        <v>130</v>
+      </c>
+      <c r="C48" s="16">
         <v>23</v>
       </c>
-      <c r="C48" s="16">
+      <c r="D48" s="16">
         <v>65</v>
       </c>
-      <c r="D48" s="16">
+      <c r="E48" s="16">
         <v>280</v>
       </c>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16">
+      <c r="F48" s="16"/>
+      <c r="G48" s="16">
         <v>265</v>
       </c>
-      <c r="G48" s="17">
+      <c r="H48" s="17">
         <v>150</v>
       </c>
-      <c r="H48" s="17"/>
       <c r="I48" s="17">
         <v>375</v>
       </c>
-      <c r="J48" s="18">
+      <c r="J48" s="17">
         <v>640</v>
       </c>
-      <c r="K48" s="18">
+      <c r="K48" s="18"/>
+      <c r="L48" s="18">
         <v>400</v>
       </c>
-      <c r="L48" s="18">
+      <c r="M48" s="18">
         <v>600</v>
       </c>
-      <c r="M48" s="19">
+      <c r="N48" s="19">
         <v>900</v>
       </c>
-      <c r="N48" s="23">
+      <c r="O48" s="23">
         <v>1200</v>
       </c>
-      <c r="O48" s="23">
+      <c r="P48" s="23">
         <v>30000</v>
       </c>
-      <c r="P48" s="29"/>
-      <c r="Q48" s="23">
+      <c r="Q48" s="29"/>
+      <c r="R48" s="23">
         <v>3500</v>
       </c>
-      <c r="R48" s="23">
+      <c r="S48" s="23">
         <v>2750</v>
       </c>
-      <c r="S48" s="23">
+      <c r="T48" s="23">
+        <v>2200</v>
+      </c>
+      <c r="V48" s="23">
         <v>1600</v>
       </c>
-      <c r="T48" s="23">
+      <c r="W48" s="23">
         <v>4200</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B49" s="16">
+      <c r="B49" s="16"/>
+      <c r="C49" s="16">
         <v>5</v>
       </c>
-      <c r="C49" s="16"/>
       <c r="D49" s="16">
+        <v>4</v>
+      </c>
+      <c r="E49" s="16">
         <v>3</v>
       </c>
-      <c r="E49" s="16"/>
-      <c r="F49" s="17">
+      <c r="F49" s="16"/>
+      <c r="G49" s="17">
         <v>3.6</v>
       </c>
-      <c r="G49" s="17">
+      <c r="H49" s="17">
         <v>2.6</v>
       </c>
-      <c r="H49" s="17"/>
       <c r="I49" s="17"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18">
+      <c r="J49" s="17"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18">
         <v>4.5</v>
       </c>
-      <c r="L49" s="18">
+      <c r="M49" s="18">
         <v>2.6</v>
       </c>
-      <c r="M49" s="20"/>
-      <c r="N49" s="29">
+      <c r="N49" s="20"/>
+      <c r="O49" s="29">
         <v>3.2</v>
       </c>
-      <c r="O49" s="23">
+      <c r="P49" s="23">
         <v>2.7</v>
       </c>
-      <c r="P49" s="29"/>
-      <c r="Q49" s="23">
+      <c r="Q49" s="29"/>
+      <c r="R49" s="23">
         <v>3.75</v>
       </c>
-      <c r="R49" s="29"/>
-      <c r="S49" s="23">
+      <c r="S49" s="29"/>
+      <c r="T49" s="23">
+        <v>3</v>
+      </c>
+      <c r="V49" s="23">
         <v>2.2999999999999998</v>
       </c>
-      <c r="T49" s="29">
+      <c r="W49" s="29">
         <v>3.6</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16">
-        <v>20</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="C50" s="16"/>
       <c r="D50" s="16">
+        <v>8</v>
+      </c>
+      <c r="E50" s="16">
+        <v>50</v>
+      </c>
+      <c r="F50" s="16">
         <v>30</v>
       </c>
-      <c r="E50" s="16">
-        <v>30</v>
-      </c>
-      <c r="F50" s="16">
-        <v>25</v>
-      </c>
-      <c r="G50" s="17">
-        <v>33</v>
-      </c>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18">
-        <v>35</v>
-      </c>
+      <c r="G50" s="16"/>
+      <c r="H50" s="17">
+        <v>300</v>
+      </c>
+      <c r="I50" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="J50" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="K50" s="18"/>
       <c r="L50" s="18"/>
-      <c r="M50" s="19"/>
-      <c r="N50" s="29">
-        <v>75</v>
-      </c>
-      <c r="O50" s="29">
-        <v>1380</v>
-      </c>
+      <c r="M50" s="18"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="29"/>
       <c r="P50" s="29"/>
       <c r="Q50" s="29"/>
       <c r="R50" s="29"/>
-      <c r="S50" s="29">
-        <v>600</v>
-      </c>
+      <c r="S50" s="29"/>
       <c r="T50" s="29">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="V50" s="29"/>
+      <c r="W50" s="29"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>70</v>
+        <v>164</v>
       </c>
       <c r="B51" s="16"/>
       <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
+      <c r="D51" s="16">
+        <v>0</v>
+      </c>
+      <c r="E51" s="16">
+        <v>1.5</v>
+      </c>
       <c r="F51" s="16"/>
       <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
+      <c r="H51" s="16">
+        <v>1.5</v>
+      </c>
       <c r="I51" s="16"/>
-      <c r="J51" s="18"/>
+      <c r="J51" s="16"/>
       <c r="K51" s="18"/>
       <c r="L51" s="18"/>
-      <c r="M51" s="19"/>
-      <c r="N51" s="29"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="19"/>
       <c r="O51" s="29"/>
       <c r="P51" s="29"/>
       <c r="Q51" s="29"/>
       <c r="R51" s="29"/>
       <c r="S51" s="29"/>
-      <c r="T51" s="29"/>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T51" s="29">
+        <v>0</v>
+      </c>
+      <c r="V51" s="29">
+        <v>5</v>
+      </c>
+      <c r="W51" s="29"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>71</v>
+        <v>170</v>
       </c>
       <c r="B52" s="16"/>
       <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
+      <c r="D52" s="16">
+        <v>1</v>
+      </c>
+      <c r="E52" s="16">
+        <v>4</v>
+      </c>
       <c r="F52" s="16"/>
       <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
+      <c r="H52" s="16">
+        <v>1</v>
+      </c>
       <c r="I52" s="16"/>
-      <c r="J52" s="18"/>
+      <c r="J52" s="16"/>
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
       <c r="M52" s="18"/>
-      <c r="N52" s="29"/>
+      <c r="N52" s="18"/>
       <c r="O52" s="29"/>
       <c r="P52" s="29"/>
       <c r="Q52" s="29"/>
       <c r="R52" s="29"/>
       <c r="S52" s="29"/>
-      <c r="T52" s="29"/>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T52" s="29">
+        <v>1</v>
+      </c>
+      <c r="V52" s="29"/>
+      <c r="W52" s="29"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="B53" s="16"/>
       <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17">
-        <v>9</v>
-      </c>
-      <c r="H53" s="17"/>
+      <c r="D53" s="16">
+        <v>2.5</v>
+      </c>
+      <c r="E53" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="F53" s="16"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17">
+        <v>0.111</v>
+      </c>
       <c r="I53" s="17"/>
-      <c r="J53" s="18"/>
+      <c r="J53" s="17"/>
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
-      <c r="M53" s="20"/>
-      <c r="N53" s="29"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="20"/>
       <c r="O53" s="29"/>
       <c r="P53" s="29"/>
       <c r="Q53" s="29"/>
       <c r="R53" s="29"/>
       <c r="S53" s="29"/>
-      <c r="T53" s="29"/>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T53" s="29">
+        <v>1.25</v>
+      </c>
+      <c r="V53" s="29"/>
+      <c r="W53" s="29"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>73</v>
+        <v>212</v>
       </c>
       <c r="B54" s="16"/>
       <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
+      <c r="D54" s="16">
+        <v>20</v>
+      </c>
       <c r="E54" s="16"/>
       <c r="F54" s="16"/>
       <c r="G54" s="16">
-        <v>1.5</v>
+        <v>25</v>
       </c>
       <c r="H54" s="16"/>
       <c r="I54" s="16"/>
-      <c r="J54" s="18"/>
+      <c r="J54" s="16"/>
       <c r="K54" s="18"/>
-      <c r="L54" s="18"/>
+      <c r="L54" s="18">
+        <v>35</v>
+      </c>
       <c r="M54" s="18"/>
-      <c r="N54" s="29"/>
-      <c r="O54" s="29"/>
-      <c r="P54" s="29"/>
+      <c r="N54" s="18"/>
+      <c r="O54" s="29">
+        <v>75</v>
+      </c>
+      <c r="P54" s="29">
+        <v>1380</v>
+      </c>
       <c r="Q54" s="29"/>
       <c r="R54" s="29"/>
-      <c r="S54" s="29">
-        <v>5</v>
-      </c>
-      <c r="T54" s="29"/>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S54" s="29"/>
+      <c r="T54" s="29">
+        <v>250</v>
+      </c>
+      <c r="V54" s="29">
+        <v>600</v>
+      </c>
+      <c r="W54" s="29">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
       <c r="F55" s="16"/>
-      <c r="G55" s="16">
+      <c r="G55" s="16"/>
+      <c r="H55" s="16">
         <v>5</v>
       </c>
-      <c r="H55" s="16"/>
       <c r="I55" s="16"/>
-      <c r="J55" s="18"/>
+      <c r="J55" s="16"/>
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
       <c r="M55" s="18"/>
-      <c r="N55" s="29"/>
+      <c r="N55" s="18"/>
       <c r="O55" s="29"/>
       <c r="P55" s="29"/>
       <c r="Q55" s="29"/>
       <c r="R55" s="29"/>
       <c r="S55" s="29"/>
       <c r="T55" s="29"/>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V55" s="29"/>
+      <c r="W55" s="29"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
@@ -3205,135 +3339,148 @@
       <c r="G56" s="16"/>
       <c r="H56" s="16"/>
       <c r="I56" s="16"/>
-      <c r="J56" s="18"/>
+      <c r="J56" s="16"/>
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
-      <c r="M56" s="19"/>
-      <c r="N56" s="29"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="19"/>
       <c r="O56" s="29"/>
       <c r="P56" s="29"/>
       <c r="Q56" s="29"/>
       <c r="R56" s="29"/>
       <c r="S56" s="29"/>
       <c r="T56" s="29"/>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V56" s="29"/>
+      <c r="W56" s="29"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B57" s="16"/>
-      <c r="C57" s="16">
+      <c r="C57" s="16"/>
+      <c r="D57" s="16">
         <v>14</v>
       </c>
-      <c r="D57" s="16"/>
       <c r="E57" s="16"/>
-      <c r="F57" s="17">
+      <c r="F57" s="16"/>
+      <c r="G57" s="17">
         <v>18</v>
       </c>
-      <c r="G57" s="17">
+      <c r="H57" s="17">
         <v>28</v>
       </c>
-      <c r="H57" s="17"/>
       <c r="I57" s="17"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18">
+      <c r="J57" s="17"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18">
         <v>23</v>
       </c>
-      <c r="L57" s="18"/>
-      <c r="M57" s="20"/>
-      <c r="N57" s="29">
+      <c r="M57" s="18"/>
+      <c r="N57" s="20"/>
+      <c r="O57" s="29">
         <v>20</v>
       </c>
-      <c r="O57" s="23">
+      <c r="P57" s="23">
         <v>35</v>
       </c>
-      <c r="P57" s="29"/>
       <c r="Q57" s="29"/>
-      <c r="R57" s="29">
+      <c r="R57" s="29"/>
+      <c r="S57" s="29">
         <v>35</v>
       </c>
-      <c r="S57" s="29"/>
       <c r="T57" s="29">
+        <v>46</v>
+      </c>
+      <c r="V57" s="29"/>
+      <c r="W57" s="29">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="16"/>
+        <v>259</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
-      <c r="F58" s="17">
-        <v>20</v>
-      </c>
+      <c r="F58" s="16"/>
       <c r="G58" s="17">
         <v>20</v>
       </c>
-      <c r="H58" s="17"/>
+      <c r="H58" s="17">
+        <v>20</v>
+      </c>
       <c r="I58" s="17"/>
-      <c r="J58" s="18"/>
-      <c r="K58" s="18">
+      <c r="J58" s="17"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18">
         <v>15</v>
       </c>
-      <c r="L58" s="18">
+      <c r="M58" s="18">
         <v>18</v>
       </c>
-      <c r="M58" s="23"/>
-      <c r="N58" s="29"/>
+      <c r="N58" s="23"/>
       <c r="O58" s="29"/>
       <c r="P58" s="29"/>
       <c r="Q58" s="29"/>
       <c r="R58" s="29"/>
       <c r="S58" s="29"/>
       <c r="T58" s="29"/>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V58" s="29"/>
+      <c r="W58" s="29"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C59" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D59" s="14"/>
+        <v>76</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>76</v>
+      </c>
       <c r="E59" s="14"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="H59" s="15"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="I59" s="15"/>
       <c r="J59" s="15"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
-      <c r="N59" t="s">
-        <v>113</v>
-      </c>
+      <c r="N59" s="15"/>
       <c r="O59" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>120</v>
-      </c>
-      <c r="S59" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="P59" t="s">
+        <v>105</v>
+      </c>
+      <c r="R59" t="s">
+        <v>110</v>
+      </c>
+      <c r="V59" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B60" s="14"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="15"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="14"/>
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
@@ -3341,14 +3488,15 @@
       <c r="J60" s="15"/>
       <c r="K60" s="15"/>
       <c r="L60" s="15"/>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M60" s="15"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
-      <c r="D61" s="15"/>
+      <c r="D61" s="14"/>
       <c r="E61" s="15"/>
       <c r="F61" s="15"/>
       <c r="G61" s="15"/>
@@ -3357,212 +3505,213 @@
       <c r="J61" s="15"/>
       <c r="K61" s="15"/>
       <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
     </row>
     <row r="67" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
+        <v>120</v>
+      </c>
+      <c r="C67" t="s">
+        <v>127</v>
+      </c>
+      <c r="D67" t="s">
         <v>130</v>
       </c>
-      <c r="C67" t="s">
+      <c r="E67" t="s">
+        <v>133</v>
+      </c>
+      <c r="F67" t="s">
+        <v>135</v>
+      </c>
+      <c r="G67" t="s">
         <v>137</v>
       </c>
-      <c r="D67" t="s">
-        <v>140</v>
-      </c>
-      <c r="E67" t="s">
-        <v>143</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="H67" t="s">
+        <v>139</v>
+      </c>
+      <c r="J67" t="s">
+        <v>141</v>
+      </c>
+      <c r="K67" t="s">
         <v>145</v>
       </c>
-      <c r="G67" t="s">
+      <c r="L67" t="s">
+        <v>149</v>
+      </c>
+      <c r="M67" t="s">
         <v>147</v>
       </c>
-      <c r="H67" t="s">
-        <v>149</v>
-      </c>
-      <c r="J67" t="s">
+      <c r="N67" t="s">
         <v>151</v>
       </c>
-      <c r="K67" t="s">
+      <c r="O67" t="s">
+        <v>153</v>
+      </c>
+      <c r="P67" t="s">
         <v>155</v>
       </c>
-      <c r="L67" t="s">
-        <v>159</v>
-      </c>
-      <c r="M67" t="s">
+      <c r="R67" t="s">
         <v>157</v>
       </c>
-      <c r="N67" t="s">
-        <v>161</v>
-      </c>
-      <c r="O67" t="s">
-        <v>163</v>
-      </c>
-      <c r="P67" t="s">
+      <c r="S67" t="s">
+        <v>162</v>
+      </c>
+      <c r="T67" t="s">
         <v>165</v>
       </c>
-      <c r="R67" t="s">
+      <c r="U67" t="s">
         <v>167</v>
       </c>
-      <c r="S67" t="s">
-        <v>172</v>
-      </c>
-      <c r="T67" t="s">
+      <c r="V67" t="s">
+        <v>169</v>
+      </c>
+      <c r="W67" t="s">
+        <v>171</v>
+      </c>
+      <c r="X67" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z67" t="s">
         <v>175</v>
       </c>
-      <c r="U67" t="s">
-        <v>177</v>
-      </c>
-      <c r="V67" t="s">
-        <v>179</v>
-      </c>
-      <c r="W67" t="s">
-        <v>181</v>
-      </c>
-      <c r="X67" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z67" t="s">
-        <v>185</v>
-      </c>
       <c r="AA67" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>180</v>
+      </c>
+      <c r="AC67" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD67" t="s">
+        <v>184</v>
+      </c>
+      <c r="AE67" t="s">
+        <v>186</v>
+      </c>
+      <c r="AF67" t="s">
         <v>188</v>
       </c>
-      <c r="AB67" t="s">
-        <v>190</v>
-      </c>
-      <c r="AC67" t="s">
-        <v>192</v>
-      </c>
-      <c r="AD67" t="s">
-        <v>194</v>
-      </c>
-      <c r="AE67" t="s">
+      <c r="AG67" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH67" t="s">
+        <v>193</v>
+      </c>
+      <c r="AI67" t="s">
         <v>196</v>
       </c>
-      <c r="AF67" t="s">
+      <c r="AJ67" t="s">
         <v>198</v>
       </c>
-      <c r="AG67" t="s">
-        <v>201</v>
-      </c>
-      <c r="AH67" t="s">
-        <v>203</v>
-      </c>
-      <c r="AI67" t="s">
-        <v>206</v>
-      </c>
-      <c r="AJ67" t="s">
-        <v>208</v>
-      </c>
       <c r="AL67" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C68" t="s">
+        <v>128</v>
+      </c>
+      <c r="D68" t="s">
+        <v>131</v>
+      </c>
+      <c r="E68" t="s">
+        <v>134</v>
+      </c>
+      <c r="F68" t="s">
+        <v>136</v>
+      </c>
+      <c r="G68" t="s">
         <v>138</v>
       </c>
-      <c r="D68" t="s">
-        <v>141</v>
-      </c>
-      <c r="E68" t="s">
-        <v>144</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="H68" t="s">
+        <v>140</v>
+      </c>
+      <c r="J68" t="s">
+        <v>142</v>
+      </c>
+      <c r="K68" t="s">
         <v>146</v>
       </c>
-      <c r="G68" t="s">
+      <c r="L68" t="s">
         <v>148</v>
       </c>
-      <c r="H68" t="s">
+      <c r="M68" t="s">
         <v>150</v>
       </c>
-      <c r="J68" t="s">
+      <c r="N68" t="s">
         <v>152</v>
       </c>
-      <c r="K68" t="s">
+      <c r="O68" t="s">
+        <v>154</v>
+      </c>
+      <c r="P68" t="s">
         <v>156</v>
       </c>
-      <c r="L68" t="s">
+      <c r="R68" t="s">
         <v>158</v>
       </c>
-      <c r="M68" t="s">
-        <v>160</v>
-      </c>
-      <c r="N68" t="s">
-        <v>162</v>
-      </c>
-      <c r="O68" t="s">
-        <v>164</v>
-      </c>
-      <c r="P68" t="s">
+      <c r="S68" t="s">
+        <v>163</v>
+      </c>
+      <c r="T68" t="s">
         <v>166</v>
       </c>
-      <c r="R68" t="s">
+      <c r="U68" t="s">
         <v>168</v>
       </c>
-      <c r="S68" t="s">
-        <v>173</v>
-      </c>
-      <c r="T68" t="s">
+      <c r="V68" t="s">
+        <v>115</v>
+      </c>
+      <c r="W68" t="s">
+        <v>172</v>
+      </c>
+      <c r="X68" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z68" t="s">
         <v>176</v>
       </c>
-      <c r="U68" t="s">
-        <v>178</v>
-      </c>
-      <c r="V68" t="s">
-        <v>125</v>
-      </c>
-      <c r="W68" t="s">
-        <v>182</v>
-      </c>
-      <c r="X68" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z68" t="s">
-        <v>186</v>
-      </c>
       <c r="AA68" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC68" t="s">
+        <v>183</v>
+      </c>
+      <c r="AD68" t="s">
+        <v>185</v>
+      </c>
+      <c r="AE68" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF68" t="s">
         <v>189</v>
       </c>
-      <c r="AB68" t="s">
-        <v>191</v>
-      </c>
-      <c r="AC68" t="s">
-        <v>193</v>
-      </c>
-      <c r="AD68" t="s">
-        <v>195</v>
-      </c>
-      <c r="AE68" t="s">
+      <c r="AG68" t="s">
+        <v>192</v>
+      </c>
+      <c r="AH68" t="s">
+        <v>194</v>
+      </c>
+      <c r="AI68" t="s">
         <v>197</v>
       </c>
-      <c r="AF68" t="s">
+      <c r="AJ68" t="s">
         <v>199</v>
       </c>
-      <c r="AG68" t="s">
-        <v>202</v>
-      </c>
-      <c r="AH68" t="s">
-        <v>204</v>
-      </c>
-      <c r="AI68" t="s">
-        <v>207</v>
-      </c>
-      <c r="AJ68" t="s">
-        <v>209</v>
-      </c>
       <c r="AL68" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B70">
         <v>8000</v>
@@ -3637,19 +3786,19 @@
         <v>7000</v>
       </c>
       <c r="AF70" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="AG70" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="AH70" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="AI70">
         <v>3800</v>
       </c>
       <c r="AJ70" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="AL70">
         <v>500</v>
@@ -3657,7 +3806,7 @@
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B71">
         <v>13300</v>
@@ -3740,7 +3889,7 @@
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B72">
         <v>1520</v>
@@ -3823,7 +3972,7 @@
     </row>
     <row r="73" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B73">
         <v>2600</v>
@@ -3906,7 +4055,7 @@
     </row>
     <row r="74" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B74">
         <v>40</v>
@@ -3950,7 +4099,7 @@
     </row>
     <row r="75" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="J75">
         <v>150</v>
@@ -3982,7 +4131,7 @@
     </row>
     <row r="76" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="J76">
         <v>1</v>
@@ -3990,7 +4139,7 @@
     </row>
     <row r="77" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="R77">
         <v>35</v>
@@ -4031,7 +4180,7 @@
     </row>
     <row r="78" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="R78">
         <v>44</v>
@@ -4072,7 +4221,7 @@
     </row>
     <row r="79" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="S79">
         <v>1.5</v>
@@ -4107,7 +4256,7 @@
     </row>
     <row r="80" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="R80">
         <v>2</v>
@@ -4136,7 +4285,7 @@
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="V81">
         <v>5</v>
@@ -4147,135 +4296,135 @@
     </row>
     <row r="82" spans="1:30" x14ac:dyDescent="0.25">
       <c r="Z82" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="AA82" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="AB82" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="AC82" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B87" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C87" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D87" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="E87" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="F87" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="G87" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="H87" t="s">
+        <v>228</v>
+      </c>
+      <c r="I87" t="s">
+        <v>233</v>
+      </c>
+      <c r="J87" t="s">
+        <v>233</v>
+      </c>
+      <c r="K87" t="s">
         <v>238</v>
       </c>
-      <c r="I87" t="s">
-        <v>243</v>
-      </c>
-      <c r="J87" t="s">
-        <v>243</v>
-      </c>
-      <c r="K87" t="s">
-        <v>248</v>
-      </c>
       <c r="L87" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B88" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C88" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D88" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="E88" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="F88" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="G88" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="H88" t="s">
+        <v>229</v>
+      </c>
+      <c r="I88" t="s">
+        <v>234</v>
+      </c>
+      <c r="J88" t="s">
+        <v>234</v>
+      </c>
+      <c r="K88" t="s">
         <v>239</v>
       </c>
-      <c r="I88" t="s">
-        <v>244</v>
-      </c>
-      <c r="J88" t="s">
-        <v>244</v>
-      </c>
-      <c r="K88" t="s">
-        <v>249</v>
-      </c>
       <c r="L88" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B89" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C89" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D89" t="s">
+        <v>220</v>
+      </c>
+      <c r="E89" t="s">
+        <v>220</v>
+      </c>
+      <c r="F89" t="s">
+        <v>224</v>
+      </c>
+      <c r="G89" t="s">
+        <v>224</v>
+      </c>
+      <c r="H89" t="s">
         <v>230</v>
       </c>
-      <c r="E89" t="s">
-        <v>230</v>
-      </c>
-      <c r="F89" t="s">
-        <v>234</v>
-      </c>
-      <c r="G89" t="s">
-        <v>234</v>
-      </c>
-      <c r="H89" t="s">
+      <c r="I89" t="s">
+        <v>235</v>
+      </c>
+      <c r="J89" t="s">
+        <v>235</v>
+      </c>
+      <c r="K89" t="s">
         <v>240</v>
       </c>
-      <c r="I89" t="s">
-        <v>245</v>
-      </c>
-      <c r="J89" t="s">
-        <v>245</v>
-      </c>
-      <c r="K89" t="s">
-        <v>250</v>
-      </c>
       <c r="L89" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B90">
         <v>500</v>
@@ -4304,7 +4453,7 @@
     </row>
     <row r="92" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B92">
         <v>2880</v>
@@ -4333,7 +4482,7 @@
     </row>
     <row r="93" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B93">
         <v>360</v>
@@ -4362,7 +4511,7 @@
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B94">
         <v>1440</v>
@@ -4391,7 +4540,7 @@
     </row>
     <row r="96" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B96">
         <v>6</v>
@@ -4420,45 +4569,45 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
+        <v>227</v>
+      </c>
+      <c r="E97" t="s">
+        <v>226</v>
+      </c>
+      <c r="F97" t="s">
+        <v>225</v>
+      </c>
+      <c r="G97" t="s">
+        <v>231</v>
+      </c>
+      <c r="H97" t="s">
+        <v>232</v>
+      </c>
+      <c r="I97" t="s">
+        <v>236</v>
+      </c>
+      <c r="J97" t="s">
         <v>237</v>
       </c>
-      <c r="E97" t="s">
-        <v>236</v>
-      </c>
-      <c r="F97" t="s">
-        <v>235</v>
-      </c>
-      <c r="G97" t="s">
-        <v>241</v>
-      </c>
-      <c r="H97" t="s">
-        <v>242</v>
-      </c>
-      <c r="I97" t="s">
+      <c r="K97" t="s">
+        <v>225</v>
+      </c>
+      <c r="L97" t="s">
+        <v>227</v>
+      </c>
+      <c r="M97" t="s">
         <v>246</v>
       </c>
-      <c r="J97" t="s">
-        <v>247</v>
-      </c>
-      <c r="K97" t="s">
-        <v>235</v>
-      </c>
-      <c r="L97" t="s">
-        <v>237</v>
-      </c>
-      <c r="M97" t="s">
-        <v>256</v>
-      </c>
       <c r="N97" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="O97" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B98">
         <v>25</v>
@@ -4505,7 +4654,7 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -4549,7 +4698,7 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B100">
         <v>2</v>
@@ -4596,7 +4745,7 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B101">
         <v>32</v>
@@ -4643,7 +4792,7 @@
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B102">
         <v>0.83299999999999996</v>
@@ -4690,7 +4839,7 @@
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B103">
         <v>41.6</v>
@@ -4699,7 +4848,7 @@
         <v>60</v>
       </c>
       <c r="D103" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E103">
         <v>50</v>
@@ -4737,16 +4886,16 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D105" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="J105" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="L105" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rouge + bulfrog + acu
Bullfrog - veterancy regen + regen optimalization

rouge - nerf dps was think that it was litle bit too strong, so rather
have it weak as op

ACU
-- oc is big problem so hot fix is reduce number of shots, and decrese
aoe but will need make proper fix, best is get get back and move into
capacitator funciton
-- change muzzle to acu to fit into fa
-- change rof to have 100dps insted of 88
decrese hp whie it still too strong (problem with gun that half rof
while now its 1,5:2=0,75=0,8=>187,5dps insted of 200.   Have number for
new gun but it will be later. this is kinda hot fix.
fix all upgrade values to fit into faf patches.  But some of them will
be changed later.
</commit_message>
<xml_diff>
--- a/Units.xlsx
+++ b/Units.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="275">
   <si>
     <t>Stats</t>
   </si>
@@ -330,9 +330,6 @@
     <t>Beamer</t>
   </si>
   <si>
-    <t>artilery suport</t>
-  </si>
-  <si>
     <t>transportable</t>
   </si>
   <si>
@@ -348,9 +345,6 @@
     <t>Nova</t>
   </si>
   <si>
-    <t>arti suport</t>
-  </si>
-  <si>
     <t>inu3003</t>
   </si>
   <si>
@@ -838,6 +832,18 @@
   </si>
   <si>
     <t>20/140</t>
+  </si>
+  <si>
+    <t>inb1101</t>
+  </si>
+  <si>
+    <t>t1pgen</t>
+  </si>
+  <si>
+    <t>teoreticky zmenit rof na 4s ako obsidian = 100x3=300dmg/4s =&gt; 75dps</t>
+  </si>
+  <si>
+    <t>bombard</t>
   </si>
 </sst>
 </file>
@@ -1519,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection activeCell="A73" sqref="A73"/>
       <selection pane="topRight" activeCell="S47" sqref="S47"/>
     </sheetView>
@@ -1577,19 +1583,19 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F5" t="s">
         <v>200</v>
-      </c>
-      <c r="D5" t="s">
-        <v>199</v>
-      </c>
-      <c r="E5" t="s">
-        <v>246</v>
-      </c>
-      <c r="F5" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1630,7 +1636,7 @@
         <v>37</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>43</v>
@@ -2411,7 +2417,7 @@
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
@@ -2428,12 +2434,12 @@
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>15</v>
       </c>
@@ -2448,7 +2454,7 @@
       </c>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>19</v>
       </c>
@@ -2463,31 +2469,31 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J38" t="s">
         <v>87</v>
@@ -2508,33 +2514,36 @@
         <v>100</v>
       </c>
       <c r="Q38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S38" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="T38" t="s">
-        <v>249</v>
+        <v>108</v>
       </c>
       <c r="U38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="V38" t="s">
-        <v>113</v>
+        <v>246</v>
       </c>
       <c r="W38" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="X38" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>76</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C39" s="21" t="s">
         <v>21</v>
@@ -2543,10 +2552,10 @@
         <v>77</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G39" s="22" t="s">
         <v>78</v>
@@ -2555,10 +2564,10 @@
         <v>79</v>
       </c>
       <c r="I39" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="J39" s="22" t="s">
         <v>261</v>
-      </c>
-      <c r="J39" s="22" t="s">
-        <v>263</v>
       </c>
       <c r="K39" s="27"/>
       <c r="L39" s="27" t="s">
@@ -2577,28 +2586,31 @@
         <v>101</v>
       </c>
       <c r="Q39" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R39" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S39" s="22" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="T39" s="22" t="s">
-        <v>250</v>
+        <v>109</v>
       </c>
       <c r="U39" s="22" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="V39" s="22" t="s">
-        <v>114</v>
+        <v>252</v>
       </c>
       <c r="W39" s="22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="X39" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>61</v>
       </c>
@@ -2607,7 +2619,7 @@
         <v>80</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E40" s="24" t="s">
         <v>84</v>
@@ -2641,25 +2653,28 @@
       </c>
       <c r="Q40" s="15"/>
       <c r="R40" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S40" s="28" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="T40" s="28" t="s">
-        <v>251</v>
+        <v>110</v>
       </c>
       <c r="U40" s="28" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="V40" s="28" t="s">
-        <v>115</v>
+        <v>253</v>
       </c>
       <c r="W40" s="28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="X40" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>62</v>
       </c>
@@ -2704,20 +2719,21 @@
       <c r="R41" s="23">
         <v>640</v>
       </c>
-      <c r="S41" s="23">
+      <c r="S41" s="23"/>
+      <c r="T41" s="23">
         <v>360</v>
       </c>
-      <c r="T41" s="23">
+      <c r="U41" s="23">
         <v>640</v>
       </c>
-      <c r="V41" s="23">
+      <c r="W41" s="23">
         <v>960</v>
       </c>
-      <c r="W41" s="23">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X41" s="23">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>63</v>
       </c>
@@ -2762,20 +2778,21 @@
       <c r="R42" s="23">
         <v>8000</v>
       </c>
-      <c r="S42" s="23">
+      <c r="S42" s="23"/>
+      <c r="T42" s="23">
         <v>1800</v>
       </c>
-      <c r="T42" s="23">
-        <v>6400</v>
-      </c>
-      <c r="V42" s="23">
+      <c r="U42" s="23">
+        <v>8000</v>
+      </c>
+      <c r="W42" s="23">
         <v>9600</v>
       </c>
-      <c r="W42" s="23">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X42" s="23">
+        <v>12800</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>64</v>
       </c>
@@ -2820,20 +2837,21 @@
       <c r="R43" s="23">
         <v>640</v>
       </c>
-      <c r="S43" s="23">
+      <c r="S43" s="23"/>
+      <c r="T43" s="23">
         <v>1600</v>
       </c>
-      <c r="T43" s="23">
+      <c r="U43" s="23">
         <v>3200</v>
       </c>
-      <c r="V43" s="23">
+      <c r="W43" s="23">
         <v>5000</v>
       </c>
-      <c r="W43" s="23">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X43" s="23">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>65</v>
       </c>
@@ -2880,10 +2898,11 @@
       <c r="R44" s="29"/>
       <c r="S44" s="29"/>
       <c r="T44" s="29"/>
-      <c r="V44" s="29"/>
+      <c r="U44" s="29"/>
       <c r="W44" s="29"/>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X44" s="29"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>66</v>
       </c>
@@ -2927,10 +2946,11 @@
       <c r="R45" s="29"/>
       <c r="S45" s="29"/>
       <c r="T45" s="29"/>
-      <c r="V45" s="29"/>
+      <c r="U45" s="29"/>
       <c r="W45" s="29"/>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X45" s="29"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>67</v>
       </c>
@@ -2974,10 +2994,11 @@
       <c r="R46" s="29"/>
       <c r="S46" s="29"/>
       <c r="T46" s="29"/>
-      <c r="V46" s="29"/>
+      <c r="U46" s="29"/>
       <c r="W46" s="29"/>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X46" s="29"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>68</v>
       </c>
@@ -3000,10 +3021,11 @@
       <c r="R47" s="29"/>
       <c r="S47" s="29"/>
       <c r="T47" s="29"/>
-      <c r="V47" s="29"/>
+      <c r="U47" s="29"/>
       <c r="W47" s="29"/>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X47" s="29"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>7</v>
       </c>
@@ -3043,7 +3065,7 @@
         <v>900</v>
       </c>
       <c r="O48" s="23">
-        <v>1200</v>
+        <v>1250</v>
       </c>
       <c r="P48" s="23">
         <v>30000</v>
@@ -3052,20 +3074,24 @@
       <c r="R48" s="23">
         <v>3500</v>
       </c>
-      <c r="S48" s="23">
+      <c r="S48" s="23"/>
+      <c r="T48" s="23">
         <v>3000</v>
       </c>
-      <c r="T48" s="23">
-        <v>2200</v>
+      <c r="U48" s="23">
+        <v>1800</v>
       </c>
       <c r="V48" s="23">
+        <v>860</v>
+      </c>
+      <c r="W48" s="23">
         <v>1600</v>
       </c>
-      <c r="W48" s="23">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X48" s="23">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>9</v>
       </c>
@@ -3104,27 +3130,31 @@
       </c>
       <c r="Q49" s="29"/>
       <c r="R49" s="23">
-        <v>3.75</v>
-      </c>
-      <c r="S49" s="29">
+        <v>3.2</v>
+      </c>
+      <c r="S49" s="23"/>
+      <c r="T49" s="29">
         <v>2.7</v>
       </c>
-      <c r="T49" s="23">
+      <c r="U49" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="V49" s="29">
+        <v>3.5</v>
+      </c>
+      <c r="W49" s="23">
+        <v>2.5</v>
+      </c>
+      <c r="X49" s="29">
         <v>3</v>
       </c>
-      <c r="V49" s="23">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="W49" s="29">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C50" s="16"/>
       <c r="D50" s="16">
@@ -3141,33 +3171,44 @@
         <v>300</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J50" s="17" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
+      <c r="L50" s="18">
+        <v>8</v>
+      </c>
       <c r="M50" s="18">
         <v>200</v>
       </c>
       <c r="N50" s="19"/>
-      <c r="O50" s="29"/>
+      <c r="O50" s="29">
+        <v>50</v>
+      </c>
       <c r="P50" s="29"/>
       <c r="Q50" s="29"/>
-      <c r="R50" s="29"/>
-      <c r="S50" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="T50" s="29">
+      <c r="R50" s="29">
+        <v>100</v>
+      </c>
+      <c r="S50" s="29">
+        <v>300</v>
+      </c>
+      <c r="T50" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="U50" s="29">
         <v>200</v>
       </c>
-      <c r="V50" s="29"/>
       <c r="W50" s="29"/>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X50" s="29">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B51" s="16"/>
       <c r="C51" s="16"/>
@@ -3190,24 +3231,33 @@
         <v>1.75</v>
       </c>
       <c r="N51" s="19"/>
-      <c r="O51" s="29"/>
+      <c r="O51" s="29">
+        <v>0</v>
+      </c>
       <c r="P51" s="29"/>
       <c r="Q51" s="29"/>
-      <c r="R51" s="29"/>
+      <c r="R51" s="29">
+        <v>0</v>
+      </c>
       <c r="S51" s="29">
+        <v>0</v>
+      </c>
+      <c r="T51" s="29">
         <v>1.3</v>
       </c>
-      <c r="T51" s="29">
+      <c r="U51" s="29">
+        <v>1.5</v>
+      </c>
+      <c r="W51" s="29">
+        <v>5</v>
+      </c>
+      <c r="X51" s="29">
         <v>0</v>
       </c>
-      <c r="V51" s="29">
-        <v>5</v>
-      </c>
-      <c r="W51" s="29"/>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B52" s="16"/>
       <c r="C52" s="16"/>
@@ -3225,27 +3275,38 @@
       <c r="I52" s="16"/>
       <c r="J52" s="16"/>
       <c r="K52" s="18"/>
-      <c r="L52" s="18"/>
+      <c r="L52" s="18">
+        <v>1</v>
+      </c>
       <c r="M52" s="18">
         <v>2</v>
       </c>
       <c r="N52" s="18"/>
-      <c r="O52" s="29"/>
+      <c r="O52" s="29">
+        <v>3</v>
+      </c>
       <c r="P52" s="29"/>
       <c r="Q52" s="29"/>
-      <c r="R52" s="29"/>
+      <c r="R52" s="29">
+        <v>4</v>
+      </c>
       <c r="S52" s="29">
         <v>1</v>
       </c>
       <c r="T52" s="29">
         <v>1</v>
       </c>
-      <c r="V52" s="29"/>
+      <c r="U52" s="29">
+        <v>1</v>
+      </c>
       <c r="W52" s="29"/>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X52" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B53" s="16"/>
       <c r="C53" s="16"/>
@@ -3263,27 +3324,38 @@
       <c r="I53" s="17"/>
       <c r="J53" s="17"/>
       <c r="K53" s="18"/>
-      <c r="L53" s="18"/>
+      <c r="L53" s="18">
+        <v>4</v>
+      </c>
       <c r="M53" s="18">
         <v>0.125</v>
       </c>
       <c r="N53" s="20"/>
-      <c r="O53" s="29"/>
+      <c r="O53" s="29">
+        <v>0.5</v>
+      </c>
       <c r="P53" s="29"/>
       <c r="Q53" s="29"/>
-      <c r="R53" s="29"/>
+      <c r="R53" s="29">
+        <v>0.25</v>
+      </c>
       <c r="S53" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="T53" s="29">
         <v>0.76900000000000002</v>
       </c>
-      <c r="T53" s="29">
-        <v>1.25</v>
-      </c>
-      <c r="V53" s="29"/>
+      <c r="U53" s="29">
+        <v>1</v>
+      </c>
       <c r="W53" s="29"/>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X53" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B54" s="16"/>
       <c r="C54" s="16"/>
@@ -3300,7 +3372,7 @@
       <c r="J54" s="16"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M54" s="18">
         <v>50</v>
@@ -3313,21 +3385,26 @@
         <v>1380</v>
       </c>
       <c r="Q54" s="29"/>
-      <c r="R54" s="29"/>
-      <c r="S54" s="29"/>
-      <c r="T54" s="29">
-        <v>250</v>
-      </c>
-      <c r="V54" s="29">
+      <c r="R54" s="29">
+        <v>100</v>
+      </c>
+      <c r="S54" s="29">
+        <v>150</v>
+      </c>
+      <c r="T54" s="29"/>
+      <c r="U54" s="29">
+        <v>200</v>
+      </c>
+      <c r="W54" s="29">
         <v>600</v>
       </c>
-      <c r="W54" s="29">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X54" s="29">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
@@ -3343,19 +3420,22 @@
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
       <c r="M55" s="18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="N55" s="18"/>
       <c r="O55" s="29"/>
       <c r="P55" s="29"/>
       <c r="Q55" s="29"/>
-      <c r="R55" s="29"/>
+      <c r="R55" s="29">
+        <v>0.1</v>
+      </c>
       <c r="S55" s="29"/>
       <c r="T55" s="29"/>
-      <c r="V55" s="29"/>
+      <c r="U55" s="29"/>
       <c r="W55" s="29"/>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X55" s="29"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>69</v>
       </c>
@@ -3380,10 +3460,11 @@
       <c r="R56" s="29"/>
       <c r="S56" s="29"/>
       <c r="T56" s="29"/>
-      <c r="V56" s="29"/>
+      <c r="U56" s="29"/>
       <c r="W56" s="29"/>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X56" s="29"/>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>70</v>
       </c>
@@ -3417,24 +3498,29 @@
         <v>35</v>
       </c>
       <c r="Q57" s="29"/>
-      <c r="R57" s="29"/>
+      <c r="R57" s="29">
+        <v>23</v>
+      </c>
       <c r="S57" s="29">
+        <v>26</v>
+      </c>
+      <c r="T57" s="29">
         <v>35</v>
       </c>
-      <c r="T57" s="29">
+      <c r="U57" s="29">
         <v>46</v>
       </c>
-      <c r="V57" s="29"/>
-      <c r="W57" s="29">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W57" s="29"/>
+      <c r="X57" s="29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>83</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>81</v>
@@ -3464,10 +3550,11 @@
       <c r="R58" s="29"/>
       <c r="S58" s="29"/>
       <c r="T58" s="29"/>
-      <c r="V58" s="29"/>
+      <c r="U58" s="29"/>
       <c r="W58" s="29"/>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X58" s="29"/>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>71</v>
       </c>
@@ -3490,27 +3577,31 @@
       <c r="J59" s="15"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
-      <c r="M59" s="15"/>
+      <c r="M59" s="15" t="s">
+        <v>86</v>
+      </c>
       <c r="N59" s="15"/>
-      <c r="O59" t="s">
+      <c r="P59" t="s">
         <v>103</v>
       </c>
-      <c r="P59" t="s">
-        <v>104</v>
-      </c>
-      <c r="R59" t="s">
-        <v>109</v>
-      </c>
-      <c r="V59" t="s">
+      <c r="T59" t="s">
+        <v>274</v>
+      </c>
+      <c r="U59" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W59" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>72</v>
       </c>
       <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
+      <c r="C60" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="D60" s="15"/>
       <c r="E60" s="14"/>
       <c r="F60" s="15"/>
@@ -3522,7 +3613,7 @@
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>73</v>
       </c>
@@ -3539,211 +3630,222 @@
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
     </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="O62" t="s">
+        <v>273</v>
+      </c>
+    </row>
     <row r="67" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
+        <v>117</v>
+      </c>
+      <c r="C67" t="s">
+        <v>124</v>
+      </c>
+      <c r="D67" t="s">
+        <v>127</v>
+      </c>
+      <c r="E67" t="s">
+        <v>130</v>
+      </c>
+      <c r="F67" t="s">
+        <v>132</v>
+      </c>
+      <c r="G67" t="s">
+        <v>134</v>
+      </c>
+      <c r="H67" t="s">
+        <v>136</v>
+      </c>
+      <c r="I67" t="s">
+        <v>271</v>
+      </c>
+      <c r="J67" t="s">
+        <v>138</v>
+      </c>
+      <c r="K67" t="s">
+        <v>142</v>
+      </c>
+      <c r="L67" t="s">
+        <v>146</v>
+      </c>
+      <c r="M67" t="s">
+        <v>144</v>
+      </c>
+      <c r="N67" t="s">
+        <v>148</v>
+      </c>
+      <c r="O67" t="s">
+        <v>150</v>
+      </c>
+      <c r="P67" t="s">
+        <v>152</v>
+      </c>
+      <c r="R67" t="s">
+        <v>154</v>
+      </c>
+      <c r="S67" t="s">
+        <v>159</v>
+      </c>
+      <c r="T67" t="s">
+        <v>162</v>
+      </c>
+      <c r="U67" t="s">
+        <v>164</v>
+      </c>
+      <c r="V67" t="s">
+        <v>166</v>
+      </c>
+      <c r="W67" t="s">
+        <v>168</v>
+      </c>
+      <c r="X67" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA67" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC67" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD67" t="s">
+        <v>181</v>
+      </c>
+      <c r="AE67" t="s">
+        <v>183</v>
+      </c>
+      <c r="AF67" t="s">
+        <v>185</v>
+      </c>
+      <c r="AG67" t="s">
+        <v>188</v>
+      </c>
+      <c r="AH67" t="s">
+        <v>190</v>
+      </c>
+      <c r="AI67" t="s">
+        <v>193</v>
+      </c>
+      <c r="AJ67" t="s">
+        <v>195</v>
+      </c>
+      <c r="AL67" t="s">
         <v>119</v>
-      </c>
-      <c r="C67" t="s">
-        <v>126</v>
-      </c>
-      <c r="D67" t="s">
-        <v>129</v>
-      </c>
-      <c r="E67" t="s">
-        <v>132</v>
-      </c>
-      <c r="F67" t="s">
-        <v>134</v>
-      </c>
-      <c r="G67" t="s">
-        <v>136</v>
-      </c>
-      <c r="H67" t="s">
-        <v>138</v>
-      </c>
-      <c r="J67" t="s">
-        <v>140</v>
-      </c>
-      <c r="K67" t="s">
-        <v>144</v>
-      </c>
-      <c r="L67" t="s">
-        <v>148</v>
-      </c>
-      <c r="M67" t="s">
-        <v>146</v>
-      </c>
-      <c r="N67" t="s">
-        <v>150</v>
-      </c>
-      <c r="O67" t="s">
-        <v>152</v>
-      </c>
-      <c r="P67" t="s">
-        <v>154</v>
-      </c>
-      <c r="R67" t="s">
-        <v>156</v>
-      </c>
-      <c r="S67" t="s">
-        <v>161</v>
-      </c>
-      <c r="T67" t="s">
-        <v>164</v>
-      </c>
-      <c r="U67" t="s">
-        <v>166</v>
-      </c>
-      <c r="V67" t="s">
-        <v>168</v>
-      </c>
-      <c r="W67" t="s">
-        <v>170</v>
-      </c>
-      <c r="X67" t="s">
-        <v>172</v>
-      </c>
-      <c r="Z67" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA67" t="s">
-        <v>177</v>
-      </c>
-      <c r="AB67" t="s">
-        <v>179</v>
-      </c>
-      <c r="AC67" t="s">
-        <v>181</v>
-      </c>
-      <c r="AD67" t="s">
-        <v>183</v>
-      </c>
-      <c r="AE67" t="s">
-        <v>185</v>
-      </c>
-      <c r="AF67" t="s">
-        <v>187</v>
-      </c>
-      <c r="AG67" t="s">
-        <v>190</v>
-      </c>
-      <c r="AH67" t="s">
-        <v>192</v>
-      </c>
-      <c r="AI67" t="s">
-        <v>195</v>
-      </c>
-      <c r="AJ67" t="s">
-        <v>197</v>
-      </c>
-      <c r="AL67" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
+        <v>126</v>
+      </c>
+      <c r="C68" t="s">
+        <v>125</v>
+      </c>
+      <c r="D68" t="s">
         <v>128</v>
       </c>
-      <c r="C68" t="s">
-        <v>127</v>
-      </c>
-      <c r="D68" t="s">
-        <v>130</v>
-      </c>
       <c r="E68" t="s">
+        <v>131</v>
+      </c>
+      <c r="F68" t="s">
         <v>133</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>135</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>137</v>
       </c>
-      <c r="H68" t="s">
+      <c r="I68" t="s">
+        <v>272</v>
+      </c>
+      <c r="J68" t="s">
         <v>139</v>
       </c>
-      <c r="J68" t="s">
-        <v>141</v>
-      </c>
       <c r="K68" t="s">
+        <v>143</v>
+      </c>
+      <c r="L68" t="s">
         <v>145</v>
       </c>
-      <c r="L68" t="s">
+      <c r="M68" t="s">
         <v>147</v>
       </c>
-      <c r="M68" t="s">
+      <c r="N68" t="s">
         <v>149</v>
       </c>
-      <c r="N68" t="s">
+      <c r="O68" t="s">
         <v>151</v>
       </c>
-      <c r="O68" t="s">
+      <c r="P68" t="s">
         <v>153</v>
       </c>
-      <c r="P68" t="s">
+      <c r="R68" t="s">
         <v>155</v>
       </c>
-      <c r="R68" t="s">
-        <v>157</v>
-      </c>
       <c r="S68" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="T68" t="s">
+        <v>163</v>
+      </c>
+      <c r="U68" t="s">
         <v>165</v>
       </c>
-      <c r="U68" t="s">
-        <v>167</v>
-      </c>
       <c r="V68" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="W68" t="s">
+        <v>169</v>
+      </c>
+      <c r="X68" t="s">
         <v>171</v>
       </c>
-      <c r="X68" t="s">
+      <c r="Z68" t="s">
         <v>173</v>
       </c>
-      <c r="Z68" t="s">
-        <v>175</v>
-      </c>
       <c r="AA68" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB68" t="s">
         <v>178</v>
       </c>
-      <c r="AB68" t="s">
+      <c r="AC68" t="s">
         <v>180</v>
       </c>
-      <c r="AC68" t="s">
+      <c r="AD68" t="s">
         <v>182</v>
       </c>
-      <c r="AD68" t="s">
+      <c r="AE68" t="s">
         <v>184</v>
       </c>
-      <c r="AE68" t="s">
+      <c r="AF68" t="s">
         <v>186</v>
       </c>
-      <c r="AF68" t="s">
-        <v>188</v>
-      </c>
       <c r="AG68" t="s">
+        <v>189</v>
+      </c>
+      <c r="AH68" t="s">
         <v>191</v>
       </c>
-      <c r="AH68" t="s">
-        <v>193</v>
-      </c>
       <c r="AI68" t="s">
+        <v>194</v>
+      </c>
+      <c r="AJ68" t="s">
         <v>196</v>
       </c>
-      <c r="AJ68" t="s">
-        <v>198</v>
-      </c>
       <c r="AL68" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B70">
         <v>8000</v>
@@ -3818,19 +3920,19 @@
         <v>7000</v>
       </c>
       <c r="AF70" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AG70" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AH70" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AI70">
         <v>3800</v>
       </c>
       <c r="AJ70" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AL70">
         <v>500</v>
@@ -3838,7 +3940,7 @@
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B71">
         <v>13300</v>
@@ -3921,7 +4023,7 @@
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B72">
         <v>1520</v>
@@ -4004,7 +4106,7 @@
     </row>
     <row r="73" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B73">
         <v>2600</v>
@@ -4087,7 +4189,7 @@
     </row>
     <row r="74" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B74">
         <v>40</v>
@@ -4131,7 +4233,7 @@
     </row>
     <row r="75" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J75">
         <v>150</v>
@@ -4163,7 +4265,7 @@
     </row>
     <row r="76" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J76">
         <v>1</v>
@@ -4171,7 +4273,7 @@
     </row>
     <row r="77" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="R77">
         <v>35</v>
@@ -4212,7 +4314,7 @@
     </row>
     <row r="78" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="R78">
         <v>44</v>
@@ -4253,7 +4355,7 @@
     </row>
     <row r="79" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S79">
         <v>1.5</v>
@@ -4288,7 +4390,7 @@
     </row>
     <row r="80" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="R80">
         <v>2</v>
@@ -4317,7 +4419,7 @@
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="V81">
         <v>5</v>
@@ -4328,135 +4430,135 @@
     </row>
     <row r="82" spans="1:30" x14ac:dyDescent="0.25">
       <c r="Z82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AA82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AB82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AC82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B87" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C87" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D87" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E87" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F87" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G87" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H87" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I87" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J87" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K87" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L87" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B88" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C88" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D88" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E88" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F88" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G88" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H88" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I88" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J88" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K88" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L88" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B89" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C89" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D89" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E89" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F89" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G89" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H89" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I89" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J89" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K89" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L89" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B90">
         <v>500</v>
@@ -4485,7 +4587,7 @@
     </row>
     <row r="92" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B92">
         <v>2880</v>
@@ -4514,7 +4616,7 @@
     </row>
     <row r="93" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B93">
         <v>360</v>
@@ -4543,7 +4645,7 @@
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B94">
         <v>1440</v>
@@ -4572,7 +4674,7 @@
     </row>
     <row r="96" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B96">
         <v>6</v>
@@ -4601,45 +4703,45 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E97" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F97" t="s">
+        <v>222</v>
+      </c>
+      <c r="G97" t="s">
+        <v>228</v>
+      </c>
+      <c r="H97" t="s">
+        <v>229</v>
+      </c>
+      <c r="I97" t="s">
+        <v>233</v>
+      </c>
+      <c r="J97" t="s">
+        <v>234</v>
+      </c>
+      <c r="K97" t="s">
+        <v>222</v>
+      </c>
+      <c r="L97" t="s">
         <v>224</v>
       </c>
-      <c r="G97" t="s">
-        <v>230</v>
-      </c>
-      <c r="H97" t="s">
-        <v>231</v>
-      </c>
-      <c r="I97" t="s">
-        <v>235</v>
-      </c>
-      <c r="J97" t="s">
-        <v>236</v>
-      </c>
-      <c r="K97" t="s">
-        <v>224</v>
-      </c>
-      <c r="L97" t="s">
-        <v>226</v>
-      </c>
       <c r="M97" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="N97" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="O97" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B98">
         <v>25</v>
@@ -4686,7 +4788,7 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -4730,7 +4832,7 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B100">
         <v>2</v>
@@ -4777,7 +4879,7 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B101">
         <v>32</v>
@@ -4824,7 +4926,7 @@
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B102">
         <v>0.83299999999999996</v>
@@ -4871,7 +4973,7 @@
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B103">
         <v>41.6</v>
@@ -4880,7 +4982,7 @@
         <v>60</v>
       </c>
       <c r="D103" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E103">
         <v>50</v>
@@ -4918,16 +5020,16 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D105" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J105" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L105" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
balance adjustments for rouge, bulfrog and acu to normalize the values to FAF standards
Bullfrog - veterancy regen + regen optimalization

rouge - nerf dps was think that it was litle bit too strong, so rather
have it weak as op

ACU
-- oc is big problem so hot fix is reduce number of shots, and decrese
aoe but will need make proper fix, best is get get back and move into
capacitator funciton
-- change muzzle to acu to fit into fa
-- change rof to have 100dps insted of 88
decrese hp whie it still too strong (problem with gun that half rof
while now its 1,5:2=0,75=0,8=>187,5dps insted of 200.   Have number for
new gun but it will be later. this is kinda hot fix.
fix all upgrade values to fit into faf patches.  But some of them will
be changed later.
</commit_message>
<xml_diff>
--- a/Units.xlsx
+++ b/Units.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="275">
   <si>
     <t>Stats</t>
   </si>
@@ -330,9 +330,6 @@
     <t>Beamer</t>
   </si>
   <si>
-    <t>artilery suport</t>
-  </si>
-  <si>
     <t>transportable</t>
   </si>
   <si>
@@ -348,9 +345,6 @@
     <t>Nova</t>
   </si>
   <si>
-    <t>arti suport</t>
-  </si>
-  <si>
     <t>inu3003</t>
   </si>
   <si>
@@ -838,6 +832,18 @@
   </si>
   <si>
     <t>20/140</t>
+  </si>
+  <si>
+    <t>inb1101</t>
+  </si>
+  <si>
+    <t>t1pgen</t>
+  </si>
+  <si>
+    <t>teoreticky zmenit rof na 4s ako obsidian = 100x3=300dmg/4s =&gt; 75dps</t>
+  </si>
+  <si>
+    <t>bombard</t>
   </si>
 </sst>
 </file>
@@ -1519,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection activeCell="A73" sqref="A73"/>
       <selection pane="topRight" activeCell="S47" sqref="S47"/>
     </sheetView>
@@ -1577,19 +1583,19 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F5" t="s">
         <v>200</v>
-      </c>
-      <c r="D5" t="s">
-        <v>199</v>
-      </c>
-      <c r="E5" t="s">
-        <v>246</v>
-      </c>
-      <c r="F5" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1630,7 +1636,7 @@
         <v>37</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>43</v>
@@ -2411,7 +2417,7 @@
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
@@ -2428,12 +2434,12 @@
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>15</v>
       </c>
@@ -2448,7 +2454,7 @@
       </c>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>19</v>
       </c>
@@ -2463,31 +2469,31 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J38" t="s">
         <v>87</v>
@@ -2508,33 +2514,36 @@
         <v>100</v>
       </c>
       <c r="Q38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S38" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="T38" t="s">
-        <v>249</v>
+        <v>108</v>
       </c>
       <c r="U38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="V38" t="s">
-        <v>113</v>
+        <v>246</v>
       </c>
       <c r="W38" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="X38" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>76</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C39" s="21" t="s">
         <v>21</v>
@@ -2543,10 +2552,10 @@
         <v>77</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G39" s="22" t="s">
         <v>78</v>
@@ -2555,10 +2564,10 @@
         <v>79</v>
       </c>
       <c r="I39" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="J39" s="22" t="s">
         <v>261</v>
-      </c>
-      <c r="J39" s="22" t="s">
-        <v>263</v>
       </c>
       <c r="K39" s="27"/>
       <c r="L39" s="27" t="s">
@@ -2577,28 +2586,31 @@
         <v>101</v>
       </c>
       <c r="Q39" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R39" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S39" s="22" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="T39" s="22" t="s">
-        <v>250</v>
+        <v>109</v>
       </c>
       <c r="U39" s="22" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="V39" s="22" t="s">
-        <v>114</v>
+        <v>252</v>
       </c>
       <c r="W39" s="22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="X39" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>61</v>
       </c>
@@ -2607,7 +2619,7 @@
         <v>80</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E40" s="24" t="s">
         <v>84</v>
@@ -2641,25 +2653,28 @@
       </c>
       <c r="Q40" s="15"/>
       <c r="R40" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S40" s="28" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="T40" s="28" t="s">
-        <v>251</v>
+        <v>110</v>
       </c>
       <c r="U40" s="28" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="V40" s="28" t="s">
-        <v>115</v>
+        <v>253</v>
       </c>
       <c r="W40" s="28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="X40" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>62</v>
       </c>
@@ -2704,20 +2719,21 @@
       <c r="R41" s="23">
         <v>640</v>
       </c>
-      <c r="S41" s="23">
+      <c r="S41" s="23"/>
+      <c r="T41" s="23">
         <v>360</v>
       </c>
-      <c r="T41" s="23">
+      <c r="U41" s="23">
         <v>640</v>
       </c>
-      <c r="V41" s="23">
+      <c r="W41" s="23">
         <v>960</v>
       </c>
-      <c r="W41" s="23">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X41" s="23">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>63</v>
       </c>
@@ -2762,20 +2778,21 @@
       <c r="R42" s="23">
         <v>8000</v>
       </c>
-      <c r="S42" s="23">
+      <c r="S42" s="23"/>
+      <c r="T42" s="23">
         <v>1800</v>
       </c>
-      <c r="T42" s="23">
-        <v>6400</v>
-      </c>
-      <c r="V42" s="23">
+      <c r="U42" s="23">
+        <v>8000</v>
+      </c>
+      <c r="W42" s="23">
         <v>9600</v>
       </c>
-      <c r="W42" s="23">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X42" s="23">
+        <v>12800</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>64</v>
       </c>
@@ -2820,20 +2837,21 @@
       <c r="R43" s="23">
         <v>640</v>
       </c>
-      <c r="S43" s="23">
+      <c r="S43" s="23"/>
+      <c r="T43" s="23">
         <v>1600</v>
       </c>
-      <c r="T43" s="23">
+      <c r="U43" s="23">
         <v>3200</v>
       </c>
-      <c r="V43" s="23">
+      <c r="W43" s="23">
         <v>5000</v>
       </c>
-      <c r="W43" s="23">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X43" s="23">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>65</v>
       </c>
@@ -2880,10 +2898,11 @@
       <c r="R44" s="29"/>
       <c r="S44" s="29"/>
       <c r="T44" s="29"/>
-      <c r="V44" s="29"/>
+      <c r="U44" s="29"/>
       <c r="W44" s="29"/>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X44" s="29"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>66</v>
       </c>
@@ -2927,10 +2946,11 @@
       <c r="R45" s="29"/>
       <c r="S45" s="29"/>
       <c r="T45" s="29"/>
-      <c r="V45" s="29"/>
+      <c r="U45" s="29"/>
       <c r="W45" s="29"/>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X45" s="29"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>67</v>
       </c>
@@ -2974,10 +2994,11 @@
       <c r="R46" s="29"/>
       <c r="S46" s="29"/>
       <c r="T46" s="29"/>
-      <c r="V46" s="29"/>
+      <c r="U46" s="29"/>
       <c r="W46" s="29"/>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X46" s="29"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>68</v>
       </c>
@@ -3000,10 +3021,11 @@
       <c r="R47" s="29"/>
       <c r="S47" s="29"/>
       <c r="T47" s="29"/>
-      <c r="V47" s="29"/>
+      <c r="U47" s="29"/>
       <c r="W47" s="29"/>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X47" s="29"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>7</v>
       </c>
@@ -3043,7 +3065,7 @@
         <v>900</v>
       </c>
       <c r="O48" s="23">
-        <v>1200</v>
+        <v>1250</v>
       </c>
       <c r="P48" s="23">
         <v>30000</v>
@@ -3052,20 +3074,24 @@
       <c r="R48" s="23">
         <v>3500</v>
       </c>
-      <c r="S48" s="23">
+      <c r="S48" s="23"/>
+      <c r="T48" s="23">
         <v>3000</v>
       </c>
-      <c r="T48" s="23">
-        <v>2200</v>
+      <c r="U48" s="23">
+        <v>1800</v>
       </c>
       <c r="V48" s="23">
+        <v>860</v>
+      </c>
+      <c r="W48" s="23">
         <v>1600</v>
       </c>
-      <c r="W48" s="23">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X48" s="23">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>9</v>
       </c>
@@ -3104,27 +3130,31 @@
       </c>
       <c r="Q49" s="29"/>
       <c r="R49" s="23">
-        <v>3.75</v>
-      </c>
-      <c r="S49" s="29">
+        <v>3.2</v>
+      </c>
+      <c r="S49" s="23"/>
+      <c r="T49" s="29">
         <v>2.7</v>
       </c>
-      <c r="T49" s="23">
+      <c r="U49" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="V49" s="29">
+        <v>3.5</v>
+      </c>
+      <c r="W49" s="23">
+        <v>2.5</v>
+      </c>
+      <c r="X49" s="29">
         <v>3</v>
       </c>
-      <c r="V49" s="23">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="W49" s="29">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C50" s="16"/>
       <c r="D50" s="16">
@@ -3141,33 +3171,44 @@
         <v>300</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J50" s="17" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
+      <c r="L50" s="18">
+        <v>8</v>
+      </c>
       <c r="M50" s="18">
         <v>200</v>
       </c>
       <c r="N50" s="19"/>
-      <c r="O50" s="29"/>
+      <c r="O50" s="29">
+        <v>50</v>
+      </c>
       <c r="P50" s="29"/>
       <c r="Q50" s="29"/>
-      <c r="R50" s="29"/>
-      <c r="S50" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="T50" s="29">
+      <c r="R50" s="29">
+        <v>100</v>
+      </c>
+      <c r="S50" s="29">
+        <v>300</v>
+      </c>
+      <c r="T50" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="U50" s="29">
         <v>200</v>
       </c>
-      <c r="V50" s="29"/>
       <c r="W50" s="29"/>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X50" s="29">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B51" s="16"/>
       <c r="C51" s="16"/>
@@ -3190,24 +3231,33 @@
         <v>1.75</v>
       </c>
       <c r="N51" s="19"/>
-      <c r="O51" s="29"/>
+      <c r="O51" s="29">
+        <v>0</v>
+      </c>
       <c r="P51" s="29"/>
       <c r="Q51" s="29"/>
-      <c r="R51" s="29"/>
+      <c r="R51" s="29">
+        <v>0</v>
+      </c>
       <c r="S51" s="29">
+        <v>0</v>
+      </c>
+      <c r="T51" s="29">
         <v>1.3</v>
       </c>
-      <c r="T51" s="29">
+      <c r="U51" s="29">
+        <v>1.5</v>
+      </c>
+      <c r="W51" s="29">
+        <v>5</v>
+      </c>
+      <c r="X51" s="29">
         <v>0</v>
       </c>
-      <c r="V51" s="29">
-        <v>5</v>
-      </c>
-      <c r="W51" s="29"/>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B52" s="16"/>
       <c r="C52" s="16"/>
@@ -3225,27 +3275,38 @@
       <c r="I52" s="16"/>
       <c r="J52" s="16"/>
       <c r="K52" s="18"/>
-      <c r="L52" s="18"/>
+      <c r="L52" s="18">
+        <v>1</v>
+      </c>
       <c r="M52" s="18">
         <v>2</v>
       </c>
       <c r="N52" s="18"/>
-      <c r="O52" s="29"/>
+      <c r="O52" s="29">
+        <v>3</v>
+      </c>
       <c r="P52" s="29"/>
       <c r="Q52" s="29"/>
-      <c r="R52" s="29"/>
+      <c r="R52" s="29">
+        <v>4</v>
+      </c>
       <c r="S52" s="29">
         <v>1</v>
       </c>
       <c r="T52" s="29">
         <v>1</v>
       </c>
-      <c r="V52" s="29"/>
+      <c r="U52" s="29">
+        <v>1</v>
+      </c>
       <c r="W52" s="29"/>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X52" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B53" s="16"/>
       <c r="C53" s="16"/>
@@ -3263,27 +3324,38 @@
       <c r="I53" s="17"/>
       <c r="J53" s="17"/>
       <c r="K53" s="18"/>
-      <c r="L53" s="18"/>
+      <c r="L53" s="18">
+        <v>4</v>
+      </c>
       <c r="M53" s="18">
         <v>0.125</v>
       </c>
       <c r="N53" s="20"/>
-      <c r="O53" s="29"/>
+      <c r="O53" s="29">
+        <v>0.5</v>
+      </c>
       <c r="P53" s="29"/>
       <c r="Q53" s="29"/>
-      <c r="R53" s="29"/>
+      <c r="R53" s="29">
+        <v>0.25</v>
+      </c>
       <c r="S53" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="T53" s="29">
         <v>0.76900000000000002</v>
       </c>
-      <c r="T53" s="29">
-        <v>1.25</v>
-      </c>
-      <c r="V53" s="29"/>
+      <c r="U53" s="29">
+        <v>1</v>
+      </c>
       <c r="W53" s="29"/>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X53" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B54" s="16"/>
       <c r="C54" s="16"/>
@@ -3300,7 +3372,7 @@
       <c r="J54" s="16"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M54" s="18">
         <v>50</v>
@@ -3313,21 +3385,26 @@
         <v>1380</v>
       </c>
       <c r="Q54" s="29"/>
-      <c r="R54" s="29"/>
-      <c r="S54" s="29"/>
-      <c r="T54" s="29">
-        <v>250</v>
-      </c>
-      <c r="V54" s="29">
+      <c r="R54" s="29">
+        <v>100</v>
+      </c>
+      <c r="S54" s="29">
+        <v>150</v>
+      </c>
+      <c r="T54" s="29"/>
+      <c r="U54" s="29">
+        <v>200</v>
+      </c>
+      <c r="W54" s="29">
         <v>600</v>
       </c>
-      <c r="W54" s="29">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X54" s="29">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
@@ -3343,19 +3420,22 @@
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
       <c r="M55" s="18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="N55" s="18"/>
       <c r="O55" s="29"/>
       <c r="P55" s="29"/>
       <c r="Q55" s="29"/>
-      <c r="R55" s="29"/>
+      <c r="R55" s="29">
+        <v>0.1</v>
+      </c>
       <c r="S55" s="29"/>
       <c r="T55" s="29"/>
-      <c r="V55" s="29"/>
+      <c r="U55" s="29"/>
       <c r="W55" s="29"/>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X55" s="29"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>69</v>
       </c>
@@ -3380,10 +3460,11 @@
       <c r="R56" s="29"/>
       <c r="S56" s="29"/>
       <c r="T56" s="29"/>
-      <c r="V56" s="29"/>
+      <c r="U56" s="29"/>
       <c r="W56" s="29"/>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X56" s="29"/>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>70</v>
       </c>
@@ -3417,24 +3498,29 @@
         <v>35</v>
       </c>
       <c r="Q57" s="29"/>
-      <c r="R57" s="29"/>
+      <c r="R57" s="29">
+        <v>23</v>
+      </c>
       <c r="S57" s="29">
+        <v>26</v>
+      </c>
+      <c r="T57" s="29">
         <v>35</v>
       </c>
-      <c r="T57" s="29">
+      <c r="U57" s="29">
         <v>46</v>
       </c>
-      <c r="V57" s="29"/>
-      <c r="W57" s="29">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W57" s="29"/>
+      <c r="X57" s="29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>83</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>81</v>
@@ -3464,10 +3550,11 @@
       <c r="R58" s="29"/>
       <c r="S58" s="29"/>
       <c r="T58" s="29"/>
-      <c r="V58" s="29"/>
+      <c r="U58" s="29"/>
       <c r="W58" s="29"/>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X58" s="29"/>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>71</v>
       </c>
@@ -3490,27 +3577,31 @@
       <c r="J59" s="15"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
-      <c r="M59" s="15"/>
+      <c r="M59" s="15" t="s">
+        <v>86</v>
+      </c>
       <c r="N59" s="15"/>
-      <c r="O59" t="s">
+      <c r="P59" t="s">
         <v>103</v>
       </c>
-      <c r="P59" t="s">
-        <v>104</v>
-      </c>
-      <c r="R59" t="s">
-        <v>109</v>
-      </c>
-      <c r="V59" t="s">
+      <c r="T59" t="s">
+        <v>274</v>
+      </c>
+      <c r="U59" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W59" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>72</v>
       </c>
       <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
+      <c r="C60" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="D60" s="15"/>
       <c r="E60" s="14"/>
       <c r="F60" s="15"/>
@@ -3522,7 +3613,7 @@
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>73</v>
       </c>
@@ -3539,211 +3630,222 @@
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
     </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="O62" t="s">
+        <v>273</v>
+      </c>
+    </row>
     <row r="67" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
+        <v>117</v>
+      </c>
+      <c r="C67" t="s">
+        <v>124</v>
+      </c>
+      <c r="D67" t="s">
+        <v>127</v>
+      </c>
+      <c r="E67" t="s">
+        <v>130</v>
+      </c>
+      <c r="F67" t="s">
+        <v>132</v>
+      </c>
+      <c r="G67" t="s">
+        <v>134</v>
+      </c>
+      <c r="H67" t="s">
+        <v>136</v>
+      </c>
+      <c r="I67" t="s">
+        <v>271</v>
+      </c>
+      <c r="J67" t="s">
+        <v>138</v>
+      </c>
+      <c r="K67" t="s">
+        <v>142</v>
+      </c>
+      <c r="L67" t="s">
+        <v>146</v>
+      </c>
+      <c r="M67" t="s">
+        <v>144</v>
+      </c>
+      <c r="N67" t="s">
+        <v>148</v>
+      </c>
+      <c r="O67" t="s">
+        <v>150</v>
+      </c>
+      <c r="P67" t="s">
+        <v>152</v>
+      </c>
+      <c r="R67" t="s">
+        <v>154</v>
+      </c>
+      <c r="S67" t="s">
+        <v>159</v>
+      </c>
+      <c r="T67" t="s">
+        <v>162</v>
+      </c>
+      <c r="U67" t="s">
+        <v>164</v>
+      </c>
+      <c r="V67" t="s">
+        <v>166</v>
+      </c>
+      <c r="W67" t="s">
+        <v>168</v>
+      </c>
+      <c r="X67" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA67" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC67" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD67" t="s">
+        <v>181</v>
+      </c>
+      <c r="AE67" t="s">
+        <v>183</v>
+      </c>
+      <c r="AF67" t="s">
+        <v>185</v>
+      </c>
+      <c r="AG67" t="s">
+        <v>188</v>
+      </c>
+      <c r="AH67" t="s">
+        <v>190</v>
+      </c>
+      <c r="AI67" t="s">
+        <v>193</v>
+      </c>
+      <c r="AJ67" t="s">
+        <v>195</v>
+      </c>
+      <c r="AL67" t="s">
         <v>119</v>
-      </c>
-      <c r="C67" t="s">
-        <v>126</v>
-      </c>
-      <c r="D67" t="s">
-        <v>129</v>
-      </c>
-      <c r="E67" t="s">
-        <v>132</v>
-      </c>
-      <c r="F67" t="s">
-        <v>134</v>
-      </c>
-      <c r="G67" t="s">
-        <v>136</v>
-      </c>
-      <c r="H67" t="s">
-        <v>138</v>
-      </c>
-      <c r="J67" t="s">
-        <v>140</v>
-      </c>
-      <c r="K67" t="s">
-        <v>144</v>
-      </c>
-      <c r="L67" t="s">
-        <v>148</v>
-      </c>
-      <c r="M67" t="s">
-        <v>146</v>
-      </c>
-      <c r="N67" t="s">
-        <v>150</v>
-      </c>
-      <c r="O67" t="s">
-        <v>152</v>
-      </c>
-      <c r="P67" t="s">
-        <v>154</v>
-      </c>
-      <c r="R67" t="s">
-        <v>156</v>
-      </c>
-      <c r="S67" t="s">
-        <v>161</v>
-      </c>
-      <c r="T67" t="s">
-        <v>164</v>
-      </c>
-      <c r="U67" t="s">
-        <v>166</v>
-      </c>
-      <c r="V67" t="s">
-        <v>168</v>
-      </c>
-      <c r="W67" t="s">
-        <v>170</v>
-      </c>
-      <c r="X67" t="s">
-        <v>172</v>
-      </c>
-      <c r="Z67" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA67" t="s">
-        <v>177</v>
-      </c>
-      <c r="AB67" t="s">
-        <v>179</v>
-      </c>
-      <c r="AC67" t="s">
-        <v>181</v>
-      </c>
-      <c r="AD67" t="s">
-        <v>183</v>
-      </c>
-      <c r="AE67" t="s">
-        <v>185</v>
-      </c>
-      <c r="AF67" t="s">
-        <v>187</v>
-      </c>
-      <c r="AG67" t="s">
-        <v>190</v>
-      </c>
-      <c r="AH67" t="s">
-        <v>192</v>
-      </c>
-      <c r="AI67" t="s">
-        <v>195</v>
-      </c>
-      <c r="AJ67" t="s">
-        <v>197</v>
-      </c>
-      <c r="AL67" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
+        <v>126</v>
+      </c>
+      <c r="C68" t="s">
+        <v>125</v>
+      </c>
+      <c r="D68" t="s">
         <v>128</v>
       </c>
-      <c r="C68" t="s">
-        <v>127</v>
-      </c>
-      <c r="D68" t="s">
-        <v>130</v>
-      </c>
       <c r="E68" t="s">
+        <v>131</v>
+      </c>
+      <c r="F68" t="s">
         <v>133</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>135</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>137</v>
       </c>
-      <c r="H68" t="s">
+      <c r="I68" t="s">
+        <v>272</v>
+      </c>
+      <c r="J68" t="s">
         <v>139</v>
       </c>
-      <c r="J68" t="s">
-        <v>141</v>
-      </c>
       <c r="K68" t="s">
+        <v>143</v>
+      </c>
+      <c r="L68" t="s">
         <v>145</v>
       </c>
-      <c r="L68" t="s">
+      <c r="M68" t="s">
         <v>147</v>
       </c>
-      <c r="M68" t="s">
+      <c r="N68" t="s">
         <v>149</v>
       </c>
-      <c r="N68" t="s">
+      <c r="O68" t="s">
         <v>151</v>
       </c>
-      <c r="O68" t="s">
+      <c r="P68" t="s">
         <v>153</v>
       </c>
-      <c r="P68" t="s">
+      <c r="R68" t="s">
         <v>155</v>
       </c>
-      <c r="R68" t="s">
-        <v>157</v>
-      </c>
       <c r="S68" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="T68" t="s">
+        <v>163</v>
+      </c>
+      <c r="U68" t="s">
         <v>165</v>
       </c>
-      <c r="U68" t="s">
-        <v>167</v>
-      </c>
       <c r="V68" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="W68" t="s">
+        <v>169</v>
+      </c>
+      <c r="X68" t="s">
         <v>171</v>
       </c>
-      <c r="X68" t="s">
+      <c r="Z68" t="s">
         <v>173</v>
       </c>
-      <c r="Z68" t="s">
-        <v>175</v>
-      </c>
       <c r="AA68" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB68" t="s">
         <v>178</v>
       </c>
-      <c r="AB68" t="s">
+      <c r="AC68" t="s">
         <v>180</v>
       </c>
-      <c r="AC68" t="s">
+      <c r="AD68" t="s">
         <v>182</v>
       </c>
-      <c r="AD68" t="s">
+      <c r="AE68" t="s">
         <v>184</v>
       </c>
-      <c r="AE68" t="s">
+      <c r="AF68" t="s">
         <v>186</v>
       </c>
-      <c r="AF68" t="s">
-        <v>188</v>
-      </c>
       <c r="AG68" t="s">
+        <v>189</v>
+      </c>
+      <c r="AH68" t="s">
         <v>191</v>
       </c>
-      <c r="AH68" t="s">
-        <v>193</v>
-      </c>
       <c r="AI68" t="s">
+        <v>194</v>
+      </c>
+      <c r="AJ68" t="s">
         <v>196</v>
       </c>
-      <c r="AJ68" t="s">
-        <v>198</v>
-      </c>
       <c r="AL68" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B70">
         <v>8000</v>
@@ -3818,19 +3920,19 @@
         <v>7000</v>
       </c>
       <c r="AF70" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AG70" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AH70" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AI70">
         <v>3800</v>
       </c>
       <c r="AJ70" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AL70">
         <v>500</v>
@@ -3838,7 +3940,7 @@
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B71">
         <v>13300</v>
@@ -3921,7 +4023,7 @@
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B72">
         <v>1520</v>
@@ -4004,7 +4106,7 @@
     </row>
     <row r="73" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B73">
         <v>2600</v>
@@ -4087,7 +4189,7 @@
     </row>
     <row r="74" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B74">
         <v>40</v>
@@ -4131,7 +4233,7 @@
     </row>
     <row r="75" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J75">
         <v>150</v>
@@ -4163,7 +4265,7 @@
     </row>
     <row r="76" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J76">
         <v>1</v>
@@ -4171,7 +4273,7 @@
     </row>
     <row r="77" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="R77">
         <v>35</v>
@@ -4212,7 +4314,7 @@
     </row>
     <row r="78" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="R78">
         <v>44</v>
@@ -4253,7 +4355,7 @@
     </row>
     <row r="79" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S79">
         <v>1.5</v>
@@ -4288,7 +4390,7 @@
     </row>
     <row r="80" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="R80">
         <v>2</v>
@@ -4317,7 +4419,7 @@
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="V81">
         <v>5</v>
@@ -4328,135 +4430,135 @@
     </row>
     <row r="82" spans="1:30" x14ac:dyDescent="0.25">
       <c r="Z82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AA82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AB82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AC82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B87" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C87" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D87" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E87" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F87" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G87" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H87" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I87" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J87" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K87" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L87" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B88" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C88" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D88" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E88" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F88" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G88" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H88" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I88" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J88" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K88" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L88" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B89" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C89" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D89" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E89" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F89" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G89" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H89" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I89" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J89" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K89" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L89" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B90">
         <v>500</v>
@@ -4485,7 +4587,7 @@
     </row>
     <row r="92" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B92">
         <v>2880</v>
@@ -4514,7 +4616,7 @@
     </row>
     <row r="93" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B93">
         <v>360</v>
@@ -4543,7 +4645,7 @@
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B94">
         <v>1440</v>
@@ -4572,7 +4674,7 @@
     </row>
     <row r="96" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B96">
         <v>6</v>
@@ -4601,45 +4703,45 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E97" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F97" t="s">
+        <v>222</v>
+      </c>
+      <c r="G97" t="s">
+        <v>228</v>
+      </c>
+      <c r="H97" t="s">
+        <v>229</v>
+      </c>
+      <c r="I97" t="s">
+        <v>233</v>
+      </c>
+      <c r="J97" t="s">
+        <v>234</v>
+      </c>
+      <c r="K97" t="s">
+        <v>222</v>
+      </c>
+      <c r="L97" t="s">
         <v>224</v>
       </c>
-      <c r="G97" t="s">
-        <v>230</v>
-      </c>
-      <c r="H97" t="s">
-        <v>231</v>
-      </c>
-      <c r="I97" t="s">
-        <v>235</v>
-      </c>
-      <c r="J97" t="s">
-        <v>236</v>
-      </c>
-      <c r="K97" t="s">
-        <v>224</v>
-      </c>
-      <c r="L97" t="s">
-        <v>226</v>
-      </c>
       <c r="M97" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="N97" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="O97" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B98">
         <v>25</v>
@@ -4686,7 +4788,7 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -4730,7 +4832,7 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B100">
         <v>2</v>
@@ -4777,7 +4879,7 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B101">
         <v>32</v>
@@ -4824,7 +4926,7 @@
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B102">
         <v>0.83299999999999996</v>
@@ -4871,7 +4973,7 @@
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B103">
         <v>41.6</v>
@@ -4880,7 +4982,7 @@
         <v>60</v>
       </c>
       <c r="D103" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E103">
         <v>50</v>
@@ -4918,16 +5020,16 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D105" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J105" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L105" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>